<commit_message>
Updating tests summary for Heuristic 2.
</commit_message>
<xml_diff>
--- a/docs/testsFSG/tests-summary.xlsx
+++ b/docs/testsFSG/tests-summary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="71">
   <si>
     <t>Run</t>
   </si>
@@ -198,9 +198,6 @@
     <t>1000 Solutions - Run 3</t>
   </si>
   <si>
-    <t>Features: 40, Heuristic: 2</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
@@ -213,19 +210,10 @@
     <t>Heuristic 2</t>
   </si>
   <si>
-    <t>Features: 40, Heuristic: 3</t>
-  </si>
-  <si>
     <t>Heuristic 3</t>
   </si>
   <si>
-    <t>Features: 40, Heuristic: 4</t>
-  </si>
-  <si>
     <t>Heuristic 4</t>
-  </si>
-  <si>
-    <t>Features: 40, Heuristic 1: MorePercInstVars</t>
   </si>
   <si>
     <t>#CTC per FM:</t>
@@ -241,6 +229,15 @@
   </si>
   <si>
     <t>#Features</t>
+  </si>
+  <si>
+    <t>Features: 40, Heuristic 2: Default + BiVarArithmetic</t>
+  </si>
+  <si>
+    <t>Features: 40, Heuristic 1: Default + MorePercInstVars</t>
+  </si>
+  <si>
+    <t>Features: 40, Heuristic 3: Default + BiVarArithmetic + OrAttr0 + OrAttr1</t>
   </si>
 </sst>
 </file>
@@ -484,19 +481,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.1713196075358119E-2</c:v>
+                  <c:v>9.1187269729718287E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1120159944739523</c:v>
+                  <c:v>0.11180847459261625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17160190134522463</c:v>
+                  <c:v>0.17014395193802512</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19181052458152417</c:v>
+                  <c:v>0.19116987590893744</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23150703440631004</c:v>
+                  <c:v>0.23112729160001227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -560,19 +557,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6.6510128502450097E-2</c:v>
+                  <c:v>6.5905807503954361E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6431743786938922E-2</c:v>
+                  <c:v>8.5653949321746303E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1072712197284221</c:v>
+                  <c:v>0.10691845154486945</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1433654095945468</c:v>
+                  <c:v>0.14034154529106099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.22956564977215757</c:v>
+                  <c:v>0.22708745996596125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -635,6 +632,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.837459345418106E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.973155770843153E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11130381037109011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12629952919295748</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14112515449175733</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1091,19 +1103,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.50496600095331901</c:v>
+                  <c:v>0.30144674955333528</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1547335308334854</c:v>
+                  <c:v>0.70487610846063131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4229073944904496</c:v>
+                  <c:v>7.1782102891205311</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.317513882842967</c:v>
+                  <c:v>30.133753885968989</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.200932943568031</c:v>
+                  <c:v>9.3311456376174444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1167,19 +1179,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.54504912456136556</c:v>
+                  <c:v>0.26271717043663456</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7720456555716841</c:v>
+                  <c:v>0.9855389183779858</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.28765774181411</c:v>
+                  <c:v>7.3579809941861845</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65.643641109764957</c:v>
+                  <c:v>31.92406529142966</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.706443362773502</c:v>
+                  <c:v>13.845771604971324</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1242,6 +1254,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.3103117867143107</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7290030969009762</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7141563995510145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.188664846837895</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.470053843172394</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2949,50 +2976,6 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14378" displayName="Table14378" ref="A95:AI110" totalsRowShown="0" dataCellStyle="Normal">
-  <autoFilter ref="A95:AI110"/>
-  <tableColumns count="35">
-    <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
-    <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
-    <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
-    <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
-    <tableColumn id="34" name="Nodes5" dataCellStyle="Normal"/>
-    <tableColumn id="33" name="Backtracks6" dataCellStyle="Normal"/>
-    <tableColumn id="32" name="Fails7" dataCellStyle="Normal"/>
-    <tableColumn id="29" name="Restarts8" dataCellStyle="Normal"/>
-    <tableColumn id="20" name="Building Time3" dataCellStyle="Normal"/>
-    <tableColumn id="21" name="Resolution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="22" name="Execution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="23" name="Building Time32" dataCellStyle="Normal"/>
-    <tableColumn id="24" name="Resolution Time23" dataCellStyle="Normal"/>
-    <tableColumn id="25" name="Execution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="26" name="Building Time33" dataCellStyle="Normal"/>
-    <tableColumn id="27" name="Resolution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="28" name="Execution Time25" dataCellStyle="Normal"/>
-    <tableColumn id="37" name="Variables3" dataCellStyle="Normal"/>
-    <tableColumn id="38" name="Constraints4" dataCellStyle="Normal"/>
-    <tableColumn id="39" name="Solutions5" dataCellStyle="Normal"/>
-    <tableColumn id="40" name="Nodes6" dataCellStyle="Normal"/>
-    <tableColumn id="41" name="Backtracks7" dataCellStyle="Normal"/>
-    <tableColumn id="42" name="Fails8" dataCellStyle="Normal"/>
-    <tableColumn id="43" name="Restarts9" dataCellStyle="Normal"/>
-    <tableColumn id="44" name="Building Time10" dataCellStyle="Normal"/>
-    <tableColumn id="45" name="Resolution Time11" dataCellStyle="Normal"/>
-    <tableColumn id="46" name="Execution Time12" dataCellStyle="Normal"/>
-    <tableColumn id="47" name="Building Time213" dataCellStyle="Normal"/>
-    <tableColumn id="48" name="Resolution Time314" dataCellStyle="Normal"/>
-    <tableColumn id="49" name="Execution Time415" dataCellStyle="Normal"/>
-    <tableColumn id="50" name="Building Time516" dataCellStyle="Normal"/>
-    <tableColumn id="51" name="Resolution Time617" dataCellStyle="Normal"/>
-    <tableColumn id="52" name="Execution Time718" dataCellStyle="Normal"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3258,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3270,22 +3253,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" t="s">
-        <v>63</v>
-      </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -3293,12 +3276,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8">
-        <f>GEOMEAN(Models!L12:L14,Models!O12:O14,Models!R12:R14)</f>
-        <v>9.1713196075358119E-2</v>
+        <f>HARMEAN(Models!L12:L14,Models!O12:O14,Models!R12:R14)</f>
+        <v>9.1187269729718287E-2</v>
       </c>
       <c r="C2" s="8">
-        <f>GEOMEAN(Models!L33:L35,Models!O33:O35,Models!R33:R35)</f>
-        <v>6.6510128502450097E-2</v>
+        <f>HARMEAN(Models!L33:L35,Models!O33:O35,Models!R33:R35)</f>
+        <v>6.5905807503954361E-2</v>
+      </c>
+      <c r="D2">
+        <f>HARMEAN(Models!L54:L56,Models!O54:O56,Models!R54:R56)</f>
+        <v>7.837459345418106E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -3306,12 +3293,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8">
-        <f>GEOMEAN(Models!L15:L17,Models!O15:O17,Models!R15:R17)</f>
-        <v>0.1120159944739523</v>
+        <f>HARMEAN(Models!L15:L17,Models!O15:O17,Models!R15:R17)</f>
+        <v>0.11180847459261625</v>
       </c>
       <c r="C3" s="8">
-        <f>GEOMEAN(Models!L36:L38,Models!O36:O38,Models!R36:R38)</f>
-        <v>8.6431743786938922E-2</v>
+        <f>HARMEAN(Models!L36:L38,Models!O36:O38,Models!R36:R38)</f>
+        <v>8.5653949321746303E-2</v>
+      </c>
+      <c r="D3">
+        <f>HARMEAN(Models!L57:L59,Models!O57:O59,Models!R57:R59)</f>
+        <v>7.973155770843153E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3319,12 +3310,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8">
-        <f>GEOMEAN(Models!L18:L20,Models!O18:O20,Models!R18:R20)</f>
-        <v>0.17160190134522463</v>
+        <f>HARMEAN(Models!L18:L20,Models!O18:O20,Models!R18:R20)</f>
+        <v>0.17014395193802512</v>
       </c>
       <c r="C4" s="8">
-        <f>GEOMEAN(Models!L39:L41,Models!O39:O41,Models!R39:R41)</f>
-        <v>0.1072712197284221</v>
+        <f>HARMEAN(Models!L39:L41,Models!O39:O41,Models!R39:R41)</f>
+        <v>0.10691845154486945</v>
+      </c>
+      <c r="D4">
+        <f>HARMEAN(Models!L60:L62,Models!O60:O62,Models!R60:R62)</f>
+        <v>0.11130381037109011</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3332,12 +3327,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8">
-        <f>GEOMEAN(Models!L21:L23,Models!O21:O23,Models!R21:R23)</f>
-        <v>0.19181052458152417</v>
+        <f>HARMEAN(Models!L21:L23,Models!O21:O23,Models!R21:R23)</f>
+        <v>0.19116987590893744</v>
       </c>
       <c r="C5" s="8">
-        <f>GEOMEAN(Models!L42:L44,Models!O42:O44,Models!R42:R44)</f>
-        <v>0.1433654095945468</v>
+        <f>HARMEAN(Models!L42:L44,Models!O42:O44,Models!R42:R44)</f>
+        <v>0.14034154529106099</v>
+      </c>
+      <c r="D5">
+        <f>HARMEAN(Models!L63:L65,Models!O63:O65,Models!R63:R65)</f>
+        <v>0.12629952919295748</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3345,32 +3344,36 @@
         <v>5</v>
       </c>
       <c r="B6" s="8">
-        <f>GEOMEAN(Models!L24:L26,Models!O24:O26,Models!R24:R26)</f>
-        <v>0.23150703440631004</v>
+        <f>HARMEAN(Models!L24:L26,Models!O24:O26,Models!R24:R26)</f>
+        <v>0.23112729160001227</v>
       </c>
       <c r="C6" s="8">
-        <f>GEOMEAN(Models!L45:L47,Models!O45:O47,Models!R45:R47)</f>
-        <v>0.22956564977215757</v>
+        <f>HARMEAN(Models!L45:L47,Models!O45:O47,Models!R45:R47)</f>
+        <v>0.22708745996596125</v>
+      </c>
+      <c r="D6">
+        <f>HARMEAN(Models!L66:L68,Models!O66:O68,Models!R66:R68)</f>
+        <v>0.14112515449175733</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
         <v>59</v>
       </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>61</v>
       </c>
-      <c r="E10" t="s">
-        <v>63</v>
-      </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3378,12 +3381,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="8">
-        <f>GEOMEAN(Models!AB12:AB14,Models!AE12:AE14,Models!AH12:AH14)</f>
-        <v>0.50496600095331901</v>
+        <f>HARMEAN(Models!AB12:AB14,Models!AE12:AE14,Models!AH12:AH14)</f>
+        <v>0.30144674955333528</v>
       </c>
       <c r="C11" s="8">
-        <f>GEOMEAN(Models!AB33:AB35,Models!AE33:AE35,Models!AH33:AH35)</f>
-        <v>0.54504912456136556</v>
+        <f>HARMEAN(Models!AB33:AB35,Models!AE33:AE35,Models!AH33:AH35)</f>
+        <v>0.26271717043663456</v>
+      </c>
+      <c r="D11">
+        <f>HARMEAN(Models!AB54:AB56,Models!AE54:AE56,Models!AH54:AH56)</f>
+        <v>0.3103117867143107</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3391,12 +3398,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="8">
-        <f>GEOMEAN(Models!AB15:AB17,Models!AE15:AE17,Models!AH15:AH17)</f>
-        <v>1.1547335308334854</v>
+        <f>HARMEAN(Models!AB15:AB17,Models!AE15:AE17,Models!AH15:AH17)</f>
+        <v>0.70487610846063131</v>
       </c>
       <c r="C12" s="8">
-        <f>GEOMEAN(Models!AB36:AB38,Models!AE36:AE38,Models!AH36:AH38)</f>
-        <v>1.7720456555716841</v>
+        <f>HARMEAN(Models!AB36:AB38,Models!AE36:AE38,Models!AH36:AH38)</f>
+        <v>0.9855389183779858</v>
+      </c>
+      <c r="D12">
+        <f>HARMEAN(Models!AB57:AB59,Models!AE57:AE59,Models!AH57:AH59)</f>
+        <v>0.7290030969009762</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -3404,12 +3415,16 @@
         <v>3</v>
       </c>
       <c r="B13" s="8">
-        <f>GEOMEAN(Models!AB18:AB20,Models!AE18:AE20,Models!AH18:AH20)</f>
-        <v>8.4229073944904496</v>
+        <f>HARMEAN(Models!AB18:AB20,Models!AE18:AE20,Models!AH18:AH20)</f>
+        <v>7.1782102891205311</v>
       </c>
       <c r="C13" s="8">
-        <f>GEOMEAN(Models!AB39:AB41,Models!AE39:AE41,Models!AH39:AH41)</f>
-        <v>10.28765774181411</v>
+        <f>HARMEAN(Models!AB39:AB41,Models!AE39:AE41,Models!AH39:AH41)</f>
+        <v>7.3579809941861845</v>
+      </c>
+      <c r="D13">
+        <f>HARMEAN(Models!AB60:AB62,Models!AE60:AE62,Models!AH60:AH62)</f>
+        <v>5.7141563995510145</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3417,12 +3432,16 @@
         <v>4</v>
       </c>
       <c r="B14" s="8">
-        <f>GEOMEAN(Models!AB21:AB23,Models!AE21:AE23,Models!AH21:AH23)</f>
-        <v>32.317513882842967</v>
+        <f>HARMEAN(Models!AB21:AB23,Models!AE21:AE23,Models!AH21:AH23)</f>
+        <v>30.133753885968989</v>
       </c>
       <c r="C14" s="8">
-        <f>GEOMEAN(Models!AB42:AB44,Models!AE42:AE44,Models!AH42:AH44)</f>
-        <v>65.643641109764957</v>
+        <f>HARMEAN(Models!AB42:AB44,Models!AE42:AE44,Models!AH42:AH44)</f>
+        <v>31.92406529142966</v>
+      </c>
+      <c r="D14">
+        <f>HARMEAN(Models!AB63:AB65,Models!AE63:AE65,Models!AH63:AH65)</f>
+        <v>36.188664846837895</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -3430,12 +3449,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="8">
-        <f>GEOMEAN(Models!AB24:AB26,Models!AE24:AE26,Models!AH24:AH26)</f>
-        <v>10.200932943568031</v>
+        <f>HARMEAN(Models!AB24:AB26,Models!AE24:AE26,Models!AH24:AH26)</f>
+        <v>9.3311456376174444</v>
       </c>
       <c r="C15" s="8">
-        <f>GEOMEAN(Models!AB45:AB47,Models!AE45:AE47,Models!AH45:AH47)</f>
-        <v>21.706443362773502</v>
+        <f>HARMEAN(Models!AB45:AB47,Models!AE45:AE47,Models!AH45:AH47)</f>
+        <v>13.845771604971324</v>
+      </c>
+      <c r="D15">
+        <f>HARMEAN(Models!AB66:AB68,Models!AE66:AE68,Models!AH66:AH68)</f>
+        <v>30.470053843172394</v>
       </c>
     </row>
   </sheetData>
@@ -3450,14 +3473,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI110"/>
+  <dimension ref="A1:AI89"/>
   <sheetViews>
-    <sheetView topLeftCell="AE28" workbookViewId="0">
-      <selection activeCell="AI48" sqref="AI48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.109375" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
@@ -3501,7 +3525,7 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -3509,7 +3533,7 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="5">
         <v>0.1</v>
@@ -3517,7 +3541,7 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3525,7 +3549,7 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -3533,7 +3557,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B6" s="5">
         <v>0.05</v>
@@ -5311,7 +5335,7 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
@@ -7081,7 +7105,7 @@
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.3">
@@ -7254,6 +7278,102 @@
       <c r="C54">
         <v>19</v>
       </c>
+      <c r="D54">
+        <v>665</v>
+      </c>
+      <c r="E54">
+        <v>723</v>
+      </c>
+      <c r="F54">
+        <v>10</v>
+      </c>
+      <c r="G54">
+        <v>32</v>
+      </c>
+      <c r="H54">
+        <v>21</v>
+      </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0.214</v>
+      </c>
+      <c r="L54">
+        <v>0.109</v>
+      </c>
+      <c r="M54">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="N54">
+        <v>0.17</v>
+      </c>
+      <c r="O54">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="P54">
+        <v>0.15</v>
+      </c>
+      <c r="Q54">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="R54">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="S54">
+        <v>0.127</v>
+      </c>
+      <c r="T54">
+        <v>2641</v>
+      </c>
+      <c r="U54">
+        <v>2699</v>
+      </c>
+      <c r="V54">
+        <v>504</v>
+      </c>
+      <c r="W54">
+        <v>2534</v>
+      </c>
+      <c r="X54">
+        <v>4061</v>
+      </c>
+      <c r="Y54">
+        <v>1527</v>
+      </c>
+      <c r="Z54">
+        <v>0</v>
+      </c>
+      <c r="AA54">
+        <v>0.18</v>
+      </c>
+      <c r="AB54">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AC54">
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="AD54">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AE54">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AF54">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="AG54">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AH54">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="AI54">
+        <v>1.0409999999999999</v>
+      </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -7265,6 +7385,102 @@
       <c r="C55">
         <v>24</v>
       </c>
+      <c r="D55">
+        <v>742</v>
+      </c>
+      <c r="E55">
+        <v>311</v>
+      </c>
+      <c r="F55">
+        <v>10</v>
+      </c>
+      <c r="G55">
+        <v>33</v>
+      </c>
+      <c r="H55">
+        <v>20</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0.216</v>
+      </c>
+      <c r="L55">
+        <v>0.113</v>
+      </c>
+      <c r="M55">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="N55">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="O55">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="P55">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="Q55">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="R55">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="S55">
+        <v>0.112</v>
+      </c>
+      <c r="T55">
+        <v>2310</v>
+      </c>
+      <c r="U55">
+        <v>2379</v>
+      </c>
+      <c r="V55">
+        <v>402</v>
+      </c>
+      <c r="W55">
+        <v>6377</v>
+      </c>
+      <c r="X55">
+        <v>11951</v>
+      </c>
+      <c r="Y55">
+        <v>5574</v>
+      </c>
+      <c r="Z55">
+        <v>0</v>
+      </c>
+      <c r="AA55">
+        <v>0.129</v>
+      </c>
+      <c r="AB55">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="AC55">
+        <v>1.351</v>
+      </c>
+      <c r="AD55">
+        <v>0.125</v>
+      </c>
+      <c r="AE55">
+        <v>1.353</v>
+      </c>
+      <c r="AF55">
+        <v>1.3939999999999999</v>
+      </c>
+      <c r="AG55">
+        <v>0.127</v>
+      </c>
+      <c r="AH55">
+        <v>1.4179999999999999</v>
+      </c>
+      <c r="AI55">
+        <v>1.458</v>
+      </c>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -7276,6 +7492,102 @@
       <c r="C56">
         <v>9</v>
       </c>
+      <c r="D56">
+        <v>734</v>
+      </c>
+      <c r="E56">
+        <v>801</v>
+      </c>
+      <c r="F56">
+        <v>10</v>
+      </c>
+      <c r="G56">
+        <v>24</v>
+      </c>
+      <c r="H56">
+        <v>14</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0.128</v>
+      </c>
+      <c r="L56">
+        <v>5.5E-2</v>
+      </c>
+      <c r="M56">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="N56">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="O56">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="P56">
+        <v>0.114</v>
+      </c>
+      <c r="Q56">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="R56">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="S56">
+        <v>0.107</v>
+      </c>
+      <c r="T56">
+        <v>934</v>
+      </c>
+      <c r="U56">
+        <v>1001</v>
+      </c>
+      <c r="V56">
+        <v>60</v>
+      </c>
+      <c r="W56">
+        <v>131</v>
+      </c>
+      <c r="X56">
+        <v>143</v>
+      </c>
+      <c r="Y56">
+        <v>12</v>
+      </c>
+      <c r="Z56">
+        <v>0</v>
+      </c>
+      <c r="AA56">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AB56">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="AC56">
+        <v>0.158</v>
+      </c>
+      <c r="AD56">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="AE56">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AF56">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="AG56">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AH56">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AI56">
+        <v>0.17699999999999999</v>
+      </c>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -7287,6 +7599,102 @@
       <c r="C57" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D57">
+        <v>1309</v>
+      </c>
+      <c r="E57">
+        <v>1434</v>
+      </c>
+      <c r="F57">
+        <v>10</v>
+      </c>
+      <c r="G57">
+        <v>30</v>
+      </c>
+      <c r="H57">
+        <v>16</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="L57">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="M57">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="N57">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="O57">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P57">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="Q57">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="R57">
+        <v>0.08</v>
+      </c>
+      <c r="S57">
+        <v>0.124</v>
+      </c>
+      <c r="T57">
+        <v>1977</v>
+      </c>
+      <c r="U57">
+        <v>2102</v>
+      </c>
+      <c r="V57">
+        <v>177</v>
+      </c>
+      <c r="W57">
+        <v>995</v>
+      </c>
+      <c r="X57">
+        <v>1637</v>
+      </c>
+      <c r="Y57">
+        <v>642</v>
+      </c>
+      <c r="Z57">
+        <v>0</v>
+      </c>
+      <c r="AA57">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AB57">
+        <v>0.437</v>
+      </c>
+      <c r="AC57">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="AD57">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="AE57">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="AF57">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="AG57">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AH57">
+        <v>0.43</v>
+      </c>
+      <c r="AI57">
+        <v>0.47399999999999998</v>
+      </c>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -7298,9 +7706,102 @@
       <c r="C58" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W58" s="2"/>
-      <c r="X58" s="2"/>
-      <c r="Y58" s="2"/>
+      <c r="D58">
+        <v>1239</v>
+      </c>
+      <c r="E58">
+        <v>1362</v>
+      </c>
+      <c r="F58">
+        <v>10</v>
+      </c>
+      <c r="G58">
+        <v>39</v>
+      </c>
+      <c r="H58">
+        <v>24</v>
+      </c>
+      <c r="I58">
+        <v>4</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="L58">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M58">
+        <v>0.127</v>
+      </c>
+      <c r="N58">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="O58">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="P58">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="Q58">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R58">
+        <v>0.08</v>
+      </c>
+      <c r="S58">
+        <v>0.124</v>
+      </c>
+      <c r="T58">
+        <v>3475</v>
+      </c>
+      <c r="U58">
+        <v>3598</v>
+      </c>
+      <c r="V58">
+        <v>569</v>
+      </c>
+      <c r="W58" s="2">
+        <v>10148</v>
+      </c>
+      <c r="X58" s="2">
+        <v>19159</v>
+      </c>
+      <c r="Y58" s="2">
+        <v>9011</v>
+      </c>
+      <c r="Z58">
+        <v>0</v>
+      </c>
+      <c r="AA58">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="AB58">
+        <v>2.6659999999999999</v>
+      </c>
+      <c r="AC58">
+        <v>2.722</v>
+      </c>
+      <c r="AD58">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AE58">
+        <v>2.5920000000000001</v>
+      </c>
+      <c r="AF58">
+        <v>2.6349999999999998</v>
+      </c>
+      <c r="AG58">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AH58">
+        <v>2.5680000000000001</v>
+      </c>
+      <c r="AI58">
+        <v>2.6110000000000002</v>
+      </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A59">
@@ -7312,6 +7813,102 @@
       <c r="C59" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D59">
+        <v>1326</v>
+      </c>
+      <c r="E59">
+        <v>1458</v>
+      </c>
+      <c r="F59">
+        <v>10</v>
+      </c>
+      <c r="G59">
+        <v>31</v>
+      </c>
+      <c r="H59">
+        <v>15</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0.192</v>
+      </c>
+      <c r="L59">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="M59">
+        <v>0.151</v>
+      </c>
+      <c r="N59">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="O59">
+        <v>0.08</v>
+      </c>
+      <c r="P59">
+        <v>0.122</v>
+      </c>
+      <c r="Q59">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="R59">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="S59">
+        <v>0.128</v>
+      </c>
+      <c r="T59">
+        <v>2662</v>
+      </c>
+      <c r="U59">
+        <v>2794</v>
+      </c>
+      <c r="V59">
+        <v>344</v>
+      </c>
+      <c r="W59">
+        <v>1293</v>
+      </c>
+      <c r="X59">
+        <v>1899</v>
+      </c>
+      <c r="Y59">
+        <v>606</v>
+      </c>
+      <c r="Z59">
+        <v>0</v>
+      </c>
+      <c r="AA59">
+        <v>0.223</v>
+      </c>
+      <c r="AB59">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AC59">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="AD59">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AE59">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="AF59">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="AG59">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AH59">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="AI59">
+        <v>0.69899999999999995</v>
+      </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A60">
@@ -7323,6 +7920,102 @@
       <c r="C60" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D60">
+        <v>2049</v>
+      </c>
+      <c r="E60">
+        <v>2249</v>
+      </c>
+      <c r="F60">
+        <v>10</v>
+      </c>
+      <c r="G60">
+        <v>42</v>
+      </c>
+      <c r="H60">
+        <v>17</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="L60">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="M60">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="N60">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="O60">
+        <v>0.115</v>
+      </c>
+      <c r="P60">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="Q60">
+        <v>0.153</v>
+      </c>
+      <c r="R60">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="S60">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="T60">
+        <v>6009</v>
+      </c>
+      <c r="U60">
+        <v>6209</v>
+      </c>
+      <c r="V60">
+        <v>1000</v>
+      </c>
+      <c r="W60">
+        <v>19928</v>
+      </c>
+      <c r="X60">
+        <v>37818</v>
+      </c>
+      <c r="Y60">
+        <v>17916</v>
+      </c>
+      <c r="Z60">
+        <v>0</v>
+      </c>
+      <c r="AA60">
+        <v>0.191</v>
+      </c>
+      <c r="AB60">
+        <v>10.653</v>
+      </c>
+      <c r="AC60">
+        <v>1.706</v>
+      </c>
+      <c r="AD60">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AE60">
+        <v>11.337</v>
+      </c>
+      <c r="AF60">
+        <v>11.384</v>
+      </c>
+      <c r="AG60">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="AH60">
+        <v>10.25</v>
+      </c>
+      <c r="AI60">
+        <v>10.298999999999999</v>
+      </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A61">
@@ -7334,6 +8027,102 @@
       <c r="C61" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D61">
+        <v>2087</v>
+      </c>
+      <c r="E61" s="2">
+        <v>2295</v>
+      </c>
+      <c r="F61" s="2">
+        <v>10</v>
+      </c>
+      <c r="G61" s="2">
+        <v>32</v>
+      </c>
+      <c r="H61" s="2">
+        <v>20</v>
+      </c>
+      <c r="I61" s="2">
+        <v>2</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="L61">
+        <v>0.153</v>
+      </c>
+      <c r="M61">
+        <v>0.217</v>
+      </c>
+      <c r="N61">
+        <v>0.151</v>
+      </c>
+      <c r="O61">
+        <v>0.108</v>
+      </c>
+      <c r="P61">
+        <v>0.157</v>
+      </c>
+      <c r="Q61">
+        <v>0.151</v>
+      </c>
+      <c r="R61">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="S61">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="T61">
+        <v>5459</v>
+      </c>
+      <c r="U61">
+        <v>5667</v>
+      </c>
+      <c r="V61">
+        <v>853</v>
+      </c>
+      <c r="W61">
+        <v>12856</v>
+      </c>
+      <c r="X61">
+        <v>24007</v>
+      </c>
+      <c r="Y61">
+        <v>11151</v>
+      </c>
+      <c r="Z61">
+        <v>0</v>
+      </c>
+      <c r="AA61">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AB61">
+        <v>4.5730000000000004</v>
+      </c>
+      <c r="AC61">
+        <v>4.62</v>
+      </c>
+      <c r="AD61">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AE61">
+        <v>4.4210000000000003</v>
+      </c>
+      <c r="AF61">
+        <v>4.47</v>
+      </c>
+      <c r="AG61">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="AH61">
+        <v>4.4560000000000004</v>
+      </c>
+      <c r="AI61">
+        <v>4.5010000000000003</v>
+      </c>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A62">
@@ -7345,6 +8134,102 @@
       <c r="C62" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D62">
+        <v>2056</v>
+      </c>
+      <c r="E62">
+        <v>2254</v>
+      </c>
+      <c r="F62">
+        <v>10</v>
+      </c>
+      <c r="G62">
+        <v>56</v>
+      </c>
+      <c r="H62">
+        <v>18</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0.15</v>
+      </c>
+      <c r="L62">
+        <v>0.104</v>
+      </c>
+      <c r="M62">
+        <v>0.151</v>
+      </c>
+      <c r="N62">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="O62">
+        <v>0.109</v>
+      </c>
+      <c r="P62">
+        <v>0.157</v>
+      </c>
+      <c r="Q62">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="R62">
+        <v>0.104</v>
+      </c>
+      <c r="S62">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="T62">
+        <v>6016</v>
+      </c>
+      <c r="U62">
+        <v>6214</v>
+      </c>
+      <c r="V62">
+        <v>1000</v>
+      </c>
+      <c r="W62">
+        <v>9861</v>
+      </c>
+      <c r="X62">
+        <v>17654</v>
+      </c>
+      <c r="Y62">
+        <v>7831</v>
+      </c>
+      <c r="Z62">
+        <v>0</v>
+      </c>
+      <c r="AA62">
+        <v>0.214</v>
+      </c>
+      <c r="AB62">
+        <v>4.8760000000000003</v>
+      </c>
+      <c r="AC62">
+        <v>4.9349999999999996</v>
+      </c>
+      <c r="AD62">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AE62">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="AF62">
+        <v>4.6970000000000001</v>
+      </c>
+      <c r="AG62">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="AH62">
+        <v>4.8550000000000004</v>
+      </c>
+      <c r="AI62">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A63">
@@ -7356,9 +8241,102 @@
       <c r="C63" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="D63" s="2">
+        <v>2744</v>
+      </c>
+      <c r="E63" s="2">
+        <v>3017</v>
+      </c>
+      <c r="F63" s="2">
+        <v>10</v>
+      </c>
+      <c r="G63">
+        <v>61</v>
+      </c>
+      <c r="H63">
+        <v>15</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0.152</v>
+      </c>
+      <c r="L63">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="M63">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="N63">
+        <v>0.16</v>
+      </c>
+      <c r="O63">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="P63">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="Q63">
+        <v>0.153</v>
+      </c>
+      <c r="R63">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="S63">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="T63">
+        <v>6704</v>
+      </c>
+      <c r="U63">
+        <v>6977</v>
+      </c>
+      <c r="V63">
+        <v>1000</v>
+      </c>
+      <c r="W63">
+        <v>32055</v>
+      </c>
+      <c r="X63">
+        <v>62039</v>
+      </c>
+      <c r="Y63">
+        <v>30025</v>
+      </c>
+      <c r="Z63">
+        <v>0</v>
+      </c>
+      <c r="AA63">
+        <v>0.246</v>
+      </c>
+      <c r="AB63">
+        <v>15.768000000000001</v>
+      </c>
+      <c r="AC63">
+        <v>15.839</v>
+      </c>
+      <c r="AD63">
+        <v>0.16</v>
+      </c>
+      <c r="AE63">
+        <v>15.113</v>
+      </c>
+      <c r="AF63">
+        <v>15.16</v>
+      </c>
+      <c r="AG63">
+        <v>0.155</v>
+      </c>
+      <c r="AH63">
+        <v>14.912000000000001</v>
+      </c>
+      <c r="AI63">
+        <v>14.959</v>
+      </c>
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A64">
@@ -7370,6 +8348,102 @@
       <c r="C64" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D64">
+        <v>2736</v>
+      </c>
+      <c r="E64">
+        <v>3008</v>
+      </c>
+      <c r="F64">
+        <v>10</v>
+      </c>
+      <c r="G64">
+        <v>54</v>
+      </c>
+      <c r="H64">
+        <v>16</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="L64">
+        <v>0.187</v>
+      </c>
+      <c r="M64">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="N64">
+        <v>0.157</v>
+      </c>
+      <c r="O64">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="P64">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="Q64">
+        <v>0.158</v>
+      </c>
+      <c r="R64">
+        <v>0.126</v>
+      </c>
+      <c r="S64">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="T64">
+        <v>6696</v>
+      </c>
+      <c r="U64">
+        <v>6968</v>
+      </c>
+      <c r="V64">
+        <v>1000</v>
+      </c>
+      <c r="W64">
+        <v>218117</v>
+      </c>
+      <c r="X64">
+        <v>434169</v>
+      </c>
+      <c r="Y64">
+        <v>216091</v>
+      </c>
+      <c r="Z64">
+        <v>0</v>
+      </c>
+      <c r="AA64">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="AB64">
+        <v>81.424000000000007</v>
+      </c>
+      <c r="AC64">
+        <v>81.481999999999999</v>
+      </c>
+      <c r="AD64">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="AE64">
+        <v>80.811000000000007</v>
+      </c>
+      <c r="AF64">
+        <v>80.869</v>
+      </c>
+      <c r="AG64">
+        <v>0.155</v>
+      </c>
+      <c r="AH64">
+        <v>99.641999999999996</v>
+      </c>
+      <c r="AI64">
+        <v>99.691999999999993</v>
+      </c>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A65">
@@ -7381,6 +8455,102 @@
       <c r="C65" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D65">
+        <v>2585</v>
+      </c>
+      <c r="E65">
+        <v>2842</v>
+      </c>
+      <c r="F65">
+        <v>10</v>
+      </c>
+      <c r="G65">
+        <v>46</v>
+      </c>
+      <c r="H65">
+        <v>17</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0.24</v>
+      </c>
+      <c r="L65">
+        <v>0.152</v>
+      </c>
+      <c r="M65">
+        <v>0.217</v>
+      </c>
+      <c r="N65">
+        <v>0.16</v>
+      </c>
+      <c r="O65">
+        <v>0.112</v>
+      </c>
+      <c r="P65">
+        <v>0.16</v>
+      </c>
+      <c r="Q65">
+        <v>0.159</v>
+      </c>
+      <c r="R65">
+        <v>0.105</v>
+      </c>
+      <c r="S65">
+        <v>0.153</v>
+      </c>
+      <c r="T65">
+        <v>6545</v>
+      </c>
+      <c r="U65">
+        <v>6802</v>
+      </c>
+      <c r="V65">
+        <v>1000</v>
+      </c>
+      <c r="W65">
+        <v>405612</v>
+      </c>
+      <c r="X65">
+        <v>809174</v>
+      </c>
+      <c r="Y65">
+        <v>403591</v>
+      </c>
+      <c r="Z65">
+        <v>0</v>
+      </c>
+      <c r="AA65">
+        <v>0.157</v>
+      </c>
+      <c r="AB65">
+        <v>173.24100000000001</v>
+      </c>
+      <c r="AC65">
+        <v>173.29</v>
+      </c>
+      <c r="AD65">
+        <v>0.155</v>
+      </c>
+      <c r="AE65">
+        <v>162.75800000000001</v>
+      </c>
+      <c r="AF65">
+        <v>162.80500000000001</v>
+      </c>
+      <c r="AG65">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="AH65">
+        <v>183.80600000000001</v>
+      </c>
+      <c r="AI65">
+        <v>183.86699999999999</v>
+      </c>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A66">
@@ -7392,6 +8562,102 @@
       <c r="C66" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D66">
+        <v>3313</v>
+      </c>
+      <c r="E66">
+        <v>3639</v>
+      </c>
+      <c r="F66">
+        <v>10</v>
+      </c>
+      <c r="G66">
+        <v>74</v>
+      </c>
+      <c r="H66">
+        <v>19</v>
+      </c>
+      <c r="I66">
+        <v>3</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="L66">
+        <v>0.159</v>
+      </c>
+      <c r="M66">
+        <v>0.215</v>
+      </c>
+      <c r="N66">
+        <v>0.158</v>
+      </c>
+      <c r="O66">
+        <v>0.155</v>
+      </c>
+      <c r="P66">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="Q66">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="R66">
+        <v>0.153</v>
+      </c>
+      <c r="S66">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="T66">
+        <v>7273</v>
+      </c>
+      <c r="U66">
+        <v>7599</v>
+      </c>
+      <c r="V66">
+        <v>1000</v>
+      </c>
+      <c r="W66">
+        <v>550945</v>
+      </c>
+      <c r="X66">
+        <v>1099800</v>
+      </c>
+      <c r="Y66">
+        <v>548911</v>
+      </c>
+      <c r="Z66">
+        <v>0</v>
+      </c>
+      <c r="AA66">
+        <v>0.249</v>
+      </c>
+      <c r="AB66">
+        <v>253.65799999999999</v>
+      </c>
+      <c r="AC66">
+        <v>253.733</v>
+      </c>
+      <c r="AD66">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="AE66">
+        <v>231.95</v>
+      </c>
+      <c r="AF66">
+        <v>232.029</v>
+      </c>
+      <c r="AG66">
+        <v>0.159</v>
+      </c>
+      <c r="AH66">
+        <v>241.191</v>
+      </c>
+      <c r="AI66">
+        <v>241.24799999999999</v>
+      </c>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A67">
@@ -7403,9 +8669,102 @@
       <c r="C67" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T67" s="2"/>
-      <c r="U67" s="2"/>
-      <c r="V67" s="2"/>
+      <c r="D67">
+        <v>3260</v>
+      </c>
+      <c r="E67">
+        <v>3585</v>
+      </c>
+      <c r="F67">
+        <v>10</v>
+      </c>
+      <c r="G67">
+        <v>60</v>
+      </c>
+      <c r="H67">
+        <v>18</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0.161</v>
+      </c>
+      <c r="L67">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="M67">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="N67">
+        <v>0.16</v>
+      </c>
+      <c r="O67">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="P67">
+        <v>0.187</v>
+      </c>
+      <c r="Q67">
+        <v>0.157</v>
+      </c>
+      <c r="R67">
+        <v>0.13</v>
+      </c>
+      <c r="S67">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="T67" s="2">
+        <v>7220</v>
+      </c>
+      <c r="U67" s="2">
+        <v>7545</v>
+      </c>
+      <c r="V67" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W67">
+        <v>249049</v>
+      </c>
+      <c r="X67" s="2">
+        <v>496026</v>
+      </c>
+      <c r="Y67" s="2">
+        <v>247022</v>
+      </c>
+      <c r="Z67">
+        <v>0</v>
+      </c>
+      <c r="AA67">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="AB67">
+        <v>72.194999999999993</v>
+      </c>
+      <c r="AC67">
+        <v>72.269000000000005</v>
+      </c>
+      <c r="AD67">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="AE67">
+        <v>73.006</v>
+      </c>
+      <c r="AF67">
+        <v>73.052999999999997</v>
+      </c>
+      <c r="AG67">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="AH67">
+        <v>75.793000000000006</v>
+      </c>
+      <c r="AI67">
+        <v>75.84</v>
+      </c>
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A68">
@@ -7417,16 +8776,106 @@
       <c r="C68" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T68" s="2"/>
-      <c r="U68" s="2"/>
-      <c r="V68" s="2"/>
-      <c r="AA68" s="2"/>
-      <c r="AB68" s="2"/>
-      <c r="AC68" s="2"/>
+      <c r="D68">
+        <v>3230</v>
+      </c>
+      <c r="E68">
+        <v>3549</v>
+      </c>
+      <c r="F68">
+        <v>10</v>
+      </c>
+      <c r="G68">
+        <v>69</v>
+      </c>
+      <c r="H68">
+        <v>34</v>
+      </c>
+      <c r="I68">
+        <v>10</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="L68">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="M68">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="N68">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="O68">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="P68">
+        <v>0.183</v>
+      </c>
+      <c r="Q68">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="R68">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="S68">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="T68" s="2">
+        <v>7190</v>
+      </c>
+      <c r="U68" s="2">
+        <v>7509</v>
+      </c>
+      <c r="V68" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W68">
+        <v>35975</v>
+      </c>
+      <c r="X68">
+        <v>69868</v>
+      </c>
+      <c r="Y68">
+        <v>33938</v>
+      </c>
+      <c r="Z68">
+        <v>0</v>
+      </c>
+      <c r="AA68" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="AB68" s="2">
+        <v>12.672000000000001</v>
+      </c>
+      <c r="AC68" s="2">
+        <v>12.718</v>
+      </c>
+      <c r="AD68">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="AE68">
+        <v>12.303000000000001</v>
+      </c>
+      <c r="AF68">
+        <v>12.35</v>
+      </c>
+      <c r="AG68">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AH68">
+        <v>12.19</v>
+      </c>
+      <c r="AI68">
+        <v>12.236000000000001</v>
+      </c>
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.3">
@@ -7658,7 +9107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>20</v>
       </c>
@@ -7673,7 +9122,7 @@
       <c r="X81" s="2"/>
       <c r="Y81" s="2"/>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>21</v>
       </c>
@@ -7684,7 +9133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>22</v>
       </c>
@@ -7695,7 +9144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>30</v>
       </c>
@@ -7709,7 +9158,7 @@
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>31</v>
       </c>
@@ -7720,7 +9169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>32</v>
       </c>
@@ -7731,7 +9180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>40</v>
       </c>
@@ -7742,7 +9191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>41</v>
       </c>
@@ -7756,7 +9205,7 @@
       <c r="U88" s="2"/>
       <c r="V88" s="2"/>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>42</v>
       </c>
@@ -7773,384 +9222,8 @@
       <c r="AB89" s="2"/>
       <c r="AC89" s="2"/>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L94" s="7"/>
-      <c r="M94" s="7"/>
-      <c r="N94" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="O94" s="7"/>
-      <c r="P94" s="7"/>
-      <c r="Q94" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="R94" s="7"/>
-      <c r="S94" s="7"/>
-      <c r="T94" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="U94" s="7"/>
-      <c r="V94" s="7"/>
-      <c r="W94" s="7"/>
-      <c r="X94" s="7"/>
-      <c r="Y94" s="7"/>
-      <c r="Z94" s="7"/>
-      <c r="AA94" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB94" s="7"/>
-      <c r="AC94" s="7"/>
-      <c r="AD94" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE94" s="7"/>
-      <c r="AF94" s="7"/>
-      <c r="AG94" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH94" s="7"/>
-      <c r="AI94" s="7"/>
-    </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>0</v>
-      </c>
-      <c r="B95" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" t="s">
-        <v>3</v>
-      </c>
-      <c r="D95" t="s">
-        <v>27</v>
-      </c>
-      <c r="E95" t="s">
-        <v>28</v>
-      </c>
-      <c r="F95" t="s">
-        <v>29</v>
-      </c>
-      <c r="G95" t="s">
-        <v>30</v>
-      </c>
-      <c r="H95" t="s">
-        <v>36</v>
-      </c>
-      <c r="I95" t="s">
-        <v>31</v>
-      </c>
-      <c r="J95" t="s">
-        <v>32</v>
-      </c>
-      <c r="K95" t="s">
-        <v>17</v>
-      </c>
-      <c r="L95" t="s">
-        <v>18</v>
-      </c>
-      <c r="M95" t="s">
-        <v>19</v>
-      </c>
-      <c r="N95" t="s">
-        <v>20</v>
-      </c>
-      <c r="O95" t="s">
-        <v>21</v>
-      </c>
-      <c r="P95" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>23</v>
-      </c>
-      <c r="R95" t="s">
-        <v>24</v>
-      </c>
-      <c r="S95" t="s">
-        <v>25</v>
-      </c>
-      <c r="T95" t="s">
-        <v>37</v>
-      </c>
-      <c r="U95" t="s">
-        <v>38</v>
-      </c>
-      <c r="V95" t="s">
-        <v>39</v>
-      </c>
-      <c r="W95" t="s">
-        <v>40</v>
-      </c>
-      <c r="X95" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y95" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z95" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA95" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB95" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC95" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD95" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE95" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF95" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG95" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH95" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI95" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <v>0</v>
-      </c>
-      <c r="B96">
-        <v>1</v>
-      </c>
-      <c r="C96">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <v>1</v>
-      </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-      <c r="C97">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <v>2</v>
-      </c>
-      <c r="B98">
-        <v>1</v>
-      </c>
-      <c r="C98">
-        <v>9</v>
-      </c>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
-      <c r="K98" s="2"/>
-      <c r="L98" s="2"/>
-      <c r="M98" s="2"/>
-      <c r="N98" s="2"/>
-      <c r="O98" s="2"/>
-      <c r="P98" s="2"/>
-      <c r="Q98" s="2"/>
-      <c r="R98" s="2"/>
-      <c r="S98" s="2"/>
-    </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <v>10</v>
-      </c>
-      <c r="B99">
-        <v>2</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>11</v>
-      </c>
-      <c r="B100">
-        <v>2</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="T100" s="2"/>
-      <c r="U100" s="2"/>
-      <c r="V100" s="2"/>
-      <c r="W100" s="2"/>
-      <c r="X100" s="2"/>
-      <c r="Y100" s="2"/>
-    </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>12</v>
-      </c>
-      <c r="B101">
-        <v>2</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <v>20</v>
-      </c>
-      <c r="B102">
-        <v>3</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="V102" s="2"/>
-      <c r="W102" s="2"/>
-      <c r="X102" s="2"/>
-      <c r="Y102" s="2"/>
-    </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <v>21</v>
-      </c>
-      <c r="B103">
-        <v>3</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A104">
-        <v>22</v>
-      </c>
-      <c r="B104">
-        <v>3</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A105">
-        <v>30</v>
-      </c>
-      <c r="B105">
-        <v>4</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-    </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A106">
-        <v>31</v>
-      </c>
-      <c r="B106">
-        <v>4</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A107">
-        <v>32</v>
-      </c>
-      <c r="B107">
-        <v>4</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <v>40</v>
-      </c>
-      <c r="B108">
-        <v>5</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A109">
-        <v>41</v>
-      </c>
-      <c r="B109">
-        <v>5</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="T109" s="2"/>
-      <c r="U109" s="2"/>
-      <c r="V109" s="2"/>
-    </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <v>42</v>
-      </c>
-      <c r="B110">
-        <v>5</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T110" s="2"/>
-      <c r="U110" s="2"/>
-      <c r="V110" s="2"/>
-      <c r="AA110" s="2"/>
-      <c r="AB110" s="2"/>
-      <c r="AC110" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="AA94:AC94"/>
-    <mergeCell ref="AD94:AF94"/>
-    <mergeCell ref="AG94:AI94"/>
-    <mergeCell ref="D94:J94"/>
-    <mergeCell ref="K94:M94"/>
-    <mergeCell ref="N94:P94"/>
-    <mergeCell ref="Q94:S94"/>
-    <mergeCell ref="T94:Z94"/>
+  <mergeCells count="32">
     <mergeCell ref="AD10:AF10"/>
     <mergeCell ref="AG10:AI10"/>
     <mergeCell ref="T10:Z10"/>
@@ -8186,12 +9259,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
-    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating tests summary for Heuristic 3.
</commit_message>
<xml_diff>
--- a/docs/testsFSG/tests-summary.xlsx
+++ b/docs/testsFSG/tests-summary.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
-    <sheet name="Models" sheetId="1" r:id="rId2"/>
+    <sheet name="40 - Models" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="72">
   <si>
     <t>Run</t>
   </si>
@@ -213,9 +213,6 @@
     <t>Heuristic 3</t>
   </si>
   <si>
-    <t>Heuristic 4</t>
-  </si>
-  <si>
     <t>#CTC per FM:</t>
   </si>
   <si>
@@ -238,6 +235,12 @@
   </si>
   <si>
     <t>Features: 40, Heuristic 3: Default + BiVarArithmetic + OrAttr0 + OrAttr1</t>
+  </si>
+  <si>
+    <t>Features: 40, Heuristic 4: Default + OrAttr0 + OrAttr1</t>
+  </si>
+  <si>
+    <t>Constraints</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,19 @@
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="169" formatCode="0.000"/>
     </dxf>
@@ -383,7 +398,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-CO"/>
-              <a:t>10 Solutions</a:t>
+              <a:t>1000 Solutions</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -429,11 +444,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$B$1</c:f>
+              <c:f>Summary!$B$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Default</c:v>
+                  <c:v>Constraints</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -452,7 +467,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Summary!$A$2:$A$6</c:f>
+              <c:f>Summary!$A$11:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -476,25 +491,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$2:$B$6</c:f>
+              <c:f>Summary!$B$11:$B$15</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9.1187269729718287E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.11180847459261625</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.17014395193802512</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.19116987590893744</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.23112729160001227</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -505,11 +505,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$C$1</c:f>
+              <c:f>Summary!$C$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Heuristic 1</c:v>
+                  <c:v>Default</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -528,7 +528,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Summary!$A$2:$A$6</c:f>
+              <c:f>Summary!$A$11:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -552,24 +552,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$C$2:$C$6</c:f>
+              <c:f>Summary!$C$11:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6.5905807503954361E-2</c:v>
+                  <c:v>0.30144674955333528</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.5653949321746303E-2</c:v>
+                  <c:v>0.70487610846063131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10691845154486945</c:v>
+                  <c:v>7.1782102891205311</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14034154529106099</c:v>
+                  <c:v>30.133753885968989</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.22708745996596125</c:v>
+                  <c:v>9.3311456376174444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -581,11 +581,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$D$1</c:f>
+              <c:f>Summary!$D$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Heuristic 2</c:v>
+                  <c:v>Heuristic 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -604,7 +604,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Summary!$A$2:$A$6</c:f>
+              <c:f>Summary!$A$11:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -628,24 +628,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$D$2:$D$6</c:f>
+              <c:f>Summary!$D$11:$D$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.837459345418106E-2</c:v>
+                  <c:v>0.26271717043663456</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.973155770843153E-2</c:v>
+                  <c:v>0.9855389183779858</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11130381037109011</c:v>
+                  <c:v>7.3579809941861845</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12629952919295748</c:v>
+                  <c:v>31.92406529142966</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14112515449175733</c:v>
+                  <c:v>13.845771604971324</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -657,11 +657,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$E$1</c:f>
+              <c:f>Summary!$E$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Heuristic 3</c:v>
+                  <c:v>Heuristic 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -680,7 +680,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Summary!$A$2:$A$6</c:f>
+              <c:f>Summary!$A$11:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -704,10 +704,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$E$2:$E$6</c:f>
+              <c:f>Summary!$E$11:$E$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.3103117867143107</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7290030969009762</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7141563995510145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.188664846837895</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.470053843172394</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -718,11 +733,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$F$1</c:f>
+              <c:f>Summary!$F$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Heuristic 4</c:v>
+                  <c:v>Heuristic 3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -741,7 +756,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Summary!$A$2:$A$6</c:f>
+              <c:f>Summary!$A$11:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -765,10 +780,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$F$2:$F$6</c:f>
+              <c:f>Summary!$F$11:$F$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.28661775870741463</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69737861410103907</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9914634565127107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.766448089786131</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.888986502272239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -783,11 +813,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="180378096"/>
-        <c:axId val="180374568"/>
+        <c:axId val="180378880"/>
+        <c:axId val="180371432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="180378096"/>
+        <c:axId val="180378880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +860,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180374568"/>
+        <c:crossAx val="180371432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -838,8 +868,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180374568"/>
+        <c:axId val="180371432"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -858,7 +889,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -889,7 +920,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180378096"/>
+        <c:crossAx val="180378880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1005,7 +1036,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-CO"/>
-              <a:t>1000 Solutions</a:t>
+              <a:t>10 Solutions - Models</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1051,7 +1082,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$B$10</c:f>
+              <c:f>Summary!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1074,7 +1105,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Summary!$A$11:$A$15</c:f>
+              <c:f>Summary!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1098,24 +1129,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$11:$B$15</c:f>
+              <c:f>Summary!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.30144674955333528</c:v>
+                  <c:v>9.1187269729718287E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70487610846063131</c:v>
+                  <c:v>0.11180847459261625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1782102891205311</c:v>
+                  <c:v>0.17014395193802512</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.133753885968989</c:v>
+                  <c:v>0.19116987590893744</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3311456376174444</c:v>
+                  <c:v>0.23112729160001227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,7 +1158,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$C$10</c:f>
+              <c:f>Summary!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1150,7 +1181,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Summary!$A$11:$A$15</c:f>
+              <c:f>Summary!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1174,24 +1205,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$C$11:$C$15</c:f>
+              <c:f>Summary!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.26271717043663456</c:v>
+                  <c:v>6.5905807503954361E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9855389183779858</c:v>
+                  <c:v>8.5653949321746303E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.3579809941861845</c:v>
+                  <c:v>0.10691845154486945</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.92406529142966</c:v>
+                  <c:v>0.14034154529106099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.845771604971324</c:v>
+                  <c:v>0.22708745996596125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1203,7 +1234,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$D$10</c:f>
+              <c:f>Summary!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1226,7 +1257,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Summary!$A$11:$A$15</c:f>
+              <c:f>Summary!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1250,24 +1281,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$D$11:$D$15</c:f>
+              <c:f>Summary!$E$2:$E$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3103117867143107</c:v>
+                  <c:v>7.837459345418106E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7290030969009762</c:v>
+                  <c:v>7.973155770843153E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7141563995510145</c:v>
+                  <c:v>0.11130381037109011</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.188664846837895</c:v>
+                  <c:v>0.12629952919295748</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.470053843172394</c:v>
+                  <c:v>0.14112515449175733</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1279,7 +1310,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$E$10</c:f>
+              <c:f>Summary!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1302,7 +1333,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Summary!$A$11:$A$15</c:f>
+              <c:f>Summary!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1326,71 +1357,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$E$11:$E$15</c:f>
+              <c:f>Summary!$F$2:$F$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Summary!$F$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Heuristic 4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Summary!$A$11:$A$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>6.5412518447039589E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>7.472896132803894E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0.10156336722046637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0.12323666324336834</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>0.15417903466059946</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Summary!$F$11:$F$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1405,11 +1390,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="180378880"/>
-        <c:axId val="180371432"/>
+        <c:axId val="248623888"/>
+        <c:axId val="248622320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="180378880"/>
+        <c:axId val="248623888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1452,7 +1437,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180371432"/>
+        <c:crossAx val="248622320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1460,9 +1445,8 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180371432"/>
+        <c:axId val="248622320"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1512,7 +1496,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180378880"/>
+        <c:crossAx val="248623888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2709,36 +2693,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
@@ -2761,6 +2715,36 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>601133</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>296333</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
@@ -2775,11 +2759,11 @@
   <autoFilter ref="A10:F15"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Models"/>
-    <tableColumn id="2" name="Default" dataDxfId="1"/>
-    <tableColumn id="3" name="Heuristic 1" dataDxfId="0"/>
-    <tableColumn id="4" name="Heuristic 2"/>
-    <tableColumn id="5" name="Heuristic 3"/>
-    <tableColumn id="6" name="Heuristic 4"/>
+    <tableColumn id="6" name="Constraints"/>
+    <tableColumn id="2" name="Default" dataDxfId="5"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="4"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="1"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2790,11 +2774,11 @@
   <autoFilter ref="A1:F6"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Models"/>
-    <tableColumn id="2" name="Default" dataDxfId="2"/>
+    <tableColumn id="6" name="Constraints"/>
+    <tableColumn id="2" name="Default" dataDxfId="6"/>
     <tableColumn id="3" name="Heuristic 1"/>
-    <tableColumn id="4" name="Heuristic 2"/>
-    <tableColumn id="5" name="Heuristic 3"/>
-    <tableColumn id="6" name="Heuristic 4"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="3"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2935,6 +2919,50 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1437" displayName="Table1437" ref="A74:AI89" totalsRowShown="0" dataCellStyle="Normal">
   <autoFilter ref="A74:AI89"/>
+  <tableColumns count="35">
+    <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
+    <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
+    <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
+    <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
+    <tableColumn id="34" name="Nodes5" dataCellStyle="Normal"/>
+    <tableColumn id="33" name="Backtracks6" dataCellStyle="Normal"/>
+    <tableColumn id="32" name="Fails7" dataCellStyle="Normal"/>
+    <tableColumn id="29" name="Restarts8" dataCellStyle="Normal"/>
+    <tableColumn id="20" name="Building Time3" dataCellStyle="Normal"/>
+    <tableColumn id="21" name="Resolution Time2" dataCellStyle="Normal"/>
+    <tableColumn id="22" name="Execution Time2" dataCellStyle="Normal"/>
+    <tableColumn id="23" name="Building Time32" dataCellStyle="Normal"/>
+    <tableColumn id="24" name="Resolution Time23" dataCellStyle="Normal"/>
+    <tableColumn id="25" name="Execution Time24" dataCellStyle="Normal"/>
+    <tableColumn id="26" name="Building Time33" dataCellStyle="Normal"/>
+    <tableColumn id="27" name="Resolution Time24" dataCellStyle="Normal"/>
+    <tableColumn id="28" name="Execution Time25" dataCellStyle="Normal"/>
+    <tableColumn id="37" name="Variables3" dataCellStyle="Normal"/>
+    <tableColumn id="38" name="Constraints4" dataCellStyle="Normal"/>
+    <tableColumn id="39" name="Solutions5" dataCellStyle="Normal"/>
+    <tableColumn id="40" name="Nodes6" dataCellStyle="Normal"/>
+    <tableColumn id="41" name="Backtracks7" dataCellStyle="Normal"/>
+    <tableColumn id="42" name="Fails8" dataCellStyle="Normal"/>
+    <tableColumn id="43" name="Restarts9" dataCellStyle="Normal"/>
+    <tableColumn id="44" name="Building Time10" dataCellStyle="Normal"/>
+    <tableColumn id="45" name="Resolution Time11" dataCellStyle="Normal"/>
+    <tableColumn id="46" name="Execution Time12" dataCellStyle="Normal"/>
+    <tableColumn id="47" name="Building Time213" dataCellStyle="Normal"/>
+    <tableColumn id="48" name="Resolution Time314" dataCellStyle="Normal"/>
+    <tableColumn id="49" name="Execution Time415" dataCellStyle="Normal"/>
+    <tableColumn id="50" name="Building Time516" dataCellStyle="Normal"/>
+    <tableColumn id="51" name="Resolution Time617" dataCellStyle="Normal"/>
+    <tableColumn id="52" name="Execution Time718" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14378" displayName="Table14378" ref="A95:AI110" totalsRowShown="0" dataCellStyle="Normal">
+  <autoFilter ref="A95:AI110"/>
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
@@ -3241,8 +3269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3256,104 +3284,144 @@
         <v>58</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8">
-        <f>HARMEAN(Models!L12:L14,Models!O12:O14,Models!R12:R14)</f>
+      <c r="B2">
+        <f>'40 - Models'!B2*'40 - Models'!B6*'40 - Models'!B12+'40 - Models'!B2*'40 - Models'!B3*'40 - Models'!B12</f>
+        <v>6</v>
+      </c>
+      <c r="C2" s="8">
+        <f>HARMEAN('40 - Models'!L12:L14,'40 - Models'!O12:O14,'40 - Models'!R12:R14)</f>
         <v>9.1187269729718287E-2</v>
       </c>
-      <c r="C2" s="8">
-        <f>HARMEAN(Models!L33:L35,Models!O33:O35,Models!R33:R35)</f>
+      <c r="D2" s="8">
+        <f>HARMEAN('40 - Models'!L33:L35,'40 - Models'!O33:O35,'40 - Models'!R33:R35)</f>
         <v>6.5905807503954361E-2</v>
       </c>
-      <c r="D2">
-        <f>HARMEAN(Models!L54:L56,Models!O54:O56,Models!R54:R56)</f>
+      <c r="E2" s="8">
+        <f>HARMEAN('40 - Models'!L54:L56,'40 - Models'!O54:O56,'40 - Models'!R54:R56)</f>
         <v>7.837459345418106E-2</v>
+      </c>
+      <c r="F2" s="8">
+        <f>HARMEAN('40 - Models'!L75:L77,'40 - Models'!O75:O77,'40 - Models'!R75:R77)</f>
+        <v>6.5412518447039589E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
-        <f>HARMEAN(Models!L15:L17,Models!O15:O17,Models!R15:R17)</f>
+      <c r="B3">
+        <f>'40 - Models'!B2*'40 - Models'!B6*'40 - Models'!B15+'40 - Models'!B2*'40 - Models'!B3*'40 - Models'!B15</f>
+        <v>12</v>
+      </c>
+      <c r="C3" s="8">
+        <f>HARMEAN('40 - Models'!L15:L17,'40 - Models'!O15:O17,'40 - Models'!R15:R17)</f>
         <v>0.11180847459261625</v>
       </c>
-      <c r="C3" s="8">
-        <f>HARMEAN(Models!L36:L38,Models!O36:O38,Models!R36:R38)</f>
+      <c r="D3" s="8">
+        <f>HARMEAN('40 - Models'!L36:L38,'40 - Models'!O36:O38,'40 - Models'!R36:R38)</f>
         <v>8.5653949321746303E-2</v>
       </c>
-      <c r="D3">
-        <f>HARMEAN(Models!L57:L59,Models!O57:O59,Models!R57:R59)</f>
+      <c r="E3" s="8">
+        <f>HARMEAN('40 - Models'!L57:L59,'40 - Models'!O57:O59,'40 - Models'!R57:R59)</f>
         <v>7.973155770843153E-2</v>
+      </c>
+      <c r="F3" s="8">
+        <f>HARMEAN('40 - Models'!L78:L80,'40 - Models'!O78:O80,'40 - Models'!R78:R80)</f>
+        <v>7.472896132803894E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
-        <f>HARMEAN(Models!L18:L20,Models!O18:O20,Models!R18:R20)</f>
+      <c r="B4">
+        <f>'40 - Models'!B2*'40 - Models'!B6*'40 - Models'!B18+'40 - Models'!B2*'40 - Models'!B3*'40 - Models'!B18</f>
+        <v>18</v>
+      </c>
+      <c r="C4" s="8">
+        <f>HARMEAN('40 - Models'!L18:L20,'40 - Models'!O18:O20,'40 - Models'!R18:R20)</f>
         <v>0.17014395193802512</v>
       </c>
-      <c r="C4" s="8">
-        <f>HARMEAN(Models!L39:L41,Models!O39:O41,Models!R39:R41)</f>
+      <c r="D4" s="8">
+        <f>HARMEAN('40 - Models'!L39:L41,'40 - Models'!O39:O41,'40 - Models'!R39:R41)</f>
         <v>0.10691845154486945</v>
       </c>
-      <c r="D4">
-        <f>HARMEAN(Models!L60:L62,Models!O60:O62,Models!R60:R62)</f>
+      <c r="E4" s="8">
+        <f>HARMEAN('40 - Models'!L60:L62,'40 - Models'!O60:O62,'40 - Models'!R60:R62)</f>
         <v>0.11130381037109011</v>
+      </c>
+      <c r="F4" s="8">
+        <f>HARMEAN('40 - Models'!L81:L83,'40 - Models'!O81:O83,'40 - Models'!R81:R83)</f>
+        <v>0.10156336722046637</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
-        <f>HARMEAN(Models!L21:L23,Models!O21:O23,Models!R21:R23)</f>
+      <c r="B5">
+        <f>'40 - Models'!B2*'40 - Models'!B6*'40 - Models'!B21+'40 - Models'!B2*'40 - Models'!B3*'40 - Models'!B21</f>
+        <v>24</v>
+      </c>
+      <c r="C5" s="8">
+        <f>HARMEAN('40 - Models'!L21:L23,'40 - Models'!O21:O23,'40 - Models'!R21:R23)</f>
         <v>0.19116987590893744</v>
       </c>
-      <c r="C5" s="8">
-        <f>HARMEAN(Models!L42:L44,Models!O42:O44,Models!R42:R44)</f>
+      <c r="D5" s="8">
+        <f>HARMEAN('40 - Models'!L42:L44,'40 - Models'!O42:O44,'40 - Models'!R42:R44)</f>
         <v>0.14034154529106099</v>
       </c>
-      <c r="D5">
-        <f>HARMEAN(Models!L63:L65,Models!O63:O65,Models!R63:R65)</f>
+      <c r="E5" s="8">
+        <f>HARMEAN('40 - Models'!L63:L65,'40 - Models'!O63:O65,'40 - Models'!R63:R65)</f>
         <v>0.12629952919295748</v>
+      </c>
+      <c r="F5" s="8">
+        <f>HARMEAN('40 - Models'!L84:L86,'40 - Models'!O84:O86,'40 - Models'!R84:R86)</f>
+        <v>0.12323666324336834</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
-        <f>HARMEAN(Models!L24:L26,Models!O24:O26,Models!R24:R26)</f>
+      <c r="B6">
+        <f>'40 - Models'!B2*'40 - Models'!B6*'40 - Models'!B24+'40 - Models'!B2*'40 - Models'!B3*'40 - Models'!B24</f>
+        <v>30</v>
+      </c>
+      <c r="C6" s="8">
+        <f>HARMEAN('40 - Models'!L24:L26,'40 - Models'!O24:O26,'40 - Models'!R24:R26)</f>
         <v>0.23112729160001227</v>
       </c>
-      <c r="C6" s="8">
-        <f>HARMEAN(Models!L45:L47,Models!O45:O47,Models!R45:R47)</f>
+      <c r="D6" s="8">
+        <f>HARMEAN('40 - Models'!L45:L47,'40 - Models'!O45:O47,'40 - Models'!R45:R47)</f>
         <v>0.22708745996596125</v>
       </c>
-      <c r="D6">
-        <f>HARMEAN(Models!L66:L68,Models!O66:O68,Models!R66:R68)</f>
+      <c r="E6" s="8">
+        <f>HARMEAN('40 - Models'!L66:L68,'40 - Models'!O66:O68,'40 - Models'!R66:R68)</f>
         <v>0.14112515449175733</v>
+      </c>
+      <c r="F6" s="8">
+        <f>HARMEAN('40 - Models'!L87:L89,'40 - Models'!O87:O89,'40 - Models'!R87:R89)</f>
+        <v>0.15417903466059946</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3361,104 +3429,124 @@
         <v>58</v>
       </c>
       <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>59</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>60</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" s="8">
-        <f>HARMEAN(Models!AB12:AB14,Models!AE12:AE14,Models!AH12:AH14)</f>
+      <c r="C11" s="8">
+        <f>HARMEAN('40 - Models'!AB12:AB14,'40 - Models'!AE12:AE14,'40 - Models'!AH12:AH14)</f>
         <v>0.30144674955333528</v>
       </c>
-      <c r="C11" s="8">
-        <f>HARMEAN(Models!AB33:AB35,Models!AE33:AE35,Models!AH33:AH35)</f>
+      <c r="D11" s="8">
+        <f>HARMEAN('40 - Models'!AB33:AB35,'40 - Models'!AE33:AE35,'40 - Models'!AH33:AH35)</f>
         <v>0.26271717043663456</v>
       </c>
-      <c r="D11">
-        <f>HARMEAN(Models!AB54:AB56,Models!AE54:AE56,Models!AH54:AH56)</f>
+      <c r="E11" s="8">
+        <f>HARMEAN('40 - Models'!AB54:AB56,'40 - Models'!AE54:AE56,'40 - Models'!AH54:AH56)</f>
         <v>0.3103117867143107</v>
+      </c>
+      <c r="F11" s="8">
+        <f>HARMEAN('40 - Models'!AB75:AB77,'40 - Models'!AE75:AE77,'40 - Models'!AH75:AH77)</f>
+        <v>0.28661775870741463</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12" s="8">
-        <f>HARMEAN(Models!AB15:AB17,Models!AE15:AE17,Models!AH15:AH17)</f>
+      <c r="C12" s="8">
+        <f>HARMEAN('40 - Models'!AB15:AB17,'40 - Models'!AE15:AE17,'40 - Models'!AH15:AH17)</f>
         <v>0.70487610846063131</v>
       </c>
-      <c r="C12" s="8">
-        <f>HARMEAN(Models!AB36:AB38,Models!AE36:AE38,Models!AH36:AH38)</f>
+      <c r="D12" s="8">
+        <f>HARMEAN('40 - Models'!AB36:AB38,'40 - Models'!AE36:AE38,'40 - Models'!AH36:AH38)</f>
         <v>0.9855389183779858</v>
       </c>
-      <c r="D12">
-        <f>HARMEAN(Models!AB57:AB59,Models!AE57:AE59,Models!AH57:AH59)</f>
+      <c r="E12" s="8">
+        <f>HARMEAN('40 - Models'!AB57:AB59,'40 - Models'!AE57:AE59,'40 - Models'!AH57:AH59)</f>
         <v>0.7290030969009762</v>
+      </c>
+      <c r="F12" s="8">
+        <f>HARMEAN('40 - Models'!AB78:AB80,'40 - Models'!AE78:AE80,'40 - Models'!AH78:AH80)</f>
+        <v>0.69737861410103907</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
-      <c r="B13" s="8">
-        <f>HARMEAN(Models!AB18:AB20,Models!AE18:AE20,Models!AH18:AH20)</f>
+      <c r="C13" s="8">
+        <f>HARMEAN('40 - Models'!AB18:AB20,'40 - Models'!AE18:AE20,'40 - Models'!AH18:AH20)</f>
         <v>7.1782102891205311</v>
       </c>
-      <c r="C13" s="8">
-        <f>HARMEAN(Models!AB39:AB41,Models!AE39:AE41,Models!AH39:AH41)</f>
+      <c r="D13" s="8">
+        <f>HARMEAN('40 - Models'!AB39:AB41,'40 - Models'!AE39:AE41,'40 - Models'!AH39:AH41)</f>
         <v>7.3579809941861845</v>
       </c>
-      <c r="D13">
-        <f>HARMEAN(Models!AB60:AB62,Models!AE60:AE62,Models!AH60:AH62)</f>
+      <c r="E13" s="8">
+        <f>HARMEAN('40 - Models'!AB60:AB62,'40 - Models'!AE60:AE62,'40 - Models'!AH60:AH62)</f>
         <v>5.7141563995510145</v>
+      </c>
+      <c r="F13" s="8">
+        <f>HARMEAN('40 - Models'!AB81:AB83,'40 - Models'!AE81:AE83,'40 - Models'!AH81:AH83)</f>
+        <v>4.9914634565127107</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
-      <c r="B14" s="8">
-        <f>HARMEAN(Models!AB21:AB23,Models!AE21:AE23,Models!AH21:AH23)</f>
+      <c r="C14" s="8">
+        <f>HARMEAN('40 - Models'!AB21:AB23,'40 - Models'!AE21:AE23,'40 - Models'!AH21:AH23)</f>
         <v>30.133753885968989</v>
       </c>
-      <c r="C14" s="8">
-        <f>HARMEAN(Models!AB42:AB44,Models!AE42:AE44,Models!AH42:AH44)</f>
+      <c r="D14" s="8">
+        <f>HARMEAN('40 - Models'!AB42:AB44,'40 - Models'!AE42:AE44,'40 - Models'!AH42:AH44)</f>
         <v>31.92406529142966</v>
       </c>
-      <c r="D14">
-        <f>HARMEAN(Models!AB63:AB65,Models!AE63:AE65,Models!AH63:AH65)</f>
+      <c r="E14" s="8">
+        <f>HARMEAN('40 - Models'!AB63:AB65,'40 - Models'!AE63:AE65,'40 - Models'!AH63:AH65)</f>
         <v>36.188664846837895</v>
+      </c>
+      <c r="F14" s="8">
+        <f>HARMEAN('40 - Models'!AB84:AB86,'40 - Models'!AE84:AE86,'40 - Models'!AH84:AH86)</f>
+        <v>31.766448089786131</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
-      <c r="B15" s="8">
-        <f>HARMEAN(Models!AB24:AB26,Models!AE24:AE26,Models!AH24:AH26)</f>
+      <c r="C15" s="8">
+        <f>HARMEAN('40 - Models'!AB24:AB26,'40 - Models'!AE24:AE26,'40 - Models'!AH24:AH26)</f>
         <v>9.3311456376174444</v>
       </c>
-      <c r="C15" s="8">
-        <f>HARMEAN(Models!AB45:AB47,Models!AE45:AE47,Models!AH45:AH47)</f>
+      <c r="D15" s="8">
+        <f>HARMEAN('40 - Models'!AB45:AB47,'40 - Models'!AE45:AE47,'40 - Models'!AH45:AH47)</f>
         <v>13.845771604971324</v>
       </c>
-      <c r="D15">
-        <f>HARMEAN(Models!AB66:AB68,Models!AE66:AE68,Models!AH66:AH68)</f>
+      <c r="E15" s="8">
+        <f>HARMEAN('40 - Models'!AB66:AB68,'40 - Models'!AE66:AE68,'40 - Models'!AH66:AH68)</f>
         <v>30.470053843172394</v>
+      </c>
+      <c r="F15" s="8">
+        <f>HARMEAN('40 - Models'!AB87:AB89,'40 - Models'!AE87:AE89,'40 - Models'!AH87:AH89)</f>
+        <v>33.888986502272239</v>
       </c>
     </row>
   </sheetData>
@@ -3473,10 +3561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI89"/>
+  <dimension ref="A1:AI110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="AH77" sqref="AH77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3525,7 +3613,7 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -3533,7 +3621,7 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="5">
         <v>0.1</v>
@@ -3541,7 +3629,7 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3549,7 +3637,7 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -3557,7 +3645,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="5">
         <v>0.05</v>
@@ -5335,7 +5423,7 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
@@ -7105,7 +7193,7 @@
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.3">
@@ -8875,7 +8963,7 @@
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.3">
@@ -9048,6 +9136,102 @@
       <c r="C75">
         <v>19</v>
       </c>
+      <c r="D75">
+        <v>665</v>
+      </c>
+      <c r="E75">
+        <v>723</v>
+      </c>
+      <c r="F75">
+        <v>10</v>
+      </c>
+      <c r="G75">
+        <v>32</v>
+      </c>
+      <c r="H75">
+        <v>21</v>
+      </c>
+      <c r="I75">
+        <v>3</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="L75">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="M75">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="N75">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="O75">
+        <v>6.2E-2</v>
+      </c>
+      <c r="P75">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="Q75">
+        <v>0.114</v>
+      </c>
+      <c r="R75">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="S75">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="T75">
+        <v>2641</v>
+      </c>
+      <c r="U75">
+        <v>2699</v>
+      </c>
+      <c r="V75">
+        <v>504</v>
+      </c>
+      <c r="W75">
+        <v>2534</v>
+      </c>
+      <c r="X75">
+        <v>4061</v>
+      </c>
+      <c r="Y75">
+        <v>1527</v>
+      </c>
+      <c r="Z75">
+        <v>0</v>
+      </c>
+      <c r="AA75">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="AB75">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="AC75">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="AD75">
+        <v>0.113</v>
+      </c>
+      <c r="AE75">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AF75">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="AG75">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AH75">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="AI75">
+        <v>0.81599999999999995</v>
+      </c>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A76">
@@ -9059,6 +9243,102 @@
       <c r="C76">
         <v>24</v>
       </c>
+      <c r="D76">
+        <v>742</v>
+      </c>
+      <c r="E76">
+        <v>811</v>
+      </c>
+      <c r="F76">
+        <v>10</v>
+      </c>
+      <c r="G76">
+        <v>33</v>
+      </c>
+      <c r="H76">
+        <v>20</v>
+      </c>
+      <c r="I76">
+        <v>2</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>0.123</v>
+      </c>
+      <c r="L76">
+        <v>6.2E-2</v>
+      </c>
+      <c r="M76">
+        <v>0.1</v>
+      </c>
+      <c r="N76">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="O76">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="P76">
+        <v>9.4E-2</v>
+      </c>
+      <c r="Q76">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="R76">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="S76">
+        <v>0.106</v>
+      </c>
+      <c r="T76">
+        <v>2310</v>
+      </c>
+      <c r="U76">
+        <v>2379</v>
+      </c>
+      <c r="V76">
+        <v>402</v>
+      </c>
+      <c r="W76">
+        <v>6377</v>
+      </c>
+      <c r="X76">
+        <v>11951</v>
+      </c>
+      <c r="Y76">
+        <v>5574</v>
+      </c>
+      <c r="Z76">
+        <v>0</v>
+      </c>
+      <c r="AA76">
+        <v>0.188</v>
+      </c>
+      <c r="AB76">
+        <v>1.375</v>
+      </c>
+      <c r="AC76">
+        <v>1.429</v>
+      </c>
+      <c r="AD76">
+        <v>0.114</v>
+      </c>
+      <c r="AE76">
+        <v>1.254</v>
+      </c>
+      <c r="AF76">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="AG76">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="AH76">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="AI76">
+        <v>1.2649999999999999</v>
+      </c>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A77">
@@ -9070,6 +9350,102 @@
       <c r="C77">
         <v>9</v>
       </c>
+      <c r="D77">
+        <v>734</v>
+      </c>
+      <c r="E77">
+        <v>801</v>
+      </c>
+      <c r="F77">
+        <v>10</v>
+      </c>
+      <c r="G77">
+        <v>24</v>
+      </c>
+      <c r="H77">
+        <v>14</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="L77">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="M77">
+        <v>0.124</v>
+      </c>
+      <c r="N77">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="O77">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="P77">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="Q77">
+        <v>0.16</v>
+      </c>
+      <c r="R77">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="S77">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="T77">
+        <v>934</v>
+      </c>
+      <c r="U77">
+        <v>1001</v>
+      </c>
+      <c r="V77">
+        <v>60</v>
+      </c>
+      <c r="W77">
+        <v>131</v>
+      </c>
+      <c r="X77">
+        <v>143</v>
+      </c>
+      <c r="Y77">
+        <v>12</v>
+      </c>
+      <c r="Z77">
+        <v>0</v>
+      </c>
+      <c r="AA77">
+        <v>0.152</v>
+      </c>
+      <c r="AB77">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AC77">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="AD77">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AE77">
+        <v>0.109</v>
+      </c>
+      <c r="AF77">
+        <v>0.15</v>
+      </c>
+      <c r="AG77">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AH77">
+        <v>0.108</v>
+      </c>
+      <c r="AI77">
+        <v>0.14799999999999999</v>
+      </c>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A78">
@@ -9081,6 +9457,102 @@
       <c r="C78" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D78">
+        <v>1309</v>
+      </c>
+      <c r="E78">
+        <v>1434</v>
+      </c>
+      <c r="F78">
+        <v>10</v>
+      </c>
+      <c r="G78">
+        <v>30</v>
+      </c>
+      <c r="H78">
+        <v>16</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0.123</v>
+      </c>
+      <c r="L78">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="M78">
+        <v>0.112</v>
+      </c>
+      <c r="N78">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="O78">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="P78">
+        <v>0.124</v>
+      </c>
+      <c r="Q78">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="R78">
+        <v>7.8E-2</v>
+      </c>
+      <c r="S78">
+        <v>0.125</v>
+      </c>
+      <c r="T78">
+        <v>1977</v>
+      </c>
+      <c r="U78">
+        <v>2102</v>
+      </c>
+      <c r="V78">
+        <v>177</v>
+      </c>
+      <c r="W78">
+        <v>995</v>
+      </c>
+      <c r="X78">
+        <v>1637</v>
+      </c>
+      <c r="Y78">
+        <v>642</v>
+      </c>
+      <c r="Z78">
+        <v>0</v>
+      </c>
+      <c r="AA78">
+        <v>0.186</v>
+      </c>
+      <c r="AB78">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="AC78">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="AD78">
+        <v>0.123</v>
+      </c>
+      <c r="AE78">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="AF78">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="AG78">
+        <v>0.18</v>
+      </c>
+      <c r="AH78">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="AI78">
+        <v>0.48099999999999998</v>
+      </c>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A79">
@@ -9092,9 +9564,102 @@
       <c r="C79" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W79" s="2"/>
-      <c r="X79" s="2"/>
-      <c r="Y79" s="2"/>
+      <c r="D79" s="2">
+        <v>1239</v>
+      </c>
+      <c r="E79" s="2">
+        <v>1362</v>
+      </c>
+      <c r="F79" s="2">
+        <v>10</v>
+      </c>
+      <c r="G79">
+        <v>39</v>
+      </c>
+      <c r="H79">
+        <v>24</v>
+      </c>
+      <c r="I79">
+        <v>4</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0.121</v>
+      </c>
+      <c r="L79">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="M79">
+        <v>0.111</v>
+      </c>
+      <c r="N79">
+        <v>0.125</v>
+      </c>
+      <c r="O79">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="P79">
+        <v>0.12</v>
+      </c>
+      <c r="Q79">
+        <v>0.125</v>
+      </c>
+      <c r="R79">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="S79">
+        <v>0.111</v>
+      </c>
+      <c r="T79">
+        <v>3475</v>
+      </c>
+      <c r="U79">
+        <v>3598</v>
+      </c>
+      <c r="V79">
+        <v>569</v>
+      </c>
+      <c r="W79" s="2">
+        <v>10148</v>
+      </c>
+      <c r="X79" s="2">
+        <v>19159</v>
+      </c>
+      <c r="Y79" s="2">
+        <v>9011</v>
+      </c>
+      <c r="Z79">
+        <v>0</v>
+      </c>
+      <c r="AA79">
+        <v>0.125</v>
+      </c>
+      <c r="AB79">
+        <v>2.4449999999999998</v>
+      </c>
+      <c r="AC79">
+        <v>2.4860000000000002</v>
+      </c>
+      <c r="AD79">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AE79">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="AF79">
+        <v>2.5350000000000001</v>
+      </c>
+      <c r="AG79">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AH79">
+        <v>2.4529999999999998</v>
+      </c>
+      <c r="AI79">
+        <v>2.4980000000000002</v>
+      </c>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A80">
@@ -9106,8 +9671,104 @@
       <c r="C80" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D80">
+        <v>1326</v>
+      </c>
+      <c r="E80">
+        <v>1458</v>
+      </c>
+      <c r="F80">
+        <v>10</v>
+      </c>
+      <c r="G80">
+        <v>31</v>
+      </c>
+      <c r="H80">
+        <v>15</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0.124</v>
+      </c>
+      <c r="L80">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M80">
+        <v>0.11</v>
+      </c>
+      <c r="N80">
+        <v>0.124</v>
+      </c>
+      <c r="O80">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="P80">
+        <v>0.115</v>
+      </c>
+      <c r="Q80">
+        <v>0.125</v>
+      </c>
+      <c r="R80">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="S80">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="T80">
+        <v>2662</v>
+      </c>
+      <c r="U80">
+        <v>2794</v>
+      </c>
+      <c r="V80">
+        <v>344</v>
+      </c>
+      <c r="W80">
+        <v>1293</v>
+      </c>
+      <c r="X80">
+        <v>1899</v>
+      </c>
+      <c r="Y80">
+        <v>606</v>
+      </c>
+      <c r="Z80">
+        <v>0</v>
+      </c>
+      <c r="AA80">
+        <v>0.121</v>
+      </c>
+      <c r="AB80">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="AC80">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="AD80">
+        <v>0.122</v>
+      </c>
+      <c r="AE80">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="AF80">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="AG80">
+        <v>0.124</v>
+      </c>
+      <c r="AH80">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="AI80">
+        <v>0.61599999999999999</v>
+      </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>20</v>
       </c>
@@ -9117,12 +9778,104 @@
       <c r="C81" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="V81" s="2"/>
-      <c r="W81" s="2"/>
-      <c r="X81" s="2"/>
-      <c r="Y81" s="2"/>
+      <c r="D81">
+        <v>2049</v>
+      </c>
+      <c r="E81">
+        <v>2249</v>
+      </c>
+      <c r="F81">
+        <v>10</v>
+      </c>
+      <c r="G81">
+        <v>42</v>
+      </c>
+      <c r="H81">
+        <v>17</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="L81">
+        <v>0.1</v>
+      </c>
+      <c r="M81">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="N81">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="O81">
+        <v>0.1</v>
+      </c>
+      <c r="P81">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="Q81">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="R81">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="S81">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="T81">
+        <v>6009</v>
+      </c>
+      <c r="U81">
+        <v>6209</v>
+      </c>
+      <c r="V81" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W81" s="2">
+        <v>19928</v>
+      </c>
+      <c r="X81" s="2">
+        <v>37818</v>
+      </c>
+      <c r="Y81" s="2">
+        <v>17916</v>
+      </c>
+      <c r="Z81">
+        <v>0</v>
+      </c>
+      <c r="AA81">
+        <v>0.13</v>
+      </c>
+      <c r="AB81">
+        <v>9.08</v>
+      </c>
+      <c r="AC81">
+        <v>9.125</v>
+      </c>
+      <c r="AD81">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="AE81">
+        <v>9.0510000000000002</v>
+      </c>
+      <c r="AF81">
+        <v>9.0969999999999995</v>
+      </c>
+      <c r="AG81">
+        <v>0.129</v>
+      </c>
+      <c r="AH81">
+        <v>9.077</v>
+      </c>
+      <c r="AI81">
+        <v>9.1199999999999992</v>
+      </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>21</v>
       </c>
@@ -9132,8 +9885,104 @@
       <c r="C82" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D82">
+        <v>2087</v>
+      </c>
+      <c r="E82">
+        <v>2295</v>
+      </c>
+      <c r="F82">
+        <v>10</v>
+      </c>
+      <c r="G82">
+        <v>32</v>
+      </c>
+      <c r="H82">
+        <v>20</v>
+      </c>
+      <c r="I82">
+        <v>2</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="L82">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="M82">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="N82">
+        <v>0.157</v>
+      </c>
+      <c r="O82">
+        <v>0.125</v>
+      </c>
+      <c r="P82">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="Q82">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="R82">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="S82">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="T82">
+        <v>5459</v>
+      </c>
+      <c r="U82">
+        <v>5667</v>
+      </c>
+      <c r="V82">
+        <v>853</v>
+      </c>
+      <c r="W82">
+        <v>12856</v>
+      </c>
+      <c r="X82">
+        <v>24007</v>
+      </c>
+      <c r="Y82">
+        <v>11151</v>
+      </c>
+      <c r="Z82">
+        <v>0</v>
+      </c>
+      <c r="AA82">
+        <v>0.129</v>
+      </c>
+      <c r="AB82">
+        <v>3.86</v>
+      </c>
+      <c r="AC82">
+        <v>3.9039999999999999</v>
+      </c>
+      <c r="AD82">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AE82">
+        <v>3.907</v>
+      </c>
+      <c r="AF82">
+        <v>3.95</v>
+      </c>
+      <c r="AG82">
+        <v>0.13</v>
+      </c>
+      <c r="AH82">
+        <v>3.8319999999999999</v>
+      </c>
+      <c r="AI82">
+        <v>3.8759999999999999</v>
+      </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>22</v>
       </c>
@@ -9143,8 +9992,104 @@
       <c r="C83" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D83">
+        <v>2056</v>
+      </c>
+      <c r="E83">
+        <v>2254</v>
+      </c>
+      <c r="F83">
+        <v>10</v>
+      </c>
+      <c r="G83">
+        <v>56</v>
+      </c>
+      <c r="H83">
+        <v>18</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="L83">
+        <v>0.108</v>
+      </c>
+      <c r="M83">
+        <v>0.15</v>
+      </c>
+      <c r="N83">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="O83">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="P83">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="Q83">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="R83">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="S83">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="T83">
+        <v>6016</v>
+      </c>
+      <c r="U83">
+        <v>6214</v>
+      </c>
+      <c r="V83">
+        <v>1000</v>
+      </c>
+      <c r="W83">
+        <v>9861</v>
+      </c>
+      <c r="X83">
+        <v>17654</v>
+      </c>
+      <c r="Y83">
+        <v>7831</v>
+      </c>
+      <c r="Z83">
+        <v>0</v>
+      </c>
+      <c r="AA83">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AB83">
+        <v>4.1059999999999999</v>
+      </c>
+      <c r="AC83">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="AD83">
+        <v>0.13</v>
+      </c>
+      <c r="AE83">
+        <v>4.0860000000000003</v>
+      </c>
+      <c r="AF83">
+        <v>4.1289999999999996</v>
+      </c>
+      <c r="AG83">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="AH83">
+        <v>4.8070000000000004</v>
+      </c>
+      <c r="AI83">
+        <v>4.8540000000000001</v>
+      </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>30</v>
       </c>
@@ -9154,11 +10099,104 @@
       <c r="C84" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
+      <c r="D84" s="2">
+        <v>2744</v>
+      </c>
+      <c r="E84" s="2">
+        <v>3017</v>
+      </c>
+      <c r="F84" s="2">
+        <v>10</v>
+      </c>
+      <c r="G84">
+        <v>61</v>
+      </c>
+      <c r="H84">
+        <v>15</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="L84">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="M84">
+        <v>0.161</v>
+      </c>
+      <c r="N84">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="O84">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="P84">
+        <v>0.16</v>
+      </c>
+      <c r="Q84">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="R84">
+        <v>0.122</v>
+      </c>
+      <c r="S84">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="T84" s="2">
+        <v>6104</v>
+      </c>
+      <c r="U84" s="2">
+        <v>6977</v>
+      </c>
+      <c r="V84" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W84">
+        <v>32055</v>
+      </c>
+      <c r="X84">
+        <v>62039</v>
+      </c>
+      <c r="Y84">
+        <v>30025</v>
+      </c>
+      <c r="Z84">
+        <v>0</v>
+      </c>
+      <c r="AA84">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB84">
+        <v>13.327</v>
+      </c>
+      <c r="AC84">
+        <v>13.375999999999999</v>
+      </c>
+      <c r="AD84">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="AE84">
+        <v>13.291</v>
+      </c>
+      <c r="AF84">
+        <v>13.337999999999999</v>
+      </c>
+      <c r="AG84">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AH84">
+        <v>13.196999999999999</v>
+      </c>
+      <c r="AI84">
+        <v>13.244</v>
+      </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>31</v>
       </c>
@@ -9168,8 +10206,104 @@
       <c r="C85" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D85">
+        <v>2736</v>
+      </c>
+      <c r="E85">
+        <v>3008</v>
+      </c>
+      <c r="F85">
+        <v>10</v>
+      </c>
+      <c r="G85" s="2">
+        <v>54</v>
+      </c>
+      <c r="H85" s="2">
+        <v>16</v>
+      </c>
+      <c r="I85" s="2">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="L85">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="M85">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="N85">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="O85">
+        <v>0.124</v>
+      </c>
+      <c r="P85">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="Q85">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="R85">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="S85">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="T85">
+        <v>6696</v>
+      </c>
+      <c r="U85">
+        <v>6968</v>
+      </c>
+      <c r="V85">
+        <v>1000</v>
+      </c>
+      <c r="W85">
+        <v>218117</v>
+      </c>
+      <c r="X85">
+        <v>434169</v>
+      </c>
+      <c r="Y85">
+        <v>216091</v>
+      </c>
+      <c r="Z85">
+        <v>0</v>
+      </c>
+      <c r="AA85">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="AB85">
+        <v>80.658000000000001</v>
+      </c>
+      <c r="AC85">
+        <v>80.725999999999999</v>
+      </c>
+      <c r="AD85">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AE85">
+        <v>74.775999999999996</v>
+      </c>
+      <c r="AF85">
+        <v>74.819000000000003</v>
+      </c>
+      <c r="AG85">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="AH85">
+        <v>76.950999999999993</v>
+      </c>
+      <c r="AI85">
+        <v>76.995999999999995</v>
+      </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>32</v>
       </c>
@@ -9179,8 +10313,104 @@
       <c r="C86" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D86">
+        <v>2585</v>
+      </c>
+      <c r="E86">
+        <v>2842</v>
+      </c>
+      <c r="F86">
+        <v>10</v>
+      </c>
+      <c r="G86">
+        <v>46</v>
+      </c>
+      <c r="H86">
+        <v>17</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L86">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="M86">
+        <v>0.159</v>
+      </c>
+      <c r="N86">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="O86">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="P86">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="Q86">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="R86">
+        <v>0.124</v>
+      </c>
+      <c r="S86">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="T86">
+        <v>6545</v>
+      </c>
+      <c r="U86">
+        <v>6802</v>
+      </c>
+      <c r="V86">
+        <v>1000</v>
+      </c>
+      <c r="W86">
+        <v>405612</v>
+      </c>
+      <c r="X86">
+        <v>809174</v>
+      </c>
+      <c r="Y86">
+        <v>403591</v>
+      </c>
+      <c r="Z86">
+        <v>0</v>
+      </c>
+      <c r="AA86">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AB86">
+        <v>154.97</v>
+      </c>
+      <c r="AC86">
+        <v>155.01499999999999</v>
+      </c>
+      <c r="AD86">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="AE86">
+        <v>183.48699999999999</v>
+      </c>
+      <c r="AF86">
+        <v>183.55099999999999</v>
+      </c>
+      <c r="AG86">
+        <v>0.152</v>
+      </c>
+      <c r="AH86">
+        <v>151.53700000000001</v>
+      </c>
+      <c r="AI86">
+        <v>151.58600000000001</v>
+      </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>40</v>
       </c>
@@ -9190,8 +10420,104 @@
       <c r="C87" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D87">
+        <v>3313</v>
+      </c>
+      <c r="E87">
+        <v>3639</v>
+      </c>
+      <c r="F87">
+        <v>10</v>
+      </c>
+      <c r="G87">
+        <v>74</v>
+      </c>
+      <c r="H87">
+        <v>19</v>
+      </c>
+      <c r="I87">
+        <v>3</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="L87">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="M87">
+        <v>0.186</v>
+      </c>
+      <c r="N87">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="O87">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="P87">
+        <v>0.19</v>
+      </c>
+      <c r="Q87">
+        <v>0.182</v>
+      </c>
+      <c r="R87">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="S87">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="T87">
+        <v>7273</v>
+      </c>
+      <c r="U87">
+        <v>7599</v>
+      </c>
+      <c r="V87">
+        <v>1000</v>
+      </c>
+      <c r="W87">
+        <v>550945</v>
+      </c>
+      <c r="X87">
+        <v>1099800</v>
+      </c>
+      <c r="Y87">
+        <v>548911</v>
+      </c>
+      <c r="Z87">
+        <v>0</v>
+      </c>
+      <c r="AA87">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="AB87">
+        <v>244.131</v>
+      </c>
+      <c r="AC87">
+        <v>244.197</v>
+      </c>
+      <c r="AD87">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AE87">
+        <v>250.42400000000001</v>
+      </c>
+      <c r="AF87">
+        <v>250.47800000000001</v>
+      </c>
+      <c r="AG87">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="AH87">
+        <v>259.51600000000002</v>
+      </c>
+      <c r="AI87">
+        <v>259.58</v>
+      </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>41</v>
       </c>
@@ -9201,11 +10527,104 @@
       <c r="C88" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T88" s="2"/>
-      <c r="U88" s="2"/>
-      <c r="V88" s="2"/>
+      <c r="D88">
+        <v>3260</v>
+      </c>
+      <c r="E88">
+        <v>3585</v>
+      </c>
+      <c r="F88">
+        <v>10</v>
+      </c>
+      <c r="G88">
+        <v>60</v>
+      </c>
+      <c r="H88">
+        <v>18</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>0.15</v>
+      </c>
+      <c r="L88">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="M88">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="N88">
+        <v>0.159</v>
+      </c>
+      <c r="O88">
+        <v>0.159</v>
+      </c>
+      <c r="P88">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="Q88">
+        <v>0.15</v>
+      </c>
+      <c r="R88">
+        <v>0.15</v>
+      </c>
+      <c r="S88">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="T88" s="2">
+        <v>7220</v>
+      </c>
+      <c r="U88" s="2">
+        <v>7545</v>
+      </c>
+      <c r="V88" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W88">
+        <v>249049</v>
+      </c>
+      <c r="X88">
+        <v>496026</v>
+      </c>
+      <c r="Y88">
+        <v>247022</v>
+      </c>
+      <c r="Z88">
+        <v>0</v>
+      </c>
+      <c r="AA88">
+        <v>0.217</v>
+      </c>
+      <c r="AB88">
+        <v>86.528999999999996</v>
+      </c>
+      <c r="AC88">
+        <v>86.597999999999999</v>
+      </c>
+      <c r="AD88">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="AE88">
+        <v>103.95</v>
+      </c>
+      <c r="AF88">
+        <v>104.033</v>
+      </c>
+      <c r="AG88">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AH88">
+        <v>97.766999999999996</v>
+      </c>
+      <c r="AI88">
+        <v>97.828999999999994</v>
+      </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>42</v>
       </c>
@@ -9215,15 +10634,1682 @@
       <c r="C89" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T89" s="2"/>
-      <c r="U89" s="2"/>
-      <c r="V89" s="2"/>
-      <c r="AA89" s="2"/>
-      <c r="AB89" s="2"/>
-      <c r="AC89" s="2"/>
+      <c r="D89">
+        <v>3230</v>
+      </c>
+      <c r="E89">
+        <v>3549</v>
+      </c>
+      <c r="F89">
+        <v>10</v>
+      </c>
+      <c r="G89">
+        <v>69</v>
+      </c>
+      <c r="H89">
+        <v>34</v>
+      </c>
+      <c r="I89">
+        <v>10</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="L89">
+        <v>0.157</v>
+      </c>
+      <c r="M89">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="N89">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="O89">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="P89">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="Q89">
+        <v>0.152</v>
+      </c>
+      <c r="R89">
+        <v>0.155</v>
+      </c>
+      <c r="S89">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="T89" s="2">
+        <v>7190</v>
+      </c>
+      <c r="U89" s="2">
+        <v>7509</v>
+      </c>
+      <c r="V89" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W89">
+        <v>35975</v>
+      </c>
+      <c r="X89">
+        <v>69868</v>
+      </c>
+      <c r="Y89">
+        <v>33938</v>
+      </c>
+      <c r="Z89">
+        <v>0</v>
+      </c>
+      <c r="AA89" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="AB89" s="2">
+        <v>13.507</v>
+      </c>
+      <c r="AC89" s="2">
+        <v>13.579000000000001</v>
+      </c>
+      <c r="AD89">
+        <v>0.151</v>
+      </c>
+      <c r="AE89">
+        <v>13.396000000000001</v>
+      </c>
+      <c r="AF89">
+        <v>13.446999999999999</v>
+      </c>
+      <c r="AG89">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="AH89">
+        <v>13.598000000000001</v>
+      </c>
+      <c r="AI89">
+        <v>13.647</v>
+      </c>
+    </row>
+    <row r="93" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="94" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L94" s="7"/>
+      <c r="M94" s="7"/>
+      <c r="N94" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O94" s="7"/>
+      <c r="P94" s="7"/>
+      <c r="Q94" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R94" s="7"/>
+      <c r="S94" s="7"/>
+      <c r="T94" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="U94" s="7"/>
+      <c r="V94" s="7"/>
+      <c r="W94" s="7"/>
+      <c r="X94" s="7"/>
+      <c r="Y94" s="7"/>
+      <c r="Z94" s="7"/>
+      <c r="AA94" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB94" s="7"/>
+      <c r="AC94" s="7"/>
+      <c r="AD94" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE94" s="7"/>
+      <c r="AF94" s="7"/>
+      <c r="AG94" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH94" s="7"/>
+      <c r="AI94" s="7"/>
+    </row>
+    <row r="95" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95" t="s">
+        <v>28</v>
+      </c>
+      <c r="F95" t="s">
+        <v>29</v>
+      </c>
+      <c r="G95" t="s">
+        <v>30</v>
+      </c>
+      <c r="H95" t="s">
+        <v>36</v>
+      </c>
+      <c r="I95" t="s">
+        <v>31</v>
+      </c>
+      <c r="J95" t="s">
+        <v>32</v>
+      </c>
+      <c r="K95" t="s">
+        <v>17</v>
+      </c>
+      <c r="L95" t="s">
+        <v>18</v>
+      </c>
+      <c r="M95" t="s">
+        <v>19</v>
+      </c>
+      <c r="N95" t="s">
+        <v>20</v>
+      </c>
+      <c r="O95" t="s">
+        <v>21</v>
+      </c>
+      <c r="P95" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>23</v>
+      </c>
+      <c r="R95" t="s">
+        <v>24</v>
+      </c>
+      <c r="S95" t="s">
+        <v>25</v>
+      </c>
+      <c r="T95" t="s">
+        <v>37</v>
+      </c>
+      <c r="U95" t="s">
+        <v>38</v>
+      </c>
+      <c r="V95" t="s">
+        <v>39</v>
+      </c>
+      <c r="W95" t="s">
+        <v>40</v>
+      </c>
+      <c r="X95" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y95" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z95" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA95" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB95" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC95" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD95" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE95" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF95" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG95" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH95" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI95" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="96" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>19</v>
+      </c>
+      <c r="D96">
+        <v>665</v>
+      </c>
+      <c r="E96">
+        <v>723</v>
+      </c>
+      <c r="F96">
+        <v>10</v>
+      </c>
+      <c r="G96">
+        <v>32</v>
+      </c>
+      <c r="H96">
+        <v>21</v>
+      </c>
+      <c r="I96">
+        <v>3</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="L96">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="M96">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="N96">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="O96">
+        <v>6.2E-2</v>
+      </c>
+      <c r="P96">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="Q96">
+        <v>0.114</v>
+      </c>
+      <c r="R96">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="S96">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="T96">
+        <v>2641</v>
+      </c>
+      <c r="U96">
+        <v>2699</v>
+      </c>
+      <c r="V96">
+        <v>504</v>
+      </c>
+      <c r="W96">
+        <v>2534</v>
+      </c>
+      <c r="X96">
+        <v>4061</v>
+      </c>
+      <c r="Y96">
+        <v>1527</v>
+      </c>
+      <c r="Z96">
+        <v>0</v>
+      </c>
+      <c r="AA96">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="AB96">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="AC96">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="AD96">
+        <v>0.113</v>
+      </c>
+      <c r="AE96">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AF96">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="AG96">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AH96">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="AI96">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="97" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>1</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>24</v>
+      </c>
+      <c r="D97">
+        <v>742</v>
+      </c>
+      <c r="E97">
+        <v>811</v>
+      </c>
+      <c r="F97">
+        <v>10</v>
+      </c>
+      <c r="G97">
+        <v>33</v>
+      </c>
+      <c r="H97">
+        <v>20</v>
+      </c>
+      <c r="I97">
+        <v>2</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0.123</v>
+      </c>
+      <c r="L97">
+        <v>6.2E-2</v>
+      </c>
+      <c r="M97">
+        <v>0.1</v>
+      </c>
+      <c r="N97">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="O97">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="P97">
+        <v>9.4E-2</v>
+      </c>
+      <c r="Q97">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="R97">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="S97">
+        <v>0.106</v>
+      </c>
+      <c r="T97">
+        <v>2310</v>
+      </c>
+      <c r="U97">
+        <v>2379</v>
+      </c>
+      <c r="V97">
+        <v>402</v>
+      </c>
+      <c r="W97">
+        <v>6377</v>
+      </c>
+      <c r="X97">
+        <v>11951</v>
+      </c>
+      <c r="Y97">
+        <v>5574</v>
+      </c>
+      <c r="Z97">
+        <v>0</v>
+      </c>
+      <c r="AA97">
+        <v>0.188</v>
+      </c>
+      <c r="AB97">
+        <v>1.375</v>
+      </c>
+      <c r="AC97">
+        <v>1.429</v>
+      </c>
+      <c r="AD97">
+        <v>0.114</v>
+      </c>
+      <c r="AE97">
+        <v>1.254</v>
+      </c>
+      <c r="AF97">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="AG97">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="AH97">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="AI97">
+        <v>1.2649999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98">
+        <v>9</v>
+      </c>
+      <c r="D98">
+        <v>2310</v>
+      </c>
+      <c r="E98">
+        <v>2379</v>
+      </c>
+      <c r="F98">
+        <v>402</v>
+      </c>
+      <c r="G98">
+        <v>6377</v>
+      </c>
+      <c r="H98">
+        <v>11951</v>
+      </c>
+      <c r="I98">
+        <v>5574</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="L98">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="M98">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="N98">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="O98">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="P98">
+        <v>9.4E-2</v>
+      </c>
+      <c r="Q98">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="R98">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="S98">
+        <v>0.1</v>
+      </c>
+      <c r="T98">
+        <v>934</v>
+      </c>
+      <c r="U98">
+        <v>1001</v>
+      </c>
+      <c r="V98">
+        <v>60</v>
+      </c>
+      <c r="W98">
+        <v>131</v>
+      </c>
+      <c r="X98">
+        <v>143</v>
+      </c>
+      <c r="Y98">
+        <v>12</v>
+      </c>
+      <c r="Z98">
+        <v>0</v>
+      </c>
+      <c r="AA98">
+        <v>0.152</v>
+      </c>
+      <c r="AB98">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AC98">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="AD98">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AE98">
+        <v>0.109</v>
+      </c>
+      <c r="AF98">
+        <v>0.15</v>
+      </c>
+      <c r="AG98">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AH98">
+        <v>0.108</v>
+      </c>
+      <c r="AI98">
+        <v>0.14799999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>10</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99">
+        <v>1309</v>
+      </c>
+      <c r="E99">
+        <v>1434</v>
+      </c>
+      <c r="F99">
+        <v>10</v>
+      </c>
+      <c r="G99">
+        <v>30</v>
+      </c>
+      <c r="H99">
+        <v>16</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0.123</v>
+      </c>
+      <c r="L99">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="M99">
+        <v>0.112</v>
+      </c>
+      <c r="N99">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="O99">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="P99">
+        <v>0.124</v>
+      </c>
+      <c r="Q99">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="R99">
+        <v>7.8E-2</v>
+      </c>
+      <c r="S99">
+        <v>0.125</v>
+      </c>
+      <c r="T99">
+        <v>1977</v>
+      </c>
+      <c r="U99">
+        <v>2102</v>
+      </c>
+      <c r="V99">
+        <v>177</v>
+      </c>
+      <c r="W99">
+        <v>995</v>
+      </c>
+      <c r="X99">
+        <v>1637</v>
+      </c>
+      <c r="Y99">
+        <v>642</v>
+      </c>
+      <c r="Z99">
+        <v>0</v>
+      </c>
+      <c r="AA99">
+        <v>0.186</v>
+      </c>
+      <c r="AB99">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="AC99">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="AD99">
+        <v>0.123</v>
+      </c>
+      <c r="AE99">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="AF99">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="AG99">
+        <v>0.18</v>
+      </c>
+      <c r="AH99">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="AI99">
+        <v>0.48099999999999998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>11</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" s="2">
+        <v>1239</v>
+      </c>
+      <c r="E100" s="2">
+        <v>1362</v>
+      </c>
+      <c r="F100" s="2">
+        <v>10</v>
+      </c>
+      <c r="G100">
+        <v>39</v>
+      </c>
+      <c r="H100">
+        <v>24</v>
+      </c>
+      <c r="I100">
+        <v>4</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0.121</v>
+      </c>
+      <c r="L100">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="M100">
+        <v>0.111</v>
+      </c>
+      <c r="N100">
+        <v>0.125</v>
+      </c>
+      <c r="O100">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="P100">
+        <v>0.12</v>
+      </c>
+      <c r="Q100">
+        <v>0.125</v>
+      </c>
+      <c r="R100">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="S100">
+        <v>0.111</v>
+      </c>
+      <c r="T100">
+        <v>3475</v>
+      </c>
+      <c r="U100">
+        <v>3598</v>
+      </c>
+      <c r="V100">
+        <v>569</v>
+      </c>
+      <c r="W100" s="2">
+        <v>10148</v>
+      </c>
+      <c r="X100" s="2">
+        <v>19159</v>
+      </c>
+      <c r="Y100" s="2">
+        <v>9011</v>
+      </c>
+      <c r="Z100">
+        <v>0</v>
+      </c>
+      <c r="AA100">
+        <v>0.125</v>
+      </c>
+      <c r="AB100">
+        <v>2.4449999999999998</v>
+      </c>
+      <c r="AC100">
+        <v>2.4860000000000002</v>
+      </c>
+      <c r="AD100">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AE100">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="AF100">
+        <v>2.5350000000000001</v>
+      </c>
+      <c r="AG100">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AH100">
+        <v>2.4529999999999998</v>
+      </c>
+      <c r="AI100">
+        <v>2.4980000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>12</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101">
+        <v>1326</v>
+      </c>
+      <c r="E101">
+        <v>1458</v>
+      </c>
+      <c r="F101">
+        <v>10</v>
+      </c>
+      <c r="G101">
+        <v>31</v>
+      </c>
+      <c r="H101">
+        <v>15</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
+        <v>0.124</v>
+      </c>
+      <c r="L101">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M101">
+        <v>0.11</v>
+      </c>
+      <c r="N101">
+        <v>0.124</v>
+      </c>
+      <c r="O101">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="P101">
+        <v>0.115</v>
+      </c>
+      <c r="Q101">
+        <v>0.125</v>
+      </c>
+      <c r="R101">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="S101">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="T101">
+        <v>2662</v>
+      </c>
+      <c r="U101">
+        <v>2794</v>
+      </c>
+      <c r="V101">
+        <v>344</v>
+      </c>
+      <c r="W101">
+        <v>1293</v>
+      </c>
+      <c r="X101">
+        <v>1899</v>
+      </c>
+      <c r="Y101">
+        <v>606</v>
+      </c>
+      <c r="Z101">
+        <v>0</v>
+      </c>
+      <c r="AA101">
+        <v>0.121</v>
+      </c>
+      <c r="AB101">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="AC101">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="AD101">
+        <v>0.122</v>
+      </c>
+      <c r="AE101">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="AF101">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="AG101">
+        <v>0.124</v>
+      </c>
+      <c r="AH101">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="AI101">
+        <v>0.61599999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>20</v>
+      </c>
+      <c r="B102">
+        <v>3</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102">
+        <v>2049</v>
+      </c>
+      <c r="E102">
+        <v>2249</v>
+      </c>
+      <c r="F102">
+        <v>10</v>
+      </c>
+      <c r="G102">
+        <v>42</v>
+      </c>
+      <c r="H102">
+        <v>17</v>
+      </c>
+      <c r="I102">
+        <v>1</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+      <c r="K102">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="L102">
+        <v>0.1</v>
+      </c>
+      <c r="M102">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="N102">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="O102">
+        <v>0.1</v>
+      </c>
+      <c r="P102">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="Q102">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="R102">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="S102">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="T102">
+        <v>6009</v>
+      </c>
+      <c r="U102">
+        <v>6209</v>
+      </c>
+      <c r="V102" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W102" s="2">
+        <v>19928</v>
+      </c>
+      <c r="X102" s="2">
+        <v>37818</v>
+      </c>
+      <c r="Y102" s="2">
+        <v>17916</v>
+      </c>
+      <c r="Z102">
+        <v>0</v>
+      </c>
+      <c r="AA102">
+        <v>0.13</v>
+      </c>
+      <c r="AB102">
+        <v>9.08</v>
+      </c>
+      <c r="AC102">
+        <v>9.125</v>
+      </c>
+      <c r="AD102">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="AE102">
+        <v>9.0510000000000002</v>
+      </c>
+      <c r="AF102">
+        <v>9.0969999999999995</v>
+      </c>
+      <c r="AG102">
+        <v>0.129</v>
+      </c>
+      <c r="AH102">
+        <v>9.077</v>
+      </c>
+      <c r="AI102">
+        <v>9.1199999999999992</v>
+      </c>
+    </row>
+    <row r="103" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>21</v>
+      </c>
+      <c r="B103">
+        <v>3</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103">
+        <v>2087</v>
+      </c>
+      <c r="E103">
+        <v>2295</v>
+      </c>
+      <c r="F103">
+        <v>10</v>
+      </c>
+      <c r="G103">
+        <v>32</v>
+      </c>
+      <c r="H103">
+        <v>20</v>
+      </c>
+      <c r="I103">
+        <v>2</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="L103">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="M103">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="N103">
+        <v>0.157</v>
+      </c>
+      <c r="O103">
+        <v>0.125</v>
+      </c>
+      <c r="P103">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="Q103">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="R103">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="S103">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="T103">
+        <v>5459</v>
+      </c>
+      <c r="U103">
+        <v>5667</v>
+      </c>
+      <c r="V103">
+        <v>853</v>
+      </c>
+      <c r="W103">
+        <v>12856</v>
+      </c>
+      <c r="X103">
+        <v>24007</v>
+      </c>
+      <c r="Y103">
+        <v>11151</v>
+      </c>
+      <c r="Z103">
+        <v>0</v>
+      </c>
+      <c r="AA103">
+        <v>0.129</v>
+      </c>
+      <c r="AB103">
+        <v>3.86</v>
+      </c>
+      <c r="AC103">
+        <v>3.9039999999999999</v>
+      </c>
+      <c r="AD103">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AE103">
+        <v>3.907</v>
+      </c>
+      <c r="AF103">
+        <v>3.95</v>
+      </c>
+      <c r="AG103">
+        <v>0.13</v>
+      </c>
+      <c r="AH103">
+        <v>3.8319999999999999</v>
+      </c>
+      <c r="AI103">
+        <v>3.8759999999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>22</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104">
+        <v>2056</v>
+      </c>
+      <c r="E104">
+        <v>2254</v>
+      </c>
+      <c r="F104">
+        <v>10</v>
+      </c>
+      <c r="G104">
+        <v>56</v>
+      </c>
+      <c r="H104">
+        <v>18</v>
+      </c>
+      <c r="I104">
+        <v>1</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+      <c r="K104">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="L104">
+        <v>0.108</v>
+      </c>
+      <c r="M104">
+        <v>0.15</v>
+      </c>
+      <c r="N104">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="O104">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="P104">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="Q104">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="R104">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="S104">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="T104">
+        <v>6016</v>
+      </c>
+      <c r="U104">
+        <v>6214</v>
+      </c>
+      <c r="V104">
+        <v>1000</v>
+      </c>
+      <c r="W104">
+        <v>9861</v>
+      </c>
+      <c r="X104">
+        <v>17654</v>
+      </c>
+      <c r="Y104">
+        <v>7831</v>
+      </c>
+      <c r="Z104">
+        <v>0</v>
+      </c>
+      <c r="AA104">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AB104">
+        <v>4.1059999999999999</v>
+      </c>
+      <c r="AC104">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="AD104">
+        <v>0.13</v>
+      </c>
+      <c r="AE104">
+        <v>4.0860000000000003</v>
+      </c>
+      <c r="AF104">
+        <v>4.1289999999999996</v>
+      </c>
+      <c r="AG104">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="AH104">
+        <v>4.8070000000000004</v>
+      </c>
+      <c r="AI104">
+        <v>4.8540000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>30</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" s="2">
+        <v>2744</v>
+      </c>
+      <c r="E105" s="2">
+        <v>3017</v>
+      </c>
+      <c r="F105" s="2">
+        <v>10</v>
+      </c>
+      <c r="G105">
+        <v>61</v>
+      </c>
+      <c r="H105">
+        <v>15</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+      <c r="K105">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="L105">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="M105">
+        <v>0.161</v>
+      </c>
+      <c r="N105">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="O105">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="P105">
+        <v>0.16</v>
+      </c>
+      <c r="Q105">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="R105">
+        <v>0.122</v>
+      </c>
+      <c r="S105">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="T105" s="2">
+        <v>6104</v>
+      </c>
+      <c r="U105" s="2">
+        <v>6977</v>
+      </c>
+      <c r="V105" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W105">
+        <v>32055</v>
+      </c>
+      <c r="X105">
+        <v>62039</v>
+      </c>
+      <c r="Y105">
+        <v>30025</v>
+      </c>
+      <c r="Z105">
+        <v>0</v>
+      </c>
+      <c r="AA105">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB105">
+        <v>13.327</v>
+      </c>
+      <c r="AC105">
+        <v>13.375999999999999</v>
+      </c>
+      <c r="AD105">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="AE105">
+        <v>13.291</v>
+      </c>
+      <c r="AF105">
+        <v>13.337999999999999</v>
+      </c>
+      <c r="AG105">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AH105">
+        <v>13.196999999999999</v>
+      </c>
+      <c r="AI105">
+        <v>13.244</v>
+      </c>
+    </row>
+    <row r="106" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>31</v>
+      </c>
+      <c r="B106">
+        <v>4</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106">
+        <v>2736</v>
+      </c>
+      <c r="E106">
+        <v>3008</v>
+      </c>
+      <c r="F106">
+        <v>10</v>
+      </c>
+      <c r="G106" s="2">
+        <v>54</v>
+      </c>
+      <c r="H106" s="2">
+        <v>16</v>
+      </c>
+      <c r="I106" s="2">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+      <c r="K106">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="L106">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="M106">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="N106">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="O106">
+        <v>0.124</v>
+      </c>
+      <c r="P106">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="Q106">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="R106">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="S106">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="T106">
+        <v>6696</v>
+      </c>
+      <c r="U106">
+        <v>6968</v>
+      </c>
+      <c r="V106">
+        <v>1000</v>
+      </c>
+      <c r="W106">
+        <v>218117</v>
+      </c>
+      <c r="X106">
+        <v>434169</v>
+      </c>
+      <c r="Y106">
+        <v>216091</v>
+      </c>
+      <c r="Z106">
+        <v>0</v>
+      </c>
+      <c r="AA106">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="AB106">
+        <v>80.658000000000001</v>
+      </c>
+      <c r="AC106">
+        <v>80.725999999999999</v>
+      </c>
+      <c r="AD106">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AE106">
+        <v>74.775999999999996</v>
+      </c>
+      <c r="AF106">
+        <v>74.819000000000003</v>
+      </c>
+      <c r="AG106">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="AH106">
+        <v>76.950999999999993</v>
+      </c>
+      <c r="AI106">
+        <v>76.995999999999995</v>
+      </c>
+    </row>
+    <row r="107" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>32</v>
+      </c>
+      <c r="B107">
+        <v>4</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D107">
+        <v>2585</v>
+      </c>
+      <c r="E107">
+        <v>2842</v>
+      </c>
+      <c r="F107">
+        <v>10</v>
+      </c>
+      <c r="G107">
+        <v>46</v>
+      </c>
+      <c r="H107">
+        <v>17</v>
+      </c>
+      <c r="I107">
+        <v>1</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+      <c r="K107">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L107">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="M107">
+        <v>0.159</v>
+      </c>
+      <c r="N107">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="O107">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="P107">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="Q107">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="R107">
+        <v>0.124</v>
+      </c>
+      <c r="S107">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="T107">
+        <v>6545</v>
+      </c>
+      <c r="U107">
+        <v>6802</v>
+      </c>
+      <c r="V107">
+        <v>1000</v>
+      </c>
+      <c r="W107">
+        <v>405612</v>
+      </c>
+      <c r="X107">
+        <v>809174</v>
+      </c>
+      <c r="Y107">
+        <v>403591</v>
+      </c>
+      <c r="Z107">
+        <v>0</v>
+      </c>
+      <c r="AA107">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AB107">
+        <v>154.97</v>
+      </c>
+      <c r="AC107">
+        <v>155.01499999999999</v>
+      </c>
+      <c r="AD107">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="AE107">
+        <v>183.48699999999999</v>
+      </c>
+      <c r="AF107">
+        <v>183.55099999999999</v>
+      </c>
+      <c r="AG107">
+        <v>0.152</v>
+      </c>
+      <c r="AH107">
+        <v>151.53700000000001</v>
+      </c>
+      <c r="AI107">
+        <v>151.58600000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>40</v>
+      </c>
+      <c r="B108">
+        <v>5</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108">
+        <v>3313</v>
+      </c>
+      <c r="E108">
+        <v>3639</v>
+      </c>
+      <c r="F108">
+        <v>10</v>
+      </c>
+      <c r="G108">
+        <v>74</v>
+      </c>
+      <c r="H108">
+        <v>19</v>
+      </c>
+      <c r="I108">
+        <v>3</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="L108">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="M108">
+        <v>0.186</v>
+      </c>
+      <c r="N108">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="O108">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="P108">
+        <v>0.19</v>
+      </c>
+      <c r="Q108">
+        <v>0.182</v>
+      </c>
+      <c r="R108">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="S108">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="T108">
+        <v>7273</v>
+      </c>
+      <c r="U108">
+        <v>7599</v>
+      </c>
+      <c r="V108">
+        <v>1000</v>
+      </c>
+      <c r="W108">
+        <v>550945</v>
+      </c>
+      <c r="X108">
+        <v>1099800</v>
+      </c>
+      <c r="Y108">
+        <v>548911</v>
+      </c>
+      <c r="Z108">
+        <v>0</v>
+      </c>
+      <c r="AA108">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="AB108">
+        <v>244.131</v>
+      </c>
+      <c r="AC108">
+        <v>244.197</v>
+      </c>
+    </row>
+    <row r="109" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>41</v>
+      </c>
+      <c r="B109">
+        <v>5</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T109" s="2"/>
+      <c r="U109" s="2"/>
+      <c r="V109" s="2"/>
+    </row>
+    <row r="110" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>42</v>
+      </c>
+      <c r="B110">
+        <v>5</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T110" s="2"/>
+      <c r="U110" s="2"/>
+      <c r="V110" s="2"/>
+      <c r="AA110" s="2"/>
+      <c r="AB110" s="2"/>
+      <c r="AC110" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="40">
+    <mergeCell ref="AA94:AC94"/>
+    <mergeCell ref="AD94:AF94"/>
+    <mergeCell ref="AG94:AI94"/>
+    <mergeCell ref="D94:J94"/>
+    <mergeCell ref="K94:M94"/>
+    <mergeCell ref="N94:P94"/>
+    <mergeCell ref="Q94:S94"/>
+    <mergeCell ref="T94:Z94"/>
     <mergeCell ref="AD10:AF10"/>
     <mergeCell ref="AG10:AI10"/>
     <mergeCell ref="T10:Z10"/>
@@ -9259,11 +12345,12 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating tests summary for Heuristic 1 + 80.
</commit_message>
<xml_diff>
--- a/docs/testsFSG/tests-summary.xlsx
+++ b/docs/testsFSG/tests-summary.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="86">
   <si>
     <t>Run</t>
   </si>
@@ -291,7 +291,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -362,72 +362,69 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -918,11 +915,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="248623888"/>
-        <c:axId val="248622320"/>
+        <c:axId val="310206632"/>
+        <c:axId val="310259848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="248623888"/>
+        <c:axId val="310206632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,7 +962,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248622320"/>
+        <c:crossAx val="310259848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -973,7 +970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="248622320"/>
+        <c:axId val="310259848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1024,7 +1021,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248623888"/>
+        <c:crossAx val="310206632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1570,11 +1567,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="247358848"/>
-        <c:axId val="247360024"/>
+        <c:axId val="312050712"/>
+        <c:axId val="311439192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="247358848"/>
+        <c:axId val="312050712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1614,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247360024"/>
+        <c:crossAx val="311439192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1625,7 +1622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="247360024"/>
+        <c:axId val="311439192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1676,7 +1673,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247358848"/>
+        <c:crossAx val="312050712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1965,6 +1962,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.11439175202788675</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14781688745976435</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24908093144028493</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26994033745986379</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30074901114503988</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2092,67 +2104,6 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Summary!$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Heuristic 4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Summary!$A$21:$A$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Summary!$G$21:$G$25</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2162,11 +2113,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="249265040"/>
-        <c:axId val="249265824"/>
+        <c:axId val="468572608"/>
+        <c:axId val="468578096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="249265040"/>
+        <c:axId val="468572608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2209,7 +2160,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249265824"/>
+        <c:crossAx val="468578096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2217,7 +2168,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="249265824"/>
+        <c:axId val="468578096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,7 +2219,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249265040"/>
+        <c:crossAx val="468572608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2557,6 +2508,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.56580424271293084</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.128869116490275</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.410604615631556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.871834631856656</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5724833041754245</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2684,67 +2650,6 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Summary!$G$29</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Heuristic 4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Summary!$A$30:$A$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Summary!$G$30:$G$34</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2754,11 +2659,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="248625064"/>
-        <c:axId val="247355320"/>
+        <c:axId val="387462000"/>
+        <c:axId val="387461216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="248625064"/>
+        <c:axId val="387462000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2801,7 +2706,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247355320"/>
+        <c:crossAx val="387461216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2809,7 +2714,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="247355320"/>
+        <c:axId val="387461216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2860,7 +2765,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248625064"/>
+        <c:crossAx val="387462000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5230,19 +5135,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>601133</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>4234</xdr:rowOff>
+      <xdr:colOff>601132</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>296333</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>296332</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5260,19 +5165,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>4233</xdr:rowOff>
+      <xdr:colOff>448733</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>139699</xdr:rowOff>
+      <xdr:colOff>143933</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>135467</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5300,9 +5205,9 @@
     </tableColumn>
     <tableColumn id="2" name="Default" dataDxfId="17"/>
     <tableColumn id="3" name="Heuristic 1" dataDxfId="16"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="13"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="12"/>
-    <tableColumn id="7" name="Heuristic 4" dataDxfId="10"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="15"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="14"/>
+    <tableColumn id="7" name="Heuristic 4" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5358,7 +5263,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="0" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -5536,38 +5441,37 @@
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'40 - Models'!$B$2*'40 - Models'!$B$6*Table5[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table5[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="18"/>
+    <tableColumn id="2" name="Default" dataDxfId="12"/>
     <tableColumn id="3" name="Heuristic 1"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="15"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="14"/>
-    <tableColumn id="7" name="Heuristic 4" dataDxfId="11"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="11"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="10"/>
+    <tableColumn id="7" name="Heuristic 4" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table414" displayName="Table414" ref="A20:G25" totalsRowShown="0">
-  <autoFilter ref="A20:G25"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table414" displayName="Table414" ref="A20:F25" totalsRowShown="0">
+  <autoFilter ref="A20:F25"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Models"/>
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'80 - Models'!$B$2*'80 - Models'!$B$6*Table414[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table414[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="9"/>
-    <tableColumn id="3" name="Heuristic 1" dataDxfId="8"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="7"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="6"/>
-    <tableColumn id="7" name="Heuristic 4" dataDxfId="5"/>
+    <tableColumn id="2" name="Default" dataDxfId="8"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="7"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="6"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table41415" displayName="Table41415" ref="A29:G34" totalsRowShown="0">
-  <autoFilter ref="A29:G34"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table41415" displayName="Table41415" ref="A29:F34" totalsRowShown="0">
+  <autoFilter ref="A29:F34"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Models"/>
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'80 - Models'!$B$2*'80 - Models'!$B$6*Table41415[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table41415[[#This Row],[Models]]</calculatedColumnFormula>
@@ -5576,7 +5480,6 @@
     <tableColumn id="3" name="Heuristic 1" dataDxfId="3"/>
     <tableColumn id="4" name="Heuristic 2" dataDxfId="2"/>
     <tableColumn id="5" name="Heuristic 3" dataDxfId="1"/>
-    <tableColumn id="7" name="Heuristic 4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6067,8 +5970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6109,23 +6012,23 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table5[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table5[[#This Row],[Models]]</f>
         <v>6</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <f>HARMEAN('40 - Models'!L12:L14,'40 - Models'!O12:O14,'40 - Models'!R12:R14)</f>
         <v>9.1187269729718287E-2</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <f>HARMEAN('40 - Models'!L33:L35,'40 - Models'!O33:O35,'40 - Models'!R33:R35)</f>
         <v>6.5905807503954361E-2</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <f>HARMEAN('40 - Models'!L54:L56,'40 - Models'!O54:O56,'40 - Models'!R54:R56)</f>
         <v>7.837459345418106E-2</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <f>HARMEAN('40 - Models'!L75:L77,'40 - Models'!O75:O77,'40 - Models'!R75:R77)</f>
         <v>6.5412518447039589E-2</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <f>HARMEAN('40 - Models'!L96:L98,'40 - Models'!O96:O98,'40 - Models'!R96:R98)</f>
         <v>6.6179246981599299E-2</v>
       </c>
@@ -6138,23 +6041,23 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table5[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table5[[#This Row],[Models]]</f>
         <v>12</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <f>HARMEAN('40 - Models'!L15:L17,'40 - Models'!O15:O17,'40 - Models'!R15:R17)</f>
         <v>0.11180847459261625</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <f>HARMEAN('40 - Models'!L36:L38,'40 - Models'!O36:O38,'40 - Models'!R36:R38)</f>
         <v>8.5653949321746303E-2</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <f>HARMEAN('40 - Models'!L57:L59,'40 - Models'!O57:O59,'40 - Models'!R57:R59)</f>
         <v>7.973155770843153E-2</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <f>HARMEAN('40 - Models'!L78:L80,'40 - Models'!O78:O80,'40 - Models'!R78:R80)</f>
         <v>7.472896132803894E-2</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <f>HARMEAN('40 - Models'!L99:L101,'40 - Models'!O99:O101,'40 - Models'!R99:R101)</f>
         <v>9.5173665888558606E-2</v>
       </c>
@@ -6167,23 +6070,23 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table5[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table5[[#This Row],[Models]]</f>
         <v>18</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <f>HARMEAN('40 - Models'!L18:L20,'40 - Models'!O18:O20,'40 - Models'!R18:R20)</f>
         <v>0.17014395193802512</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <f>HARMEAN('40 - Models'!L39:L41,'40 - Models'!O39:O41,'40 - Models'!R39:R41)</f>
         <v>0.10691845154486945</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <f>HARMEAN('40 - Models'!L60:L62,'40 - Models'!O60:O62,'40 - Models'!R60:R62)</f>
         <v>0.11130381037109011</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <f>HARMEAN('40 - Models'!L81:L83,'40 - Models'!O81:O83,'40 - Models'!R81:R83)</f>
         <v>0.10156336722046637</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <f>HARMEAN('40 - Models'!L102:L104,'40 - Models'!O102:O104,'40 - Models'!R102:R104)</f>
         <v>0.11448383890884309</v>
       </c>
@@ -6196,23 +6099,23 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table5[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table5[[#This Row],[Models]]</f>
         <v>24</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <f>HARMEAN('40 - Models'!L21:L23,'40 - Models'!O21:O23,'40 - Models'!R21:R23)</f>
         <v>0.19116987590893744</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <f>HARMEAN('40 - Models'!L42:L44,'40 - Models'!O42:O44,'40 - Models'!R42:R44)</f>
         <v>0.14034154529106099</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <f>HARMEAN('40 - Models'!L63:L65,'40 - Models'!O63:O65,'40 - Models'!R63:R65)</f>
         <v>0.12629952919295748</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <f>HARMEAN('40 - Models'!L84:L86,'40 - Models'!O84:O86,'40 - Models'!R84:R86)</f>
         <v>0.12323666324336834</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <f>HARMEAN('40 - Models'!L105:L107,'40 - Models'!O105:O107,'40 - Models'!R105:R107)</f>
         <v>0.1695255987848355</v>
       </c>
@@ -6225,23 +6128,23 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table5[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table5[[#This Row],[Models]]</f>
         <v>30</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <f>HARMEAN('40 - Models'!L24:L26,'40 - Models'!O24:O26,'40 - Models'!R24:R26)</f>
         <v>0.23112729160001227</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <f>HARMEAN('40 - Models'!L45:L47,'40 - Models'!O45:O47,'40 - Models'!R45:R47)</f>
         <v>0.22708745996596125</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <f>HARMEAN('40 - Models'!L66:L68,'40 - Models'!O66:O68,'40 - Models'!R66:R68)</f>
         <v>0.14112515449175733</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <f>HARMEAN('40 - Models'!L87:L89,'40 - Models'!O87:O89,'40 - Models'!R87:R89)</f>
         <v>0.15417903466059946</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <f>HARMEAN('40 - Models'!L108:L110,'40 - Models'!O108:O110,'40 - Models'!R108:R110)</f>
         <v>0.18908759871486996</v>
       </c>
@@ -6277,23 +6180,23 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table4[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table4[[#This Row],[Models]]</f>
         <v>6</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <f>HARMEAN('40 - Models'!AB12:AB14,'40 - Models'!AE12:AE14,'40 - Models'!AH12:AH14)</f>
         <v>0.30144674955333528</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <f>HARMEAN('40 - Models'!AB33:AB35,'40 - Models'!AE33:AE35,'40 - Models'!AH33:AH35)</f>
         <v>0.26271717043663456</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <f>HARMEAN('40 - Models'!AB54:AB56,'40 - Models'!AE54:AE56,'40 - Models'!AH54:AH56)</f>
         <v>0.3103117867143107</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <f>HARMEAN('40 - Models'!AB75:AB77,'40 - Models'!AE75:AE77,'40 - Models'!AH75:AH77)</f>
         <v>0.28661775870741463</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <f>HARMEAN('40 - Models'!AB96:AB98,'40 - Models'!AE96:AE98,'40 - Models'!AH96:AH98)</f>
         <v>0.31720926936384841</v>
       </c>
@@ -6306,23 +6209,23 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table4[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table4[[#This Row],[Models]]</f>
         <v>12</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <f>HARMEAN('40 - Models'!AB15:AB17,'40 - Models'!AE15:AE17,'40 - Models'!AH15:AH17)</f>
         <v>0.70487610846063131</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <f>HARMEAN('40 - Models'!AB36:AB38,'40 - Models'!AE36:AE38,'40 - Models'!AH36:AH38)</f>
         <v>0.9855389183779858</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <f>HARMEAN('40 - Models'!AB57:AB59,'40 - Models'!AE57:AE59,'40 - Models'!AH57:AH59)</f>
         <v>0.7290030969009762</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <f>HARMEAN('40 - Models'!AB78:AB80,'40 - Models'!AE78:AE80,'40 - Models'!AH78:AH80)</f>
         <v>0.69737861410103907</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <f>HARMEAN('40 - Models'!AB99:AB101,'40 - Models'!AE99:AE101,'40 - Models'!AH99:AH101)</f>
         <v>0.91456162496331495</v>
       </c>
@@ -6335,23 +6238,23 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table4[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table4[[#This Row],[Models]]</f>
         <v>18</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <f>HARMEAN('40 - Models'!AB18:AB20,'40 - Models'!AE18:AE20,'40 - Models'!AH18:AH20)</f>
         <v>7.1782102891205311</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <f>HARMEAN('40 - Models'!AB39:AB41,'40 - Models'!AE39:AE41,'40 - Models'!AH39:AH41)</f>
         <v>7.3579809941861845</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <f>HARMEAN('40 - Models'!AB60:AB62,'40 - Models'!AE60:AE62,'40 - Models'!AH60:AH62)</f>
         <v>5.7141563995510145</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <f>HARMEAN('40 - Models'!AB81:AB83,'40 - Models'!AE81:AE83,'40 - Models'!AH81:AH83)</f>
         <v>4.9914634565127107</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <f>HARMEAN('40 - Models'!AB102:AB104,'40 - Models'!AE102:AE104,'40 - Models'!AH102:AH104)</f>
         <v>4.3989062384179087</v>
       </c>
@@ -6364,23 +6267,23 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table4[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table4[[#This Row],[Models]]</f>
         <v>24</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <f>HARMEAN('40 - Models'!AB21:AB23,'40 - Models'!AE21:AE23,'40 - Models'!AH21:AH23)</f>
         <v>30.133753885968989</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <f>HARMEAN('40 - Models'!AB42:AB44,'40 - Models'!AE42:AE44,'40 - Models'!AH42:AH44)</f>
         <v>31.92406529142966</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <f>HARMEAN('40 - Models'!AB63:AB65,'40 - Models'!AE63:AE65,'40 - Models'!AH63:AH65)</f>
         <v>36.188664846837895</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <f>HARMEAN('40 - Models'!AB84:AB86,'40 - Models'!AE84:AE86,'40 - Models'!AH84:AH86)</f>
         <v>31.766448089786131</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <f>HARMEAN('40 - Models'!AB105:AB107,'40 - Models'!AE105:AE107,'40 - Models'!AH105:AH107)</f>
         <v>35.275599422759733</v>
       </c>
@@ -6393,28 +6296,28 @@
         <f>'40 - Models'!$B$2*'40 - Models'!$B$6*Table4[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table4[[#This Row],[Models]]</f>
         <v>30</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <f>HARMEAN('40 - Models'!AB24:AB26,'40 - Models'!AE24:AE26,'40 - Models'!AH24:AH26)</f>
         <v>9.3311456376174444</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <f>HARMEAN('40 - Models'!AB45:AB47,'40 - Models'!AE45:AE47,'40 - Models'!AH45:AH47)</f>
         <v>13.845771604971324</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <f>HARMEAN('40 - Models'!AB66:AB68,'40 - Models'!AE66:AE68,'40 - Models'!AH66:AH68)</f>
         <v>30.470053843172394</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <f>HARMEAN('40 - Models'!AB87:AB89,'40 - Models'!AE87:AE89,'40 - Models'!AH87:AH89)</f>
         <v>33.888986502272239</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <f>HARMEAN('40 - Models'!AB108:AB110,'40 - Models'!AE108:AE110,'40 - Models'!AH108:AH110)</f>
         <v>9.9094177195687347</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -6433,11 +6336,8 @@
       <c r="F20" t="s">
         <v>61</v>
       </c>
-      <c r="G20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -6445,16 +6345,18 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table414[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table414[[#This Row],[Models]]</f>
         <v>12</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <f>HARMEAN('80 - Models'!L12:L14,'80 - Models'!O12:O14,'80 - Models'!R12:R14)</f>
         <v>0.12522936270672017</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D21" s="7">
+        <f>HARMEAN('80 - Models'!L33:L35,'80 - Models'!O33:O35,'80 - Models'!R33:R35)</f>
+        <v>0.11439175202788675</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -6462,16 +6364,18 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table414[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table414[[#This Row],[Models]]</f>
         <v>24</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <f>HARMEAN('80 - Models'!L15:L17,'80 - Models'!O15:O17,'80 - Models'!R15:R17)</f>
         <v>0.22079819666039632</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D22" s="7">
+        <f>HARMEAN('80 - Models'!L36:L38,'80 - Models'!O36:O38,'80 - Models'!R36:R38)</f>
+        <v>0.14781688745976435</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -6479,16 +6383,18 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table414[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table414[[#This Row],[Models]]</f>
         <v>36</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <f>HARMEAN('80 - Models'!L18:L20,'80 - Models'!O18:O20,'80 - Models'!R18:R20)</f>
         <v>0.37773472606510916</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" s="7">
+        <f>HARMEAN('80 - Models'!L39:L41,'80 - Models'!O39:O41,'80 - Models'!R39:R41)</f>
+        <v>0.24908093144028493</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
@@ -6496,16 +6402,18 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table414[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table414[[#This Row],[Models]]</f>
         <v>48</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <f>HARMEAN('80 - Models'!L21:L23,'80 - Models'!O21:O23,'80 - Models'!R21:R23)</f>
         <v>0.5730018492119725</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" s="7">
+        <f>HARMEAN('80 - Models'!L42:L44,'80 - Models'!O42:O44,'80 - Models'!R42:R44)</f>
+        <v>0.26994033745986379</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -6513,16 +6421,18 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table414[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table414[[#This Row],[Models]]</f>
         <v>60</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <f>HARMEAN('80 - Models'!L24:L26,'80 - Models'!O24:O26,'80 - Models'!R24:R26)</f>
         <v>0.68858636014817731</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" s="7">
+        <f>HARMEAN('80 - Models'!L45:L47,'80 - Models'!O45:O47,'80 - Models'!R45:R47)</f>
+        <v>0.30074901114503988</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -6541,11 +6451,8 @@
       <c r="F29" t="s">
         <v>61</v>
       </c>
-      <c r="G29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
@@ -6553,16 +6460,18 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table41415[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table41415[[#This Row],[Models]]</f>
         <v>12</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <f>HARMEAN('80 - Models'!AB12:AB14,'80 - Models'!AE12:AE14,'80 - Models'!AH12:AH14)</f>
         <v>0.42042899495736996</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D30" s="7">
+        <f>HARMEAN('80 - Models'!AB33:AB35,'80 - Models'!AE33:AE35,'80 - Models'!AH33:AH35)</f>
+        <v>0.56580424271293084</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2</v>
       </c>
@@ -6570,16 +6479,18 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table41415[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table41415[[#This Row],[Models]]</f>
         <v>24</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <f>HARMEAN('80 - Models'!AB15:AB17,'80 - Models'!AE15:AE17,'80 - Models'!AH15:AH17)</f>
         <v>9.1304432066740002</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D31" s="7">
+        <f>HARMEAN('80 - Models'!AB36:AB38,'80 - Models'!AE36:AE38,'80 - Models'!AH36:AH38)</f>
+        <v>20.128869116490275</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -6587,16 +6498,18 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table41415[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table41415[[#This Row],[Models]]</f>
         <v>36</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="7">
         <f>HARMEAN('80 - Models'!AB18:AB20,'80 - Models'!AE18:AE20,'80 - Models'!AH18:AH20)</f>
         <v>25.844199160281665</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D32" s="7">
+        <f>HARMEAN('80 - Models'!AB39:AB41,'80 - Models'!AE39:AE41,'80 - Models'!AH39:AH41)</f>
+        <v>37.410604615631556</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -6604,16 +6517,18 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table41415[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table41415[[#This Row],[Models]]</f>
         <v>48</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <f>HARMEAN('80 - Models'!AB21:AB23,'80 - Models'!AE21:AE23,'80 - Models'!AH21:AH23)</f>
         <v>20.128765769100387</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D33" s="7">
+        <f>HARMEAN('80 - Models'!AB42:AB44,'80 - Models'!AE42:AE44,'80 - Models'!AH42:AH44)</f>
+        <v>13.871834631856656</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>5</v>
       </c>
@@ -6621,14 +6536,16 @@
         <f>'80 - Models'!$B$2*'80 - Models'!$B$6*Table41415[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table41415[[#This Row],[Models]]</f>
         <v>60</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <f>HARMEAN('80 - Models'!AB24:AB26,'80 - Models'!AE24:AE26,'80 - Models'!AH24:AH26)</f>
         <v>42.83365578908839</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
+      <c r="D34" s="7">
+        <f>HARMEAN('80 - Models'!AB45:AB47,'80 - Models'!AE45:AE47,'80 - Models'!AH45:AH47)</f>
+        <v>8.5724833041754245</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6743,54 +6660,54 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7" t="s">
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7" t="s">
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7" t="s">
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7" t="s">
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="7" t="s">
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE10" s="7"/>
-      <c r="AF10" s="7"/>
-      <c r="AG10" s="7" t="s">
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH10" s="7"/>
-      <c r="AI10" s="7"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -8513,54 +8430,54 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7" t="s">
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7" t="s">
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7" t="s">
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7" t="s">
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="7" t="s">
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8"/>
+      <c r="Z31" s="8"/>
+      <c r="AA31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB31" s="7"/>
-      <c r="AC31" s="7"/>
-      <c r="AD31" s="7" t="s">
+      <c r="AB31" s="8"/>
+      <c r="AC31" s="8"/>
+      <c r="AD31" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE31" s="7"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="7" t="s">
+      <c r="AE31" s="8"/>
+      <c r="AF31" s="8"/>
+      <c r="AG31" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH31" s="7"/>
-      <c r="AI31" s="7"/>
+      <c r="AH31" s="8"/>
+      <c r="AI31" s="8"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -10283,54 +10200,54 @@
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7" t="s">
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7" t="s">
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O52" s="7"/>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="7" t="s">
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R52" s="7"/>
-      <c r="S52" s="7"/>
-      <c r="T52" s="7" t="s">
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U52" s="7"/>
-      <c r="V52" s="7"/>
-      <c r="W52" s="7"/>
-      <c r="X52" s="7"/>
-      <c r="Y52" s="7"/>
-      <c r="Z52" s="7"/>
-      <c r="AA52" s="7" t="s">
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
+      <c r="AA52" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB52" s="7"/>
-      <c r="AC52" s="7"/>
-      <c r="AD52" s="7" t="s">
+      <c r="AB52" s="8"/>
+      <c r="AC52" s="8"/>
+      <c r="AD52" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE52" s="7"/>
-      <c r="AF52" s="7"/>
-      <c r="AG52" s="7" t="s">
+      <c r="AE52" s="8"/>
+      <c r="AF52" s="8"/>
+      <c r="AG52" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH52" s="7"/>
-      <c r="AI52" s="7"/>
+      <c r="AH52" s="8"/>
+      <c r="AI52" s="8"/>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -12053,54 +11970,54 @@
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="7"/>
-      <c r="K73" s="7" t="s">
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7" t="s">
+      <c r="L73" s="8"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O73" s="7"/>
-      <c r="P73" s="7"/>
-      <c r="Q73" s="7" t="s">
+      <c r="O73" s="8"/>
+      <c r="P73" s="8"/>
+      <c r="Q73" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R73" s="7"/>
-      <c r="S73" s="7"/>
-      <c r="T73" s="7" t="s">
+      <c r="R73" s="8"/>
+      <c r="S73" s="8"/>
+      <c r="T73" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U73" s="7"/>
-      <c r="V73" s="7"/>
-      <c r="W73" s="7"/>
-      <c r="X73" s="7"/>
-      <c r="Y73" s="7"/>
-      <c r="Z73" s="7"/>
-      <c r="AA73" s="7" t="s">
+      <c r="U73" s="8"/>
+      <c r="V73" s="8"/>
+      <c r="W73" s="8"/>
+      <c r="X73" s="8"/>
+      <c r="Y73" s="8"/>
+      <c r="Z73" s="8"/>
+      <c r="AA73" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB73" s="7"/>
-      <c r="AC73" s="7"/>
-      <c r="AD73" s="7" t="s">
+      <c r="AB73" s="8"/>
+      <c r="AC73" s="8"/>
+      <c r="AD73" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE73" s="7"/>
-      <c r="AF73" s="7"/>
-      <c r="AG73" s="7" t="s">
+      <c r="AE73" s="8"/>
+      <c r="AF73" s="8"/>
+      <c r="AG73" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH73" s="7"/>
-      <c r="AI73" s="7"/>
+      <c r="AH73" s="8"/>
+      <c r="AI73" s="8"/>
     </row>
     <row r="74" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -13823,54 +13740,54 @@
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7" t="s">
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="8"/>
+      <c r="J94" s="8"/>
+      <c r="K94" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L94" s="7"/>
-      <c r="M94" s="7"/>
-      <c r="N94" s="7" t="s">
+      <c r="L94" s="8"/>
+      <c r="M94" s="8"/>
+      <c r="N94" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O94" s="7"/>
-      <c r="P94" s="7"/>
-      <c r="Q94" s="7" t="s">
+      <c r="O94" s="8"/>
+      <c r="P94" s="8"/>
+      <c r="Q94" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R94" s="7"/>
-      <c r="S94" s="7"/>
-      <c r="T94" s="7" t="s">
+      <c r="R94" s="8"/>
+      <c r="S94" s="8"/>
+      <c r="T94" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U94" s="7"/>
-      <c r="V94" s="7"/>
-      <c r="W94" s="7"/>
-      <c r="X94" s="7"/>
-      <c r="Y94" s="7"/>
-      <c r="Z94" s="7"/>
-      <c r="AA94" s="7" t="s">
+      <c r="U94" s="8"/>
+      <c r="V94" s="8"/>
+      <c r="W94" s="8"/>
+      <c r="X94" s="8"/>
+      <c r="Y94" s="8"/>
+      <c r="Z94" s="8"/>
+      <c r="AA94" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB94" s="7"/>
-      <c r="AC94" s="7"/>
-      <c r="AD94" s="7" t="s">
+      <c r="AB94" s="8"/>
+      <c r="AC94" s="8"/>
+      <c r="AD94" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE94" s="7"/>
-      <c r="AF94" s="7"/>
-      <c r="AG94" s="7" t="s">
+      <c r="AE94" s="8"/>
+      <c r="AF94" s="8"/>
+      <c r="AG94" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH94" s="7"/>
-      <c r="AI94" s="7"/>
+      <c r="AH94" s="8"/>
+      <c r="AI94" s="8"/>
     </row>
     <row r="95" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
@@ -15586,14 +15503,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="AA94:AC94"/>
-    <mergeCell ref="AD94:AF94"/>
-    <mergeCell ref="AG94:AI94"/>
-    <mergeCell ref="D94:J94"/>
-    <mergeCell ref="K94:M94"/>
-    <mergeCell ref="N94:P94"/>
-    <mergeCell ref="Q94:S94"/>
-    <mergeCell ref="T94:Z94"/>
+    <mergeCell ref="AA73:AC73"/>
+    <mergeCell ref="AD73:AF73"/>
+    <mergeCell ref="AG73:AI73"/>
+    <mergeCell ref="D73:J73"/>
+    <mergeCell ref="K73:M73"/>
+    <mergeCell ref="N73:P73"/>
+    <mergeCell ref="Q73:S73"/>
+    <mergeCell ref="T73:Z73"/>
+    <mergeCell ref="AA31:AC31"/>
+    <mergeCell ref="AD31:AF31"/>
+    <mergeCell ref="AG31:AI31"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="N31:P31"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="T31:Z31"/>
     <mergeCell ref="AD10:AF10"/>
     <mergeCell ref="AG10:AI10"/>
     <mergeCell ref="T10:Z10"/>
@@ -15610,22 +15535,14 @@
     <mergeCell ref="N10:P10"/>
     <mergeCell ref="Q10:S10"/>
     <mergeCell ref="AA10:AC10"/>
-    <mergeCell ref="AA31:AC31"/>
-    <mergeCell ref="AD31:AF31"/>
-    <mergeCell ref="AG31:AI31"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="N31:P31"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="AA73:AC73"/>
-    <mergeCell ref="AD73:AF73"/>
-    <mergeCell ref="AG73:AI73"/>
-    <mergeCell ref="D73:J73"/>
-    <mergeCell ref="K73:M73"/>
-    <mergeCell ref="N73:P73"/>
-    <mergeCell ref="Q73:S73"/>
-    <mergeCell ref="T73:Z73"/>
+    <mergeCell ref="AA94:AC94"/>
+    <mergeCell ref="AD94:AF94"/>
+    <mergeCell ref="AG94:AI94"/>
+    <mergeCell ref="D94:J94"/>
+    <mergeCell ref="K94:M94"/>
+    <mergeCell ref="N94:P94"/>
+    <mergeCell ref="Q94:S94"/>
+    <mergeCell ref="T94:Z94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -15643,8 +15560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI110"/>
   <sheetViews>
-    <sheetView topLeftCell="Z7" workbookViewId="0">
-      <selection activeCell="AJ27" sqref="AJ27"/>
+    <sheetView topLeftCell="Z25" workbookViewId="0">
+      <selection activeCell="AJ48" sqref="AJ48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15706,54 +15623,54 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7" t="s">
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7" t="s">
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7" t="s">
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7" t="s">
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="7" t="s">
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE10" s="7"/>
-      <c r="AF10" s="7"/>
-      <c r="AG10" s="7" t="s">
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH10" s="7"/>
-      <c r="AI10" s="7"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -17476,54 +17393,54 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7" t="s">
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7" t="s">
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7" t="s">
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7" t="s">
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="7" t="s">
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8"/>
+      <c r="Z31" s="8"/>
+      <c r="AA31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB31" s="7"/>
-      <c r="AC31" s="7"/>
-      <c r="AD31" s="7" t="s">
+      <c r="AB31" s="8"/>
+      <c r="AC31" s="8"/>
+      <c r="AD31" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE31" s="7"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="7" t="s">
+      <c r="AE31" s="8"/>
+      <c r="AF31" s="8"/>
+      <c r="AG31" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH31" s="7"/>
-      <c r="AI31" s="7"/>
+      <c r="AH31" s="8"/>
+      <c r="AI31" s="8"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -17632,140 +17549,1610 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>19</v>
+      </c>
+      <c r="D33">
+        <v>1298</v>
+      </c>
+      <c r="E33">
+        <v>1420</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="G33">
+        <v>46</v>
+      </c>
+      <c r="H33">
+        <v>16</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0.161</v>
+      </c>
+      <c r="L33">
+        <v>0.125</v>
+      </c>
+      <c r="M33">
+        <v>0.18</v>
+      </c>
+      <c r="N33">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="O33">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="P33">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="Q33">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="R33">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="S33">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="T33">
+        <v>5258</v>
+      </c>
+      <c r="U33">
+        <v>5380</v>
+      </c>
+      <c r="V33">
+        <v>1000</v>
+      </c>
+      <c r="W33">
+        <v>23532</v>
+      </c>
+      <c r="X33">
+        <v>45027</v>
+      </c>
+      <c r="Y33">
+        <v>21518</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AB33">
+        <v>11.699</v>
+      </c>
+      <c r="AC33">
+        <v>11.75</v>
+      </c>
+      <c r="AD33">
+        <v>0.161</v>
+      </c>
+      <c r="AE33">
+        <v>10.167</v>
+      </c>
+      <c r="AF33">
+        <v>10.214</v>
+      </c>
+      <c r="AG33">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AH33">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="AI33">
+        <v>9.9969999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>24</v>
+      </c>
+      <c r="D34">
+        <v>1401</v>
+      </c>
+      <c r="E34">
+        <v>1534</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34">
+        <v>44</v>
+      </c>
+      <c r="H34">
+        <v>17</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="L34">
+        <v>0.11</v>
+      </c>
+      <c r="M34">
+        <v>0.154</v>
+      </c>
+      <c r="N34">
+        <v>0.154</v>
+      </c>
+      <c r="O34">
+        <v>0.09</v>
+      </c>
+      <c r="P34">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="Q34">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="R34">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="S34">
+        <v>0.128</v>
+      </c>
+      <c r="T34" s="2">
+        <v>5361</v>
+      </c>
+      <c r="U34" s="2">
+        <v>5494</v>
+      </c>
+      <c r="V34" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W34">
+        <v>57160</v>
+      </c>
+      <c r="X34">
+        <v>112286</v>
+      </c>
+      <c r="Y34">
+        <v>55151</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="AB34">
+        <v>19.152999999999999</v>
+      </c>
+      <c r="AC34">
+        <v>19.207999999999998</v>
+      </c>
+      <c r="AD34">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="AE34">
+        <v>18.62</v>
+      </c>
+      <c r="AF34">
+        <v>18.670000000000002</v>
+      </c>
+      <c r="AG34">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AH34">
+        <v>19.187999999999999</v>
+      </c>
+      <c r="AI34">
+        <v>19.228999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>1324</v>
+      </c>
+      <c r="E35">
+        <v>1449</v>
+      </c>
+      <c r="F35">
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <v>58</v>
+      </c>
+      <c r="H35">
+        <v>81</v>
+      </c>
+      <c r="I35">
+        <v>35</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="L35">
+        <v>0.125</v>
+      </c>
+      <c r="M35">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="N35">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="O35">
+        <v>0.111</v>
+      </c>
+      <c r="P35">
+        <v>0.155</v>
+      </c>
+      <c r="Q35">
+        <v>0.151</v>
+      </c>
+      <c r="R35">
+        <v>0.123</v>
+      </c>
+      <c r="S35">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="T35">
+        <v>1380</v>
+      </c>
+      <c r="U35">
+        <v>1505</v>
+      </c>
+      <c r="V35">
+        <v>24</v>
+      </c>
+      <c r="W35">
+        <v>219</v>
+      </c>
+      <c r="X35">
+        <v>391</v>
+      </c>
+      <c r="Y35">
+        <v>172</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <v>0.154</v>
+      </c>
+      <c r="AB35">
+        <v>0.193</v>
+      </c>
+      <c r="AC35">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="AD35">
+        <v>0.15</v>
+      </c>
+      <c r="AE35">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AF35">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="AG35">
+        <v>0.159</v>
+      </c>
+      <c r="AH35">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="AI35">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36">
+        <v>2712</v>
+      </c>
+      <c r="E36">
+        <v>2986</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="G36">
+        <v>59</v>
+      </c>
+      <c r="H36">
+        <v>16</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0.154</v>
+      </c>
+      <c r="L36">
+        <v>0.13</v>
+      </c>
+      <c r="M36">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="N36">
+        <v>0.186</v>
+      </c>
+      <c r="O36">
+        <v>0.17</v>
+      </c>
+      <c r="P36">
+        <v>0.221</v>
+      </c>
+      <c r="Q36">
+        <v>0.193</v>
+      </c>
+      <c r="R36">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="S36">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="T36">
+        <v>6672</v>
+      </c>
+      <c r="U36">
+        <v>6946</v>
+      </c>
+      <c r="V36">
+        <v>1000</v>
+      </c>
+      <c r="W36">
+        <v>34535</v>
+      </c>
+      <c r="X36">
+        <v>67002</v>
+      </c>
+      <c r="Y36">
+        <v>32506</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <v>0.16</v>
+      </c>
+      <c r="AB36">
+        <v>15.256</v>
+      </c>
+      <c r="AC36">
+        <v>15.305999999999999</v>
+      </c>
+      <c r="AD36">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="AE36">
+        <v>14.387</v>
+      </c>
+      <c r="AF36">
+        <v>14.441000000000001</v>
+      </c>
+      <c r="AG36">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="AH36">
+        <v>13.555</v>
+      </c>
+      <c r="AI36">
+        <v>13.606999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>11</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37">
+        <v>2658</v>
+      </c>
+      <c r="E37">
+        <v>2921</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37">
+        <v>71</v>
+      </c>
+      <c r="H37">
+        <v>18</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0.16</v>
+      </c>
+      <c r="L37">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="M37">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="N37">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="O37">
+        <v>0.126</v>
+      </c>
+      <c r="P37">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="Q37">
+        <v>0.152</v>
+      </c>
+      <c r="R37">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="S37">
+        <v>0.185</v>
+      </c>
+      <c r="T37" s="2">
+        <v>6618</v>
+      </c>
+      <c r="U37" s="2">
+        <v>6881</v>
+      </c>
+      <c r="V37" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W37">
+        <v>24321</v>
+      </c>
+      <c r="X37">
+        <v>46544</v>
+      </c>
+      <c r="Y37">
+        <v>22276</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <v>0.161</v>
+      </c>
+      <c r="AB37">
+        <v>12.82</v>
+      </c>
+      <c r="AC37">
+        <v>12.872</v>
+      </c>
+      <c r="AD37">
+        <v>0.16</v>
+      </c>
+      <c r="AE37">
+        <v>14.275</v>
+      </c>
+      <c r="AF37">
+        <v>14.329000000000001</v>
+      </c>
+      <c r="AG37">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="AH37">
+        <v>13.141999999999999</v>
+      </c>
+      <c r="AI37">
+        <v>13.202999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>12</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C38" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38">
+        <v>2616</v>
+      </c>
+      <c r="E38">
+        <v>2878</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <v>62</v>
+      </c>
+      <c r="H38">
+        <v>17</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0.154</v>
+      </c>
+      <c r="L38">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="M38">
+        <v>0.189</v>
+      </c>
+      <c r="N38">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="O38">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="P38">
+        <v>0.185</v>
+      </c>
+      <c r="Q38">
+        <v>0.157</v>
+      </c>
+      <c r="R38">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="S38">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="T38">
+        <v>6576</v>
+      </c>
+      <c r="U38">
+        <v>6838</v>
+      </c>
+      <c r="V38">
+        <v>1000</v>
+      </c>
+      <c r="W38">
+        <v>699070</v>
+      </c>
+      <c r="X38">
+        <v>1396067</v>
+      </c>
+      <c r="Y38">
+        <v>697041</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AB38">
+        <v>193.613</v>
+      </c>
+      <c r="AC38">
+        <v>193.66499999999999</v>
+      </c>
+      <c r="AD38">
+        <v>0.21</v>
+      </c>
+      <c r="AE38">
+        <v>216.87700000000001</v>
+      </c>
+      <c r="AF38">
+        <v>216.94399999999999</v>
+      </c>
+      <c r="AG38">
+        <v>0.221</v>
+      </c>
+      <c r="AH38">
+        <v>228.99600000000001</v>
+      </c>
+      <c r="AI38">
+        <v>229.059</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C39" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39">
+        <v>3994</v>
+      </c>
+      <c r="E39">
+        <v>4393</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>79</v>
+      </c>
+      <c r="H39">
+        <v>20</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="L39">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="M39">
+        <v>0.317</v>
+      </c>
+      <c r="N39">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O39">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="P39">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="Q39">
+        <v>0.315</v>
+      </c>
+      <c r="R39">
+        <v>0.318</v>
+      </c>
+      <c r="S39">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="T39">
+        <v>7954</v>
+      </c>
+      <c r="U39">
+        <v>8353</v>
+      </c>
+      <c r="V39">
+        <v>1000</v>
+      </c>
+      <c r="W39">
+        <v>52304</v>
+      </c>
+      <c r="X39">
+        <v>102504</v>
+      </c>
+      <c r="Y39">
+        <v>50259</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
+      <c r="AA39">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="AB39">
+        <v>45.445999999999998</v>
+      </c>
+      <c r="AC39">
+        <v>45.539000000000001</v>
+      </c>
+      <c r="AD39">
+        <v>0.308</v>
+      </c>
+      <c r="AE39">
+        <v>45.85</v>
+      </c>
+      <c r="AF39">
+        <v>45.945</v>
+      </c>
+      <c r="AG39">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="AH39">
+        <v>50.021000000000001</v>
+      </c>
+      <c r="AI39">
+        <v>50.12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>21</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>3886</v>
+      </c>
+      <c r="E40">
+        <v>4275</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>65</v>
+      </c>
+      <c r="H40">
+        <v>18</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="L40">
+        <v>0.222</v>
+      </c>
+      <c r="M40">
+        <v>0.3</v>
+      </c>
+      <c r="N40">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="O40">
+        <v>0.245</v>
+      </c>
+      <c r="P40">
+        <v>0.33</v>
+      </c>
+      <c r="Q40">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="R40">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="S40">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="T40">
+        <v>7846</v>
+      </c>
+      <c r="U40">
+        <v>8235</v>
+      </c>
+      <c r="V40">
+        <v>1000</v>
+      </c>
+      <c r="W40">
+        <v>641535</v>
+      </c>
+      <c r="X40">
+        <v>1280987</v>
+      </c>
+      <c r="Y40">
+        <v>639498</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
+      <c r="AA40">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="AB40">
+        <v>287.80599999999998</v>
+      </c>
+      <c r="AC40">
+        <v>287.88200000000001</v>
+      </c>
+      <c r="AD40">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="AE40">
+        <v>300.07100000000003</v>
+      </c>
+      <c r="AF40">
+        <v>300.14</v>
+      </c>
+      <c r="AG40">
+        <v>0.254</v>
+      </c>
+      <c r="AH40">
+        <v>304.97899999999998</v>
+      </c>
+      <c r="AI40">
+        <v>305.06599999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>22</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>3972</v>
+      </c>
+      <c r="E41">
+        <v>4371</v>
+      </c>
+      <c r="F41">
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>48</v>
+      </c>
+      <c r="H41">
+        <v>17</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0.219</v>
+      </c>
+      <c r="L41">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="M41">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="N41">
+        <v>0.254</v>
+      </c>
+      <c r="O41">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="P41">
+        <v>0.315</v>
+      </c>
+      <c r="Q41">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="R41">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="S41">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="T41">
+        <v>7932</v>
+      </c>
+      <c r="U41">
+        <v>8331</v>
+      </c>
+      <c r="V41">
+        <v>1000</v>
+      </c>
+      <c r="W41">
+        <v>24297</v>
+      </c>
+      <c r="X41">
+        <v>46549</v>
+      </c>
+      <c r="Y41">
+        <v>22282</v>
+      </c>
+      <c r="Z41">
+        <v>0</v>
+      </c>
+      <c r="AA41">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="AB41">
+        <v>15.8</v>
+      </c>
+      <c r="AC41">
+        <v>15.87</v>
+      </c>
+      <c r="AD41">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="AE41">
+        <v>19.134</v>
+      </c>
+      <c r="AF41">
+        <v>19.228999999999999</v>
+      </c>
+      <c r="AG41">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="AH41">
+        <v>19.559000000000001</v>
+      </c>
+      <c r="AI41">
+        <v>19.643000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>30</v>
       </c>
       <c r="B42">
         <v>4</v>
       </c>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42">
+        <v>5414</v>
+      </c>
+      <c r="E42">
+        <v>5955</v>
+      </c>
+      <c r="F42">
+        <v>10</v>
+      </c>
+      <c r="G42">
+        <v>72</v>
+      </c>
+      <c r="H42">
+        <v>16</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="L42">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="M42">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="N42">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="O42">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="P42">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="Q42">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="R42">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="S42">
+        <v>0.36</v>
+      </c>
+      <c r="T42">
+        <v>9374</v>
+      </c>
+      <c r="U42">
+        <v>9915</v>
+      </c>
+      <c r="V42">
+        <v>1000</v>
+      </c>
+      <c r="W42">
+        <v>13922</v>
+      </c>
+      <c r="X42">
+        <v>25752</v>
+      </c>
+      <c r="Y42">
+        <v>11884</v>
+      </c>
+      <c r="Z42">
+        <v>0</v>
+      </c>
+      <c r="AA42">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AB42">
+        <v>12.994</v>
+      </c>
+      <c r="AC42">
+        <v>13.071</v>
+      </c>
+      <c r="AD42">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="AE42">
+        <v>13.489000000000001</v>
+      </c>
+      <c r="AF42">
+        <v>13.568</v>
+      </c>
+      <c r="AG42">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="AH42">
+        <v>13.494</v>
+      </c>
+      <c r="AI42">
+        <v>13.573</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>31</v>
       </c>
       <c r="B43">
         <v>4</v>
       </c>
-      <c r="C43" s="3"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43">
+        <v>5241</v>
+      </c>
+      <c r="E43">
+        <v>5768</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+      <c r="G43">
+        <v>105</v>
+      </c>
+      <c r="H43">
+        <v>20</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0.22</v>
+      </c>
+      <c r="L43">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="M43">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="N43">
+        <v>0.247</v>
+      </c>
+      <c r="O43">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="P43">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="Q43">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="R43">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="S43">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="T43">
+        <v>9201</v>
+      </c>
+      <c r="U43">
+        <v>9728</v>
+      </c>
+      <c r="V43">
+        <v>1000</v>
+      </c>
+      <c r="W43">
+        <v>130900</v>
+      </c>
+      <c r="X43">
+        <v>259643</v>
+      </c>
+      <c r="Y43">
+        <v>128826</v>
+      </c>
+      <c r="Z43">
+        <v>0</v>
+      </c>
+      <c r="AA43">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="AB43">
+        <v>73.477000000000004</v>
+      </c>
+      <c r="AC43">
+        <v>73.558999999999997</v>
+      </c>
+      <c r="AD43">
+        <v>0.3</v>
+      </c>
+      <c r="AE43">
+        <v>80.768000000000001</v>
+      </c>
+      <c r="AF43">
+        <v>80.858000000000004</v>
+      </c>
+      <c r="AG43">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="AH43">
+        <v>68.007999999999996</v>
+      </c>
+      <c r="AI43">
+        <v>68.093999999999994</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>32</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>5291</v>
+      </c>
+      <c r="E44">
+        <v>5828</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+      <c r="G44">
+        <v>112</v>
+      </c>
+      <c r="H44">
+        <v>16</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="L44">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="M44">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="N44">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="O44">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="P44">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="Q44">
+        <v>0.255</v>
+      </c>
+      <c r="R44">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="S44">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="T44">
+        <v>9251</v>
+      </c>
+      <c r="U44">
+        <v>9788</v>
+      </c>
+      <c r="V44">
+        <v>1000</v>
+      </c>
+      <c r="W44">
+        <v>7518</v>
+      </c>
+      <c r="X44">
+        <v>12866</v>
+      </c>
+      <c r="Y44">
+        <v>5439</v>
+      </c>
+      <c r="Z44">
+        <v>0</v>
+      </c>
+      <c r="AA44">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="AB44">
+        <v>8.3780000000000001</v>
+      </c>
+      <c r="AC44">
+        <v>8.4640000000000004</v>
+      </c>
+      <c r="AD44">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="AE44">
+        <v>7.5679999999999996</v>
+      </c>
+      <c r="AF44">
+        <v>7.6520000000000001</v>
+      </c>
+      <c r="AG44">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="AH44">
+        <v>7.61</v>
+      </c>
+      <c r="AI44">
+        <v>7.6920000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>40</v>
       </c>
       <c r="B45">
         <v>5</v>
       </c>
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45">
+        <v>6561</v>
+      </c>
+      <c r="E45">
+        <v>7225</v>
+      </c>
+      <c r="F45">
+        <v>10</v>
+      </c>
+      <c r="G45">
+        <v>127</v>
+      </c>
+      <c r="H45">
+        <v>18</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="L45">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="M45">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="N45">
+        <v>0.252</v>
+      </c>
+      <c r="O45">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="P45">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="Q45">
+        <v>0.33</v>
+      </c>
+      <c r="R45">
+        <v>0.39</v>
+      </c>
+      <c r="S45">
+        <v>0.49</v>
+      </c>
+      <c r="T45">
+        <v>10521</v>
+      </c>
+      <c r="U45">
+        <v>11185</v>
+      </c>
+      <c r="V45">
+        <v>1000</v>
+      </c>
+      <c r="W45">
+        <v>6073</v>
+      </c>
+      <c r="X45">
+        <v>9936</v>
+      </c>
+      <c r="Y45">
+        <v>3974</v>
+      </c>
+      <c r="Z45">
+        <v>0</v>
+      </c>
+      <c r="AA45">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="AB45">
+        <v>8.1240000000000006</v>
+      </c>
+      <c r="AC45">
+        <v>8.2089999999999996</v>
+      </c>
+      <c r="AD45">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="AE45">
+        <v>6.8840000000000003</v>
+      </c>
+      <c r="AF45">
+        <v>6.9640000000000004</v>
+      </c>
+      <c r="AG45">
+        <v>0.252</v>
+      </c>
+      <c r="AH45">
+        <v>6.6749999999999998</v>
+      </c>
+      <c r="AI45">
+        <v>6.766</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>41</v>
       </c>
       <c r="B46">
         <v>5</v>
       </c>
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46">
+        <v>6696</v>
+      </c>
+      <c r="E46">
+        <v>7372</v>
+      </c>
+      <c r="F46">
+        <v>10</v>
+      </c>
+      <c r="G46">
+        <v>132</v>
+      </c>
+      <c r="H46">
+        <v>20</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0.253</v>
+      </c>
+      <c r="L46">
+        <v>0.35</v>
+      </c>
+      <c r="M46">
+        <v>0.433</v>
+      </c>
+      <c r="N46">
+        <v>0.246</v>
+      </c>
+      <c r="O46">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="P46">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="Q46">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="R46">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="S46">
+        <v>0.505</v>
+      </c>
+      <c r="T46">
+        <v>10656</v>
+      </c>
+      <c r="U46">
+        <v>11332</v>
+      </c>
+      <c r="V46">
+        <v>1000</v>
+      </c>
+      <c r="W46">
+        <v>76071</v>
+      </c>
+      <c r="X46">
+        <v>149919</v>
+      </c>
+      <c r="Y46">
+        <v>73964</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
+      <c r="AA46">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="AB46">
+        <v>70.915000000000006</v>
+      </c>
+      <c r="AC46">
+        <v>70.995000000000005</v>
+      </c>
+      <c r="AD46">
+        <v>0.251</v>
+      </c>
+      <c r="AE46">
+        <v>71.352000000000004</v>
+      </c>
+      <c r="AF46">
+        <v>71.433000000000007</v>
+      </c>
+      <c r="AG46">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="AH46">
+        <v>60.25</v>
+      </c>
+      <c r="AI46">
+        <v>60.331000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>42</v>
       </c>
       <c r="B47">
         <v>5</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
+      <c r="C47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47">
+        <v>6475</v>
+      </c>
+      <c r="E47">
+        <v>7136</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47">
+        <v>88</v>
+      </c>
+      <c r="H47">
+        <v>23</v>
+      </c>
+      <c r="I47">
+        <v>7</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="L47">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="M47">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="N47">
+        <v>0.182</v>
+      </c>
+      <c r="O47">
+        <v>0.249</v>
+      </c>
+      <c r="P47">
+        <v>0.308</v>
+      </c>
+      <c r="Q47">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="R47">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="S47">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="T47" s="2">
+        <v>10435</v>
+      </c>
+      <c r="U47" s="2">
+        <v>11096</v>
+      </c>
+      <c r="V47" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W47">
+        <v>4961</v>
+      </c>
+      <c r="X47">
+        <v>7797</v>
+      </c>
+      <c r="Y47">
+        <v>2907</v>
+      </c>
+      <c r="Z47">
+        <v>0</v>
+      </c>
+      <c r="AA47">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="AB47">
+        <v>5.0730000000000004</v>
+      </c>
+      <c r="AC47">
+        <v>5.1349999999999998</v>
+      </c>
+      <c r="AD47">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="AE47">
+        <v>5.1180000000000003</v>
+      </c>
+      <c r="AF47">
+        <v>5.1779999999999999</v>
+      </c>
+      <c r="AG47">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="AH47">
+        <v>5.1420000000000003</v>
+      </c>
+      <c r="AI47">
+        <v>5.2030000000000003</v>
+      </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
@@ -17776,54 +19163,54 @@
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7" t="s">
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7" t="s">
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O52" s="7"/>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="7" t="s">
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R52" s="7"/>
-      <c r="S52" s="7"/>
-      <c r="T52" s="7" t="s">
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U52" s="7"/>
-      <c r="V52" s="7"/>
-      <c r="W52" s="7"/>
-      <c r="X52" s="7"/>
-      <c r="Y52" s="7"/>
-      <c r="Z52" s="7"/>
-      <c r="AA52" s="7" t="s">
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
+      <c r="AA52" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB52" s="7"/>
-      <c r="AC52" s="7"/>
-      <c r="AD52" s="7" t="s">
+      <c r="AB52" s="8"/>
+      <c r="AC52" s="8"/>
+      <c r="AD52" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE52" s="7"/>
-      <c r="AF52" s="7"/>
-      <c r="AG52" s="7" t="s">
+      <c r="AE52" s="8"/>
+      <c r="AF52" s="8"/>
+      <c r="AG52" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH52" s="7"/>
-      <c r="AI52" s="7"/>
+      <c r="AH52" s="8"/>
+      <c r="AI52" s="8"/>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -18095,54 +19482,54 @@
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="7"/>
-      <c r="K73" s="7" t="s">
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7" t="s">
+      <c r="L73" s="8"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O73" s="7"/>
-      <c r="P73" s="7"/>
-      <c r="Q73" s="7" t="s">
+      <c r="O73" s="8"/>
+      <c r="P73" s="8"/>
+      <c r="Q73" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R73" s="7"/>
-      <c r="S73" s="7"/>
-      <c r="T73" s="7" t="s">
+      <c r="R73" s="8"/>
+      <c r="S73" s="8"/>
+      <c r="T73" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U73" s="7"/>
-      <c r="V73" s="7"/>
-      <c r="W73" s="7"/>
-      <c r="X73" s="7"/>
-      <c r="Y73" s="7"/>
-      <c r="Z73" s="7"/>
-      <c r="AA73" s="7" t="s">
+      <c r="U73" s="8"/>
+      <c r="V73" s="8"/>
+      <c r="W73" s="8"/>
+      <c r="X73" s="8"/>
+      <c r="Y73" s="8"/>
+      <c r="Z73" s="8"/>
+      <c r="AA73" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB73" s="7"/>
-      <c r="AC73" s="7"/>
-      <c r="AD73" s="7" t="s">
+      <c r="AB73" s="8"/>
+      <c r="AC73" s="8"/>
+      <c r="AD73" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE73" s="7"/>
-      <c r="AF73" s="7"/>
-      <c r="AG73" s="7" t="s">
+      <c r="AE73" s="8"/>
+      <c r="AF73" s="8"/>
+      <c r="AG73" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH73" s="7"/>
-      <c r="AI73" s="7"/>
+      <c r="AH73" s="8"/>
+      <c r="AI73" s="8"/>
     </row>
     <row r="74" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -18420,54 +19807,54 @@
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7" t="s">
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="8"/>
+      <c r="J94" s="8"/>
+      <c r="K94" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L94" s="7"/>
-      <c r="M94" s="7"/>
-      <c r="N94" s="7" t="s">
+      <c r="L94" s="8"/>
+      <c r="M94" s="8"/>
+      <c r="N94" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O94" s="7"/>
-      <c r="P94" s="7"/>
-      <c r="Q94" s="7" t="s">
+      <c r="O94" s="8"/>
+      <c r="P94" s="8"/>
+      <c r="Q94" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R94" s="7"/>
-      <c r="S94" s="7"/>
-      <c r="T94" s="7" t="s">
+      <c r="R94" s="8"/>
+      <c r="S94" s="8"/>
+      <c r="T94" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U94" s="7"/>
-      <c r="V94" s="7"/>
-      <c r="W94" s="7"/>
-      <c r="X94" s="7"/>
-      <c r="Y94" s="7"/>
-      <c r="Z94" s="7"/>
-      <c r="AA94" s="7" t="s">
+      <c r="U94" s="8"/>
+      <c r="V94" s="8"/>
+      <c r="W94" s="8"/>
+      <c r="X94" s="8"/>
+      <c r="Y94" s="8"/>
+      <c r="Z94" s="8"/>
+      <c r="AA94" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AB94" s="7"/>
-      <c r="AC94" s="7"/>
-      <c r="AD94" s="7" t="s">
+      <c r="AB94" s="8"/>
+      <c r="AC94" s="8"/>
+      <c r="AD94" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE94" s="7"/>
-      <c r="AF94" s="7"/>
-      <c r="AG94" s="7" t="s">
+      <c r="AE94" s="8"/>
+      <c r="AF94" s="8"/>
+      <c r="AG94" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AH94" s="7"/>
-      <c r="AI94" s="7"/>
+      <c r="AH94" s="8"/>
+      <c r="AI94" s="8"/>
     </row>
     <row r="95" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
@@ -18749,14 +20136,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="AD94:AF94"/>
-    <mergeCell ref="AG94:AI94"/>
-    <mergeCell ref="D94:J94"/>
-    <mergeCell ref="K94:M94"/>
-    <mergeCell ref="N94:P94"/>
-    <mergeCell ref="Q94:S94"/>
-    <mergeCell ref="T94:Z94"/>
-    <mergeCell ref="AA94:AC94"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="AG10:AI10"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="N31:P31"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="AA31:AC31"/>
+    <mergeCell ref="AD31:AF31"/>
+    <mergeCell ref="AG31:AI31"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="T10:Z10"/>
+    <mergeCell ref="AA10:AC10"/>
     <mergeCell ref="AD52:AF52"/>
     <mergeCell ref="AG52:AI52"/>
     <mergeCell ref="D73:J73"/>
@@ -18773,22 +20168,14 @@
     <mergeCell ref="Q52:S52"/>
     <mergeCell ref="T52:Z52"/>
     <mergeCell ref="AA52:AC52"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="AG10:AI10"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="N31:P31"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="AA31:AC31"/>
-    <mergeCell ref="AD31:AF31"/>
-    <mergeCell ref="AG31:AI31"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="T10:Z10"/>
-    <mergeCell ref="AA10:AC10"/>
+    <mergeCell ref="AD94:AF94"/>
+    <mergeCell ref="AG94:AI94"/>
+    <mergeCell ref="D94:J94"/>
+    <mergeCell ref="K94:M94"/>
+    <mergeCell ref="N94:P94"/>
+    <mergeCell ref="Q94:S94"/>
+    <mergeCell ref="T94:Z94"/>
+    <mergeCell ref="AA94:AC94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="5">

</xml_diff>

<commit_message>
Updating tests summary for Heuristic 2 + 80.
</commit_message>
<xml_diff>
--- a/docs/testsFSG/tests-summary.xlsx
+++ b/docs/testsFSG/tests-summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8232" windowHeight="4296"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8232" windowHeight="4296" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="86">
   <si>
     <t>Run</t>
   </si>
@@ -371,7 +371,10 @@
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2038,6 +2041,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.4403439720453305E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12747786209302864</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16365266899139061</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20252825777913985</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23397925761994948</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2584,6 +2602,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.30892749190503238</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.89973204291565</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.235223571130939</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8942436050518818</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.756228717733677</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5203,11 +5236,11 @@
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'40 - Models'!$B$2*'40 - Models'!$B$6*Table4[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table4[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="17"/>
-    <tableColumn id="3" name="Heuristic 1" dataDxfId="16"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="15"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="14"/>
-    <tableColumn id="7" name="Heuristic 4" dataDxfId="13"/>
+    <tableColumn id="2" name="Default" dataDxfId="18"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="17"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="16"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="15"/>
+    <tableColumn id="7" name="Heuristic 4" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5263,7 +5296,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="1" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -5307,7 +5340,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="0" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -5441,11 +5474,11 @@
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'40 - Models'!$B$2*'40 - Models'!$B$6*Table5[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table5[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="12"/>
+    <tableColumn id="2" name="Default" dataDxfId="13"/>
     <tableColumn id="3" name="Heuristic 1"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="11"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="10"/>
-    <tableColumn id="7" name="Heuristic 4" dataDxfId="9"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="12"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="11"/>
+    <tableColumn id="7" name="Heuristic 4" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5459,10 +5492,10 @@
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'80 - Models'!$B$2*'80 - Models'!$B$6*Table414[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table414[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="8"/>
-    <tableColumn id="3" name="Heuristic 1" dataDxfId="7"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="6"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="5"/>
+    <tableColumn id="2" name="Default" dataDxfId="9"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="8"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="7"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5476,10 +5509,10 @@
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'80 - Models'!$B$2*'80 - Models'!$B$6*Table41415[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table41415[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="4"/>
-    <tableColumn id="3" name="Heuristic 1" dataDxfId="3"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="2"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="1"/>
+    <tableColumn id="2" name="Default" dataDxfId="5"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="4"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="3"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5970,8 +6003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6353,7 +6386,10 @@
         <f>HARMEAN('80 - Models'!L33:L35,'80 - Models'!O33:O35,'80 - Models'!R33:R35)</f>
         <v>0.11439175202788675</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="7">
+        <f>HARMEAN('80 - Models'!L54:L56,'80 - Models'!O54:O56,'80 - Models'!R54:R56)</f>
+        <v>8.4403439720453305E-2</v>
+      </c>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -6372,7 +6408,10 @@
         <f>HARMEAN('80 - Models'!L36:L38,'80 - Models'!O36:O38,'80 - Models'!R36:R38)</f>
         <v>0.14781688745976435</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="E22" s="7">
+        <f>HARMEAN('80 - Models'!L57:L59,'80 - Models'!O57:O59,'80 - Models'!R57:R59)</f>
+        <v>0.12747786209302864</v>
+      </c>
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -6391,7 +6430,10 @@
         <f>HARMEAN('80 - Models'!L39:L41,'80 - Models'!O39:O41,'80 - Models'!R39:R41)</f>
         <v>0.24908093144028493</v>
       </c>
-      <c r="E23" s="7"/>
+      <c r="E23" s="7">
+        <f>HARMEAN('80 - Models'!L60:L62,'80 - Models'!O60:O62,'80 - Models'!R60:R62)</f>
+        <v>0.16365266899139061</v>
+      </c>
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -6410,7 +6452,10 @@
         <f>HARMEAN('80 - Models'!L42:L44,'80 - Models'!O42:O44,'80 - Models'!R42:R44)</f>
         <v>0.26994033745986379</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="7">
+        <f>HARMEAN('80 - Models'!L63:L65,'80 - Models'!O63:O65,'80 - Models'!R63:R65)</f>
+        <v>0.20252825777913985</v>
+      </c>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -6429,7 +6474,10 @@
         <f>HARMEAN('80 - Models'!L45:L47,'80 - Models'!O45:O47,'80 - Models'!R45:R47)</f>
         <v>0.30074901114503988</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="7">
+        <f>HARMEAN('80 - Models'!L66:L68,'80 - Models'!O66:O68,'80 - Models'!R66:R68)</f>
+        <v>0.23397925761994948</v>
+      </c>
       <c r="F25" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -6468,7 +6516,10 @@
         <f>HARMEAN('80 - Models'!AB33:AB35,'80 - Models'!AE33:AE35,'80 - Models'!AH33:AH35)</f>
         <v>0.56580424271293084</v>
       </c>
-      <c r="E30" s="7"/>
+      <c r="E30" s="7">
+        <f>HARMEAN('80 - Models'!AB54:AB56,'80 - Models'!AE54:AE56,'80 - Models'!AH54:AH56)</f>
+        <v>0.30892749190503238</v>
+      </c>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -6487,7 +6538,10 @@
         <f>HARMEAN('80 - Models'!AB36:AB38,'80 - Models'!AE36:AE38,'80 - Models'!AH36:AH38)</f>
         <v>20.128869116490275</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="E31" s="7">
+        <f>HARMEAN('80 - Models'!AB57:AB59,'80 - Models'!AE57:AE59,'80 - Models'!AH57:AH59)</f>
+        <v>14.89973204291565</v>
+      </c>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -6506,7 +6560,10 @@
         <f>HARMEAN('80 - Models'!AB39:AB41,'80 - Models'!AE39:AE41,'80 - Models'!AH39:AH41)</f>
         <v>37.410604615631556</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="7">
+        <f>HARMEAN('80 - Models'!AB60:AB62,'80 - Models'!AE60:AE62,'80 - Models'!AH60:AH62)</f>
+        <v>14.235223571130939</v>
+      </c>
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -6525,7 +6582,10 @@
         <f>HARMEAN('80 - Models'!AB42:AB44,'80 - Models'!AE42:AE44,'80 - Models'!AH42:AH44)</f>
         <v>13.871834631856656</v>
       </c>
-      <c r="E33" s="7"/>
+      <c r="E33" s="7">
+        <f>HARMEAN('80 - Models'!AB63:AB65,'80 - Models'!AE63:AE65,'80 - Models'!AH63:AH65)</f>
+        <v>9.8942436050518818</v>
+      </c>
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -6544,7 +6604,10 @@
         <f>HARMEAN('80 - Models'!AB45:AB47,'80 - Models'!AE45:AE47,'80 - Models'!AH45:AH47)</f>
         <v>8.5724833041754245</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="7">
+        <f>HARMEAN('80 - Models'!AB66:AB68,'80 - Models'!AE66:AE68,'80 - Models'!AH66:AH68)</f>
+        <v>16.756228717733677</v>
+      </c>
       <c r="F34" s="7"/>
     </row>
   </sheetData>
@@ -15560,8 +15623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI110"/>
   <sheetViews>
-    <sheetView topLeftCell="Z25" workbookViewId="0">
-      <selection activeCell="AJ48" sqref="AJ48"/>
+    <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
+      <selection activeCell="V56" sqref="V56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19326,6 +19389,105 @@
       <c r="B54">
         <v>1</v>
       </c>
+      <c r="C54">
+        <v>19</v>
+      </c>
+      <c r="D54">
+        <v>1298</v>
+      </c>
+      <c r="E54">
+        <v>1420</v>
+      </c>
+      <c r="F54">
+        <v>10</v>
+      </c>
+      <c r="G54">
+        <v>37</v>
+      </c>
+      <c r="H54">
+        <v>24</v>
+      </c>
+      <c r="I54">
+        <v>5</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="L54">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="M54">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="N54">
+        <v>0.123</v>
+      </c>
+      <c r="O54">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P54">
+        <v>0.114</v>
+      </c>
+      <c r="Q54">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="R54">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="S54">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="T54">
+        <v>5258</v>
+      </c>
+      <c r="U54">
+        <v>5380</v>
+      </c>
+      <c r="V54">
+        <v>1000</v>
+      </c>
+      <c r="W54">
+        <v>33681</v>
+      </c>
+      <c r="X54">
+        <v>65329</v>
+      </c>
+      <c r="Y54">
+        <v>31674</v>
+      </c>
+      <c r="Z54">
+        <v>0</v>
+      </c>
+      <c r="AA54">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="AB54">
+        <v>9.0150000000000006</v>
+      </c>
+      <c r="AC54">
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="AD54">
+        <v>0.122</v>
+      </c>
+      <c r="AE54">
+        <v>8.7390000000000008</v>
+      </c>
+      <c r="AF54">
+        <v>8.7789999999999999</v>
+      </c>
+      <c r="AG54">
+        <v>0.122</v>
+      </c>
+      <c r="AH54">
+        <v>9.0370000000000008</v>
+      </c>
+      <c r="AI54">
+        <v>9.077</v>
+      </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -19334,6 +19496,105 @@
       <c r="B55">
         <v>1</v>
       </c>
+      <c r="C55">
+        <v>24</v>
+      </c>
+      <c r="D55">
+        <v>1401</v>
+      </c>
+      <c r="E55">
+        <v>1534</v>
+      </c>
+      <c r="F55">
+        <v>10</v>
+      </c>
+      <c r="G55">
+        <v>39</v>
+      </c>
+      <c r="H55">
+        <v>16</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0.13</v>
+      </c>
+      <c r="L55">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="M55">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="N55">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="O55">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="P55">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="Q55">
+        <v>0.218</v>
+      </c>
+      <c r="R55">
+        <v>0.09</v>
+      </c>
+      <c r="S55">
+        <v>0.18</v>
+      </c>
+      <c r="T55">
+        <v>5361</v>
+      </c>
+      <c r="U55">
+        <v>5494</v>
+      </c>
+      <c r="V55">
+        <v>1000</v>
+      </c>
+      <c r="W55">
+        <v>18942</v>
+      </c>
+      <c r="X55">
+        <v>35842</v>
+      </c>
+      <c r="Y55">
+        <v>16927</v>
+      </c>
+      <c r="Z55">
+        <v>0</v>
+      </c>
+      <c r="AA55">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="AB55">
+        <v>5.9459999999999997</v>
+      </c>
+      <c r="AC55">
+        <v>6.024</v>
+      </c>
+      <c r="AD55">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AE55">
+        <v>5.7770000000000001</v>
+      </c>
+      <c r="AF55">
+        <v>5.819</v>
+      </c>
+      <c r="AG55">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="AH55">
+        <v>6.0419999999999998</v>
+      </c>
+      <c r="AI55">
+        <v>6.0970000000000004</v>
+      </c>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -19342,6 +19603,105 @@
       <c r="B56">
         <v>1</v>
       </c>
+      <c r="C56">
+        <v>9</v>
+      </c>
+      <c r="D56">
+        <v>1324</v>
+      </c>
+      <c r="E56">
+        <v>1449</v>
+      </c>
+      <c r="F56">
+        <v>10</v>
+      </c>
+      <c r="G56">
+        <v>34</v>
+      </c>
+      <c r="H56">
+        <v>30</v>
+      </c>
+      <c r="I56">
+        <v>8</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="L56">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="M56">
+        <v>0.12</v>
+      </c>
+      <c r="N56">
+        <v>0.127</v>
+      </c>
+      <c r="O56">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="P56">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="Q56">
+        <v>0.128</v>
+      </c>
+      <c r="R56">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="S56">
+        <v>0.126</v>
+      </c>
+      <c r="T56">
+        <v>1420</v>
+      </c>
+      <c r="U56">
+        <v>1545</v>
+      </c>
+      <c r="V56">
+        <v>34</v>
+      </c>
+      <c r="W56">
+        <v>108</v>
+      </c>
+      <c r="X56">
+        <v>149</v>
+      </c>
+      <c r="Y56">
+        <v>41</v>
+      </c>
+      <c r="Z56">
+        <v>0</v>
+      </c>
+      <c r="AA56">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AB56">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="AC56">
+        <v>0.17</v>
+      </c>
+      <c r="AD56">
+        <v>0.122</v>
+      </c>
+      <c r="AE56">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AF56">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="AG56">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AH56">
+        <v>0.106</v>
+      </c>
+      <c r="AI56">
+        <v>0.14599999999999999</v>
+      </c>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -19350,7 +19710,105 @@
       <c r="B57">
         <v>2</v>
       </c>
-      <c r="C57" s="3"/>
+      <c r="C57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57">
+        <v>2712</v>
+      </c>
+      <c r="E57">
+        <v>2986</v>
+      </c>
+      <c r="F57">
+        <v>10</v>
+      </c>
+      <c r="G57">
+        <v>65</v>
+      </c>
+      <c r="H57">
+        <v>39</v>
+      </c>
+      <c r="I57">
+        <v>12</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="L57">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="M57">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="N57">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="O57">
+        <v>0.121</v>
+      </c>
+      <c r="P57">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="Q57">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="R57">
+        <v>0.121</v>
+      </c>
+      <c r="S57">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="T57">
+        <v>6672</v>
+      </c>
+      <c r="U57">
+        <v>6946</v>
+      </c>
+      <c r="V57">
+        <v>1000</v>
+      </c>
+      <c r="W57">
+        <v>154743</v>
+      </c>
+      <c r="X57">
+        <v>307426</v>
+      </c>
+      <c r="Y57">
+        <v>152720</v>
+      </c>
+      <c r="Z57">
+        <v>0</v>
+      </c>
+      <c r="AA57">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="AB57">
+        <v>50.284999999999997</v>
+      </c>
+      <c r="AC57">
+        <v>50.344999999999999</v>
+      </c>
+      <c r="AD57">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="AE57">
+        <v>48.427999999999997</v>
+      </c>
+      <c r="AF57">
+        <v>48.475000000000001</v>
+      </c>
+      <c r="AG57">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="AH57">
+        <v>48.423999999999999</v>
+      </c>
+      <c r="AI57">
+        <v>48.51</v>
+      </c>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -19359,10 +19817,105 @@
       <c r="B58">
         <v>2</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="W58" s="2"/>
-      <c r="X58" s="2"/>
-      <c r="Y58" s="2"/>
+      <c r="C58" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58">
+        <v>2658</v>
+      </c>
+      <c r="E58">
+        <v>2921</v>
+      </c>
+      <c r="F58">
+        <v>10</v>
+      </c>
+      <c r="G58">
+        <v>61</v>
+      </c>
+      <c r="H58">
+        <v>17</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0.216</v>
+      </c>
+      <c r="L58">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="M58">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="N58">
+        <v>0.158</v>
+      </c>
+      <c r="O58">
+        <v>0.113</v>
+      </c>
+      <c r="P58">
+        <v>0.16</v>
+      </c>
+      <c r="Q58">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="R58">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="S58">
+        <v>0.185</v>
+      </c>
+      <c r="T58">
+        <v>6618</v>
+      </c>
+      <c r="U58">
+        <v>6881</v>
+      </c>
+      <c r="V58">
+        <v>1000</v>
+      </c>
+      <c r="W58" s="2">
+        <v>229857</v>
+      </c>
+      <c r="X58" s="2">
+        <v>457644</v>
+      </c>
+      <c r="Y58" s="2">
+        <v>227831</v>
+      </c>
+      <c r="Z58">
+        <v>0</v>
+      </c>
+      <c r="AA58">
+        <v>0.188</v>
+      </c>
+      <c r="AB58">
+        <v>62.070999999999998</v>
+      </c>
+      <c r="AC58">
+        <v>62.128999999999998</v>
+      </c>
+      <c r="AD58">
+        <v>0.153</v>
+      </c>
+      <c r="AE58">
+        <v>66.153000000000006</v>
+      </c>
+      <c r="AF58">
+        <v>66.203000000000003</v>
+      </c>
+      <c r="AG58">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AH58">
+        <v>58.222999999999999</v>
+      </c>
+      <c r="AI58">
+        <v>58.268000000000001</v>
+      </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A59">
@@ -19371,7 +19924,105 @@
       <c r="B59">
         <v>2</v>
       </c>
-      <c r="C59" s="3"/>
+      <c r="C59" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59">
+        <v>2616</v>
+      </c>
+      <c r="E59">
+        <v>2878</v>
+      </c>
+      <c r="F59">
+        <v>10</v>
+      </c>
+      <c r="G59">
+        <v>45</v>
+      </c>
+      <c r="H59">
+        <v>15</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="L59">
+        <v>0.108</v>
+      </c>
+      <c r="M59">
+        <v>0.153</v>
+      </c>
+      <c r="N59">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="O59">
+        <v>0.123</v>
+      </c>
+      <c r="P59">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="Q59">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="R59">
+        <v>0.11</v>
+      </c>
+      <c r="S59">
+        <v>0.159</v>
+      </c>
+      <c r="T59">
+        <v>6576</v>
+      </c>
+      <c r="U59">
+        <v>6838</v>
+      </c>
+      <c r="V59">
+        <v>1000</v>
+      </c>
+      <c r="W59">
+        <v>14081</v>
+      </c>
+      <c r="X59">
+        <v>26115</v>
+      </c>
+      <c r="Y59">
+        <v>12065</v>
+      </c>
+      <c r="Z59">
+        <v>0</v>
+      </c>
+      <c r="AA59">
+        <v>0.188</v>
+      </c>
+      <c r="AB59">
+        <v>6.2</v>
+      </c>
+      <c r="AC59">
+        <v>6.2629999999999999</v>
+      </c>
+      <c r="AD59">
+        <v>0.155</v>
+      </c>
+      <c r="AE59">
+        <v>5.8550000000000004</v>
+      </c>
+      <c r="AF59">
+        <v>5.9059999999999997</v>
+      </c>
+      <c r="AG59">
+        <v>0.16</v>
+      </c>
+      <c r="AH59">
+        <v>6.1589999999999998</v>
+      </c>
+      <c r="AI59">
+        <v>6.2160000000000002</v>
+      </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A60">
@@ -19380,7 +20031,105 @@
       <c r="B60">
         <v>3</v>
       </c>
-      <c r="C60" s="3"/>
+      <c r="C60" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60">
+        <v>3994</v>
+      </c>
+      <c r="E60">
+        <v>4393</v>
+      </c>
+      <c r="F60">
+        <v>10</v>
+      </c>
+      <c r="G60">
+        <v>62</v>
+      </c>
+      <c r="H60">
+        <v>15</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60" s="2">
+        <v>0</v>
+      </c>
+      <c r="K60" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="L60" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="M60">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="N60">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="O60">
+        <v>0.161</v>
+      </c>
+      <c r="P60" s="2">
+        <v>0.224</v>
+      </c>
+      <c r="Q60" s="2">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="R60" s="2">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="S60">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="T60">
+        <v>7954</v>
+      </c>
+      <c r="U60">
+        <v>8353</v>
+      </c>
+      <c r="V60">
+        <v>1000</v>
+      </c>
+      <c r="W60">
+        <v>28369</v>
+      </c>
+      <c r="X60">
+        <v>54658</v>
+      </c>
+      <c r="Y60">
+        <v>26336</v>
+      </c>
+      <c r="Z60">
+        <v>0</v>
+      </c>
+      <c r="AA60">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="AB60">
+        <v>12.635999999999999</v>
+      </c>
+      <c r="AC60">
+        <v>12.712999999999999</v>
+      </c>
+      <c r="AD60">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AE60">
+        <v>12.284000000000001</v>
+      </c>
+      <c r="AF60">
+        <v>12.333</v>
+      </c>
+      <c r="AG60">
+        <v>0.153</v>
+      </c>
+      <c r="AH60">
+        <v>12.106</v>
+      </c>
+      <c r="AI60">
+        <v>12.161</v>
+      </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A61">
@@ -19389,12 +20138,105 @@
       <c r="B61">
         <v>3</v>
       </c>
-      <c r="C61" s="3"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
+      <c r="C61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61">
+        <v>3886</v>
+      </c>
+      <c r="E61" s="2">
+        <v>4275</v>
+      </c>
+      <c r="F61" s="2">
+        <v>10</v>
+      </c>
+      <c r="G61" s="2">
+        <v>67</v>
+      </c>
+      <c r="H61" s="2">
+        <v>20</v>
+      </c>
+      <c r="I61" s="2">
+        <v>2</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="L61">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="M61">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="N61">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="O61">
+        <v>0.155</v>
+      </c>
+      <c r="P61">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="Q61">
+        <v>0.157</v>
+      </c>
+      <c r="R61">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="S61">
+        <v>0.19</v>
+      </c>
+      <c r="T61">
+        <v>7846</v>
+      </c>
+      <c r="U61">
+        <v>8235</v>
+      </c>
+      <c r="V61">
+        <v>1000</v>
+      </c>
+      <c r="W61">
+        <v>23166</v>
+      </c>
+      <c r="X61">
+        <v>44246</v>
+      </c>
+      <c r="Y61">
+        <v>21128</v>
+      </c>
+      <c r="Z61">
+        <v>0</v>
+      </c>
+      <c r="AA61">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="AB61">
+        <v>11.249000000000001</v>
+      </c>
+      <c r="AC61">
+        <v>11.298999999999999</v>
+      </c>
+      <c r="AD61">
+        <v>0.158</v>
+      </c>
+      <c r="AE61">
+        <v>9.8379999999999992</v>
+      </c>
+      <c r="AF61">
+        <v>9.89</v>
+      </c>
+      <c r="AG61">
+        <v>0.152</v>
+      </c>
+      <c r="AH61">
+        <v>10.183999999999999</v>
+      </c>
+      <c r="AI61">
+        <v>10.236000000000001</v>
+      </c>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A62">
@@ -19403,7 +20245,105 @@
       <c r="B62">
         <v>3</v>
       </c>
-      <c r="C62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62">
+        <v>3972</v>
+      </c>
+      <c r="E62">
+        <v>4371</v>
+      </c>
+      <c r="F62">
+        <v>10</v>
+      </c>
+      <c r="G62">
+        <v>45</v>
+      </c>
+      <c r="H62">
+        <v>15</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0.255</v>
+      </c>
+      <c r="L62">
+        <v>0.22</v>
+      </c>
+      <c r="M62">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="N62">
+        <v>0.159</v>
+      </c>
+      <c r="O62">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="P62">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="Q62">
+        <v>0.157</v>
+      </c>
+      <c r="R62">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="S62">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="T62">
+        <v>7932</v>
+      </c>
+      <c r="U62">
+        <v>8331</v>
+      </c>
+      <c r="V62">
+        <v>1000</v>
+      </c>
+      <c r="W62">
+        <v>80859</v>
+      </c>
+      <c r="X62">
+        <v>159664</v>
+      </c>
+      <c r="Y62">
+        <v>78839</v>
+      </c>
+      <c r="Z62">
+        <v>0</v>
+      </c>
+      <c r="AA62">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="AB62">
+        <v>30.361000000000001</v>
+      </c>
+      <c r="AC62">
+        <v>30.446000000000002</v>
+      </c>
+      <c r="AD62">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="AE62">
+        <v>30.760999999999999</v>
+      </c>
+      <c r="AF62">
+        <v>30.812000000000001</v>
+      </c>
+      <c r="AG62">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="AH62">
+        <v>28.651</v>
+      </c>
+      <c r="AI62">
+        <v>28.701000000000001</v>
+      </c>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A63">
@@ -19412,10 +20352,105 @@
       <c r="B63">
         <v>4</v>
       </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="C63" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="2">
+        <v>5414</v>
+      </c>
+      <c r="E63" s="2">
+        <v>5955</v>
+      </c>
+      <c r="F63" s="2">
+        <v>10</v>
+      </c>
+      <c r="G63">
+        <v>61</v>
+      </c>
+      <c r="H63">
+        <v>15</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0.251</v>
+      </c>
+      <c r="L63">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="M63">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="N63">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="O63">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="P63">
+        <v>0.252</v>
+      </c>
+      <c r="Q63">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="R63">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="S63">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="T63" s="2">
+        <v>9374</v>
+      </c>
+      <c r="U63" s="2">
+        <v>9915</v>
+      </c>
+      <c r="V63" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W63">
+        <v>5715</v>
+      </c>
+      <c r="X63">
+        <v>9344</v>
+      </c>
+      <c r="Y63">
+        <v>3676</v>
+      </c>
+      <c r="Z63">
+        <v>0</v>
+      </c>
+      <c r="AA63">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="AB63">
+        <v>4.9370000000000003</v>
+      </c>
+      <c r="AC63">
+        <v>5.0309999999999997</v>
+      </c>
+      <c r="AD63">
+        <v>0.155</v>
+      </c>
+      <c r="AE63">
+        <v>4.5359999999999996</v>
+      </c>
+      <c r="AF63">
+        <v>4.5919999999999996</v>
+      </c>
+      <c r="AG63">
+        <v>0.158</v>
+      </c>
+      <c r="AH63">
+        <v>4.5250000000000004</v>
+      </c>
+      <c r="AI63">
+        <v>4.58</v>
+      </c>
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A64">
@@ -19424,7 +20459,105 @@
       <c r="B64">
         <v>4</v>
       </c>
-      <c r="C64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64">
+        <v>5241</v>
+      </c>
+      <c r="E64">
+        <v>5768</v>
+      </c>
+      <c r="F64">
+        <v>10</v>
+      </c>
+      <c r="G64" s="2">
+        <v>82</v>
+      </c>
+      <c r="H64" s="2">
+        <v>17</v>
+      </c>
+      <c r="I64" s="2">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0.158</v>
+      </c>
+      <c r="L64">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="M64">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="N64">
+        <v>0.157</v>
+      </c>
+      <c r="O64">
+        <v>0.18</v>
+      </c>
+      <c r="P64">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="Q64">
+        <v>0.158</v>
+      </c>
+      <c r="R64">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="S64">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="T64">
+        <v>9201</v>
+      </c>
+      <c r="U64">
+        <v>9728</v>
+      </c>
+      <c r="V64">
+        <v>1000</v>
+      </c>
+      <c r="W64">
+        <v>105867</v>
+      </c>
+      <c r="X64">
+        <v>209616</v>
+      </c>
+      <c r="Y64">
+        <v>103818</v>
+      </c>
+      <c r="Z64">
+        <v>0</v>
+      </c>
+      <c r="AA64">
+        <v>0.158</v>
+      </c>
+      <c r="AB64">
+        <v>44.368000000000002</v>
+      </c>
+      <c r="AC64">
+        <v>44.424999999999997</v>
+      </c>
+      <c r="AD64">
+        <v>0.161</v>
+      </c>
+      <c r="AE64">
+        <v>47.392000000000003</v>
+      </c>
+      <c r="AF64">
+        <v>47.451000000000001</v>
+      </c>
+      <c r="AG64">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="AH64">
+        <v>44.865000000000002</v>
+      </c>
+      <c r="AI64">
+        <v>44.923999999999999</v>
+      </c>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A65">
@@ -19433,7 +20566,105 @@
       <c r="B65">
         <v>4</v>
       </c>
-      <c r="C65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65">
+        <v>5291</v>
+      </c>
+      <c r="E65">
+        <v>5828</v>
+      </c>
+      <c r="F65">
+        <v>10</v>
+      </c>
+      <c r="G65">
+        <v>91</v>
+      </c>
+      <c r="H65">
+        <v>15</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="L65">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="M65">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="N65">
+        <v>0.156</v>
+      </c>
+      <c r="O65">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="P65">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="Q65">
+        <v>0.183</v>
+      </c>
+      <c r="R65">
+        <v>0.252</v>
+      </c>
+      <c r="S65">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="T65">
+        <v>9251</v>
+      </c>
+      <c r="U65">
+        <v>9788</v>
+      </c>
+      <c r="V65">
+        <v>1000</v>
+      </c>
+      <c r="W65">
+        <v>30823</v>
+      </c>
+      <c r="X65">
+        <v>59504</v>
+      </c>
+      <c r="Y65">
+        <v>28757</v>
+      </c>
+      <c r="Z65">
+        <v>0</v>
+      </c>
+      <c r="AA65">
+        <v>0.155</v>
+      </c>
+      <c r="AB65">
+        <v>18.401</v>
+      </c>
+      <c r="AC65">
+        <v>18.457000000000001</v>
+      </c>
+      <c r="AD65">
+        <v>0.16</v>
+      </c>
+      <c r="AE65">
+        <v>13.629</v>
+      </c>
+      <c r="AF65">
+        <v>13.689</v>
+      </c>
+      <c r="AG65">
+        <v>0.152</v>
+      </c>
+      <c r="AH65">
+        <v>13.895</v>
+      </c>
+      <c r="AI65">
+        <v>13.951000000000001</v>
+      </c>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A66">
@@ -19442,7 +20673,105 @@
       <c r="B66">
         <v>5</v>
       </c>
-      <c r="C66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D66">
+        <v>6561</v>
+      </c>
+      <c r="E66">
+        <v>7225</v>
+      </c>
+      <c r="F66">
+        <v>10</v>
+      </c>
+      <c r="G66">
+        <v>122</v>
+      </c>
+      <c r="H66">
+        <v>29</v>
+      </c>
+      <c r="I66">
+        <v>7</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="L66">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="M66">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="N66">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="O66">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="P66">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="Q66">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="R66">
+        <v>0.217</v>
+      </c>
+      <c r="S66">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="T66">
+        <v>10521</v>
+      </c>
+      <c r="U66">
+        <v>11185</v>
+      </c>
+      <c r="V66">
+        <v>1000</v>
+      </c>
+      <c r="W66">
+        <v>16150</v>
+      </c>
+      <c r="X66">
+        <v>30116</v>
+      </c>
+      <c r="Y66">
+        <v>14066</v>
+      </c>
+      <c r="Z66">
+        <v>0</v>
+      </c>
+      <c r="AA66">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="AB66">
+        <v>10.276999999999999</v>
+      </c>
+      <c r="AC66">
+        <v>10.336</v>
+      </c>
+      <c r="AD66">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="AE66">
+        <v>10.757</v>
+      </c>
+      <c r="AF66">
+        <v>10.818</v>
+      </c>
+      <c r="AG66">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="AH66">
+        <v>10.336</v>
+      </c>
+      <c r="AI66">
+        <v>10.4</v>
+      </c>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A67">
@@ -19451,12 +20780,105 @@
       <c r="B67">
         <v>5</v>
       </c>
-      <c r="C67" s="3"/>
-      <c r="T67" s="2"/>
-      <c r="U67" s="2"/>
-      <c r="V67" s="2"/>
-      <c r="X67" s="2"/>
-      <c r="Y67" s="2"/>
+      <c r="C67" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67">
+        <v>6696</v>
+      </c>
+      <c r="E67">
+        <v>7372</v>
+      </c>
+      <c r="F67">
+        <v>10</v>
+      </c>
+      <c r="G67">
+        <v>110</v>
+      </c>
+      <c r="H67">
+        <v>15</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0.2</v>
+      </c>
+      <c r="L67">
+        <v>0.312</v>
+      </c>
+      <c r="M67">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="N67">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="O67">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="P67">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="Q67">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="R67">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="S67">
+        <v>0.33</v>
+      </c>
+      <c r="T67" s="2">
+        <v>10656</v>
+      </c>
+      <c r="U67" s="2">
+        <v>11332</v>
+      </c>
+      <c r="V67" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W67">
+        <v>43420</v>
+      </c>
+      <c r="X67" s="2">
+        <v>84661</v>
+      </c>
+      <c r="Y67" s="2">
+        <v>41334</v>
+      </c>
+      <c r="Z67">
+        <v>0</v>
+      </c>
+      <c r="AA67">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="AB67">
+        <v>27.222999999999999</v>
+      </c>
+      <c r="AC67">
+        <v>27.317</v>
+      </c>
+      <c r="AD67">
+        <v>0.183</v>
+      </c>
+      <c r="AE67">
+        <v>28.472999999999999</v>
+      </c>
+      <c r="AF67">
+        <v>28.545999999999999</v>
+      </c>
+      <c r="AG67">
+        <v>0.185</v>
+      </c>
+      <c r="AH67">
+        <v>23.079000000000001</v>
+      </c>
+      <c r="AI67">
+        <v>23.146000000000001</v>
+      </c>
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A68">
@@ -19465,13 +20887,105 @@
       <c r="B68">
         <v>5</v>
       </c>
-      <c r="C68" s="3"/>
-      <c r="T68" s="2"/>
-      <c r="U68" s="2"/>
-      <c r="V68" s="2"/>
-      <c r="AA68" s="2"/>
-      <c r="AB68" s="2"/>
-      <c r="AC68" s="2"/>
+      <c r="C68" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68">
+        <v>6475</v>
+      </c>
+      <c r="E68">
+        <v>7136</v>
+      </c>
+      <c r="F68">
+        <v>10</v>
+      </c>
+      <c r="G68">
+        <v>80</v>
+      </c>
+      <c r="H68">
+        <v>18</v>
+      </c>
+      <c r="I68">
+        <v>2</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0.182</v>
+      </c>
+      <c r="L68">
+        <v>0.23</v>
+      </c>
+      <c r="M68">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="N68">
+        <v>0.17</v>
+      </c>
+      <c r="O68">
+        <v>0.215</v>
+      </c>
+      <c r="P68">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="Q68">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="R68">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="S68">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="T68" s="2">
+        <v>10435</v>
+      </c>
+      <c r="U68" s="2">
+        <v>11096</v>
+      </c>
+      <c r="V68" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W68">
+        <v>38334</v>
+      </c>
+      <c r="X68">
+        <v>74561</v>
+      </c>
+      <c r="Y68">
+        <v>36291</v>
+      </c>
+      <c r="Z68">
+        <v>0</v>
+      </c>
+      <c r="AA68" s="2">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="AB68" s="2">
+        <v>22.896999999999998</v>
+      </c>
+      <c r="AC68" s="2">
+        <v>22.959</v>
+      </c>
+      <c r="AD68">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="AE68">
+        <v>22.84</v>
+      </c>
+      <c r="AF68">
+        <v>22.901</v>
+      </c>
+      <c r="AG68">
+        <v>0.158</v>
+      </c>
+      <c r="AH68">
+        <v>21.071999999999999</v>
+      </c>
+      <c r="AI68">
+        <v>21.129000000000001</v>
+      </c>
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">

</xml_diff>

<commit_message>
Updating tests summary for Heuristic 3 + 80.
</commit_message>
<xml_diff>
--- a/docs/testsFSG/tests-summary.xlsx
+++ b/docs/testsFSG/tests-summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8232" windowHeight="4296" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8232" windowHeight="4296"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="85">
   <si>
     <t>Run</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Features: 80, Heuristic 3: Default + BiVarArithmetic + OrAttr0 + OrAttr1</t>
   </si>
   <si>
-    <t>Features: 80, Heuristic 4: Default + OrAttr0 + OrAttr1</t>
-  </si>
-  <si>
     <t>0, 19</t>
   </si>
   <si>
@@ -371,7 +368,34 @@
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2117,6 +2141,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.3752656488276206E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13285316265553723</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16262414002527026</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22716082133096244</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24044982172616361</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2678,6 +2717,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.36655533021610098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.063730824790003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.441589155109996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6598031875659505</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.79035970925041</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5110,13 +5164,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>601133</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>169333</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>296333</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>118533</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>135467</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5139,14 +5193,14 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>440266</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>8467</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>25401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>135466</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>143934</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>160868</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5236,17 +5290,105 @@
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'40 - Models'!$B$2*'40 - Models'!$B$6*Table4[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table4[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="18"/>
-    <tableColumn id="3" name="Heuristic 1" dataDxfId="17"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="16"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="15"/>
-    <tableColumn id="7" name="Heuristic 4" dataDxfId="14"/>
+    <tableColumn id="2" name="Default" dataDxfId="27"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="26"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="25"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="24"/>
+    <tableColumn id="7" name="Heuristic 4" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1437" displayName="Table1437" ref="A74:AI89" totalsRowShown="0" dataCellStyle="Normal">
+  <autoFilter ref="A74:AI89"/>
+  <tableColumns count="35">
+    <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
+    <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
+    <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
+    <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
+    <tableColumn id="34" name="Nodes5" dataCellStyle="Normal"/>
+    <tableColumn id="33" name="Backtracks6" dataCellStyle="Normal"/>
+    <tableColumn id="32" name="Fails7" dataCellStyle="Normal"/>
+    <tableColumn id="29" name="Restarts8" dataCellStyle="Normal"/>
+    <tableColumn id="20" name="Building Time3" dataCellStyle="Normal"/>
+    <tableColumn id="21" name="Resolution Time2" dataCellStyle="Normal"/>
+    <tableColumn id="22" name="Execution Time2" dataCellStyle="Normal"/>
+    <tableColumn id="23" name="Building Time32" dataCellStyle="Normal"/>
+    <tableColumn id="24" name="Resolution Time23" dataCellStyle="Normal"/>
+    <tableColumn id="25" name="Execution Time24" dataCellStyle="Normal"/>
+    <tableColumn id="26" name="Building Time33" dataCellStyle="Normal"/>
+    <tableColumn id="27" name="Resolution Time24" dataCellStyle="Normal"/>
+    <tableColumn id="28" name="Execution Time25" dataCellStyle="Normal"/>
+    <tableColumn id="37" name="Variables3" dataCellStyle="Normal"/>
+    <tableColumn id="38" name="Constraints4" dataCellStyle="Normal"/>
+    <tableColumn id="39" name="Solutions5" dataCellStyle="Normal"/>
+    <tableColumn id="40" name="Nodes6" dataCellStyle="Normal"/>
+    <tableColumn id="41" name="Backtracks7" dataCellStyle="Normal"/>
+    <tableColumn id="42" name="Fails8" dataCellStyle="Normal"/>
+    <tableColumn id="43" name="Restarts9" dataCellStyle="Normal"/>
+    <tableColumn id="44" name="Building Time10" dataCellStyle="Normal"/>
+    <tableColumn id="45" name="Resolution Time11" dataCellStyle="Normal"/>
+    <tableColumn id="46" name="Execution Time12" dataCellStyle="Normal"/>
+    <tableColumn id="47" name="Building Time213" dataCellStyle="Normal"/>
+    <tableColumn id="48" name="Resolution Time314" dataCellStyle="Normal"/>
+    <tableColumn id="49" name="Execution Time415" dataCellStyle="Normal"/>
+    <tableColumn id="50" name="Building Time516" dataCellStyle="Normal"/>
+    <tableColumn id="51" name="Resolution Time617" dataCellStyle="Normal"/>
+    <tableColumn id="52" name="Execution Time718" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14378" displayName="Table14378" ref="A95:AI110" totalsRowShown="0" dataCellStyle="Normal">
+  <autoFilter ref="A95:AI110"/>
+  <tableColumns count="35">
+    <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
+    <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
+    <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
+    <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
+    <tableColumn id="34" name="Nodes5" dataCellStyle="Normal"/>
+    <tableColumn id="33" name="Backtracks6" dataCellStyle="Normal"/>
+    <tableColumn id="32" name="Fails7" dataCellStyle="Normal"/>
+    <tableColumn id="29" name="Restarts8" dataCellStyle="Normal"/>
+    <tableColumn id="20" name="Building Time3" dataCellStyle="Normal"/>
+    <tableColumn id="21" name="Resolution Time2" dataCellStyle="Normal"/>
+    <tableColumn id="22" name="Execution Time2" dataCellStyle="Normal"/>
+    <tableColumn id="23" name="Building Time32" dataCellStyle="Normal"/>
+    <tableColumn id="24" name="Resolution Time23" dataCellStyle="Normal"/>
+    <tableColumn id="25" name="Execution Time24" dataCellStyle="Normal"/>
+    <tableColumn id="26" name="Building Time33" dataCellStyle="Normal"/>
+    <tableColumn id="27" name="Resolution Time24" dataCellStyle="Normal"/>
+    <tableColumn id="28" name="Execution Time25" dataCellStyle="Normal"/>
+    <tableColumn id="37" name="Variables3" dataCellStyle="Normal"/>
+    <tableColumn id="38" name="Constraints4" dataCellStyle="Normal"/>
+    <tableColumn id="39" name="Solutions5" dataCellStyle="Normal"/>
+    <tableColumn id="40" name="Nodes6" dataCellStyle="Normal"/>
+    <tableColumn id="41" name="Backtracks7" dataCellStyle="Normal"/>
+    <tableColumn id="42" name="Fails8" dataCellStyle="Normal"/>
+    <tableColumn id="43" name="Restarts9" dataCellStyle="Normal"/>
+    <tableColumn id="44" name="Building Time10" dataCellStyle="Normal"/>
+    <tableColumn id="45" name="Resolution Time11" dataCellStyle="Normal"/>
+    <tableColumn id="46" name="Execution Time12" dataCellStyle="Normal"/>
+    <tableColumn id="47" name="Building Time213" dataCellStyle="Normal"/>
+    <tableColumn id="48" name="Resolution Time314" dataCellStyle="Normal"/>
+    <tableColumn id="49" name="Execution Time415" dataCellStyle="Normal"/>
+    <tableColumn id="50" name="Building Time516" dataCellStyle="Normal"/>
+    <tableColumn id="51" name="Resolution Time617" dataCellStyle="Normal"/>
+    <tableColumn id="52" name="Execution Time718" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table19" displayName="Table19" ref="A11:AI26" totalsRowShown="0" dataCellStyle="Normal">
   <autoFilter ref="A11:AI26"/>
   <tableColumns count="35">
@@ -5290,101 +5432,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1410" displayName="Table1410" ref="A32:AI47" totalsRowShown="0" dataCellStyle="Normal">
   <autoFilter ref="A32:AI47"/>
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
-    <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
-    <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
-    <tableColumn id="34" name="Nodes5" dataCellStyle="Normal"/>
-    <tableColumn id="33" name="Backtracks6" dataCellStyle="Normal"/>
-    <tableColumn id="32" name="Fails7" dataCellStyle="Normal"/>
-    <tableColumn id="29" name="Restarts8" dataCellStyle="Normal"/>
-    <tableColumn id="20" name="Building Time3" dataCellStyle="Normal"/>
-    <tableColumn id="21" name="Resolution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="22" name="Execution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="23" name="Building Time32" dataCellStyle="Normal"/>
-    <tableColumn id="24" name="Resolution Time23" dataCellStyle="Normal"/>
-    <tableColumn id="25" name="Execution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="26" name="Building Time33" dataCellStyle="Normal"/>
-    <tableColumn id="27" name="Resolution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="28" name="Execution Time25" dataCellStyle="Normal"/>
-    <tableColumn id="37" name="Variables3" dataCellStyle="Normal"/>
-    <tableColumn id="38" name="Constraints4" dataCellStyle="Normal"/>
-    <tableColumn id="39" name="Solutions5" dataCellStyle="Normal"/>
-    <tableColumn id="40" name="Nodes6" dataCellStyle="Normal"/>
-    <tableColumn id="41" name="Backtracks7" dataCellStyle="Normal"/>
-    <tableColumn id="42" name="Fails8" dataCellStyle="Normal"/>
-    <tableColumn id="43" name="Restarts9" dataCellStyle="Normal"/>
-    <tableColumn id="44" name="Building Time10" dataCellStyle="Normal"/>
-    <tableColumn id="45" name="Resolution Time11" dataCellStyle="Normal"/>
-    <tableColumn id="46" name="Execution Time12" dataCellStyle="Normal"/>
-    <tableColumn id="47" name="Building Time213" dataCellStyle="Normal"/>
-    <tableColumn id="48" name="Resolution Time314" dataCellStyle="Normal"/>
-    <tableColumn id="49" name="Execution Time415" dataCellStyle="Normal"/>
-    <tableColumn id="50" name="Building Time516" dataCellStyle="Normal"/>
-    <tableColumn id="51" name="Resolution Time617" dataCellStyle="Normal"/>
-    <tableColumn id="52" name="Execution Time718" dataCellStyle="Normal"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table14311" displayName="Table14311" ref="A53:AI68" totalsRowShown="0" dataCellStyle="Normal">
-  <autoFilter ref="A53:AI68"/>
-  <tableColumns count="35">
-    <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
-    <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
-    <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
-    <tableColumn id="34" name="Nodes5" dataCellStyle="Normal"/>
-    <tableColumn id="33" name="Backtracks6" dataCellStyle="Normal"/>
-    <tableColumn id="32" name="Fails7" dataCellStyle="Normal"/>
-    <tableColumn id="29" name="Restarts8" dataCellStyle="Normal"/>
-    <tableColumn id="20" name="Building Time3" dataCellStyle="Normal"/>
-    <tableColumn id="21" name="Resolution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="22" name="Execution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="23" name="Building Time32" dataCellStyle="Normal"/>
-    <tableColumn id="24" name="Resolution Time23" dataCellStyle="Normal"/>
-    <tableColumn id="25" name="Execution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="26" name="Building Time33" dataCellStyle="Normal"/>
-    <tableColumn id="27" name="Resolution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="28" name="Execution Time25" dataCellStyle="Normal"/>
-    <tableColumn id="37" name="Variables3" dataCellStyle="Normal"/>
-    <tableColumn id="38" name="Constraints4" dataCellStyle="Normal"/>
-    <tableColumn id="39" name="Solutions5" dataCellStyle="Normal"/>
-    <tableColumn id="40" name="Nodes6" dataCellStyle="Normal"/>
-    <tableColumn id="41" name="Backtracks7" dataCellStyle="Normal"/>
-    <tableColumn id="42" name="Fails8" dataCellStyle="Normal"/>
-    <tableColumn id="43" name="Restarts9" dataCellStyle="Normal"/>
-    <tableColumn id="44" name="Building Time10" dataCellStyle="Normal"/>
-    <tableColumn id="45" name="Resolution Time11" dataCellStyle="Normal"/>
-    <tableColumn id="46" name="Execution Time12" dataCellStyle="Normal"/>
-    <tableColumn id="47" name="Building Time213" dataCellStyle="Normal"/>
-    <tableColumn id="48" name="Resolution Time314" dataCellStyle="Normal"/>
-    <tableColumn id="49" name="Execution Time415" dataCellStyle="Normal"/>
-    <tableColumn id="50" name="Building Time516" dataCellStyle="Normal"/>
-    <tableColumn id="51" name="Resolution Time617" dataCellStyle="Normal"/>
-    <tableColumn id="52" name="Execution Time718" dataCellStyle="Normal"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table143712" displayName="Table143712" ref="A74:AI89" totalsRowShown="0" dataCellStyle="Normal">
-  <autoFilter ref="A74:AI89"/>
-  <tableColumns count="35">
-    <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="10" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -5423,12 +5477,56 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1437813" displayName="Table1437813" ref="A95:AI110" totalsRowShown="0" dataCellStyle="Normal">
-  <autoFilter ref="A95:AI110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table14311" displayName="Table14311" ref="A53:AI68" totalsRowShown="0" dataCellStyle="Normal">
+  <autoFilter ref="A53:AI68"/>
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
+    <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
+    <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
+    <tableColumn id="34" name="Nodes5" dataCellStyle="Normal"/>
+    <tableColumn id="33" name="Backtracks6" dataCellStyle="Normal"/>
+    <tableColumn id="32" name="Fails7" dataCellStyle="Normal"/>
+    <tableColumn id="29" name="Restarts8" dataCellStyle="Normal"/>
+    <tableColumn id="20" name="Building Time3" dataCellStyle="Normal"/>
+    <tableColumn id="21" name="Resolution Time2" dataCellStyle="Normal"/>
+    <tableColumn id="22" name="Execution Time2" dataCellStyle="Normal"/>
+    <tableColumn id="23" name="Building Time32" dataCellStyle="Normal"/>
+    <tableColumn id="24" name="Resolution Time23" dataCellStyle="Normal"/>
+    <tableColumn id="25" name="Execution Time24" dataCellStyle="Normal"/>
+    <tableColumn id="26" name="Building Time33" dataCellStyle="Normal"/>
+    <tableColumn id="27" name="Resolution Time24" dataCellStyle="Normal"/>
+    <tableColumn id="28" name="Execution Time25" dataCellStyle="Normal"/>
+    <tableColumn id="37" name="Variables3" dataCellStyle="Normal"/>
+    <tableColumn id="38" name="Constraints4" dataCellStyle="Normal"/>
+    <tableColumn id="39" name="Solutions5" dataCellStyle="Normal"/>
+    <tableColumn id="40" name="Nodes6" dataCellStyle="Normal"/>
+    <tableColumn id="41" name="Backtracks7" dataCellStyle="Normal"/>
+    <tableColumn id="42" name="Fails8" dataCellStyle="Normal"/>
+    <tableColumn id="43" name="Restarts9" dataCellStyle="Normal"/>
+    <tableColumn id="44" name="Building Time10" dataCellStyle="Normal"/>
+    <tableColumn id="45" name="Resolution Time11" dataCellStyle="Normal"/>
+    <tableColumn id="46" name="Execution Time12" dataCellStyle="Normal"/>
+    <tableColumn id="47" name="Building Time213" dataCellStyle="Normal"/>
+    <tableColumn id="48" name="Resolution Time314" dataCellStyle="Normal"/>
+    <tableColumn id="49" name="Execution Time415" dataCellStyle="Normal"/>
+    <tableColumn id="50" name="Building Time516" dataCellStyle="Normal"/>
+    <tableColumn id="51" name="Resolution Time617" dataCellStyle="Normal"/>
+    <tableColumn id="52" name="Execution Time718" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table143712" displayName="Table143712" ref="A74:AI89" totalsRowShown="0" dataCellStyle="Normal">
+  <autoFilter ref="A74:AI89"/>
+  <tableColumns count="35">
+    <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="8" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -5474,11 +5572,11 @@
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'40 - Models'!$B$2*'40 - Models'!$B$6*Table5[[#This Row],[Models]]+'40 - Models'!$B$2*'40 - Models'!$B$3*Table5[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="13"/>
+    <tableColumn id="2" name="Default" dataDxfId="22"/>
     <tableColumn id="3" name="Heuristic 1"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="12"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="11"/>
-    <tableColumn id="7" name="Heuristic 4" dataDxfId="10"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="21"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="20"/>
+    <tableColumn id="7" name="Heuristic 4" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5492,10 +5590,10 @@
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'80 - Models'!$B$2*'80 - Models'!$B$6*Table414[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table414[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="9"/>
-    <tableColumn id="3" name="Heuristic 1" dataDxfId="8"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="7"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="6"/>
+    <tableColumn id="2" name="Default" dataDxfId="18"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="17"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="16"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5509,16 +5607,46 @@
     <tableColumn id="6" name="Constraints">
       <calculatedColumnFormula>'80 - Models'!$B$2*'80 - Models'!$B$6*Table41415[[#This Row],[Models]]+'80 - Models'!$B$2*'80 - Models'!$B$3*Table41415[[#This Row],[Models]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Default" dataDxfId="5"/>
-    <tableColumn id="3" name="Heuristic 1" dataDxfId="4"/>
-    <tableColumn id="4" name="Heuristic 2" dataDxfId="3"/>
-    <tableColumn id="5" name="Heuristic 3" dataDxfId="2"/>
+    <tableColumn id="2" name="Default" dataDxfId="14"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="13"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="12"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table41413" displayName="Table41413" ref="A39:F44" totalsRowShown="0">
+  <autoFilter ref="A39:F44"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Models"/>
+    <tableColumn id="6" name="Constraints"/>
+    <tableColumn id="2" name="Default" dataDxfId="7"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="6"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="5"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table4141516" displayName="Table4141516" ref="A48:F53" totalsRowShown="0">
+  <autoFilter ref="A48:F53"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Models"/>
+    <tableColumn id="6" name="Constraints"/>
+    <tableColumn id="2" name="Default" dataDxfId="3"/>
+    <tableColumn id="3" name="Heuristic 1" dataDxfId="2"/>
+    <tableColumn id="4" name="Heuristic 2" dataDxfId="1"/>
+    <tableColumn id="5" name="Heuristic 3" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A11:AI26" totalsRowShown="0" dataCellStyle="Normal">
   <autoFilter ref="A11:AI26"/>
   <tableColumns count="35">
@@ -5562,7 +5690,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A32:AI47" totalsRowShown="0" dataCellStyle="Normal">
   <autoFilter ref="A32:AI47"/>
   <tableColumns count="35">
@@ -5606,97 +5734,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="A53:AI68" totalsRowShown="0" dataCellStyle="Normal">
   <autoFilter ref="A53:AI68"/>
-  <tableColumns count="35">
-    <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
-    <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
-    <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
-    <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
-    <tableColumn id="34" name="Nodes5" dataCellStyle="Normal"/>
-    <tableColumn id="33" name="Backtracks6" dataCellStyle="Normal"/>
-    <tableColumn id="32" name="Fails7" dataCellStyle="Normal"/>
-    <tableColumn id="29" name="Restarts8" dataCellStyle="Normal"/>
-    <tableColumn id="20" name="Building Time3" dataCellStyle="Normal"/>
-    <tableColumn id="21" name="Resolution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="22" name="Execution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="23" name="Building Time32" dataCellStyle="Normal"/>
-    <tableColumn id="24" name="Resolution Time23" dataCellStyle="Normal"/>
-    <tableColumn id="25" name="Execution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="26" name="Building Time33" dataCellStyle="Normal"/>
-    <tableColumn id="27" name="Resolution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="28" name="Execution Time25" dataCellStyle="Normal"/>
-    <tableColumn id="37" name="Variables3" dataCellStyle="Normal"/>
-    <tableColumn id="38" name="Constraints4" dataCellStyle="Normal"/>
-    <tableColumn id="39" name="Solutions5" dataCellStyle="Normal"/>
-    <tableColumn id="40" name="Nodes6" dataCellStyle="Normal"/>
-    <tableColumn id="41" name="Backtracks7" dataCellStyle="Normal"/>
-    <tableColumn id="42" name="Fails8" dataCellStyle="Normal"/>
-    <tableColumn id="43" name="Restarts9" dataCellStyle="Normal"/>
-    <tableColumn id="44" name="Building Time10" dataCellStyle="Normal"/>
-    <tableColumn id="45" name="Resolution Time11" dataCellStyle="Normal"/>
-    <tableColumn id="46" name="Execution Time12" dataCellStyle="Normal"/>
-    <tableColumn id="47" name="Building Time213" dataCellStyle="Normal"/>
-    <tableColumn id="48" name="Resolution Time314" dataCellStyle="Normal"/>
-    <tableColumn id="49" name="Execution Time415" dataCellStyle="Normal"/>
-    <tableColumn id="50" name="Building Time516" dataCellStyle="Normal"/>
-    <tableColumn id="51" name="Resolution Time617" dataCellStyle="Normal"/>
-    <tableColumn id="52" name="Execution Time718" dataCellStyle="Normal"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1437" displayName="Table1437" ref="A74:AI89" totalsRowShown="0" dataCellStyle="Normal">
-  <autoFilter ref="A74:AI89"/>
-  <tableColumns count="35">
-    <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataCellStyle="Normal"/>
-    <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
-    <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
-    <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
-    <tableColumn id="34" name="Nodes5" dataCellStyle="Normal"/>
-    <tableColumn id="33" name="Backtracks6" dataCellStyle="Normal"/>
-    <tableColumn id="32" name="Fails7" dataCellStyle="Normal"/>
-    <tableColumn id="29" name="Restarts8" dataCellStyle="Normal"/>
-    <tableColumn id="20" name="Building Time3" dataCellStyle="Normal"/>
-    <tableColumn id="21" name="Resolution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="22" name="Execution Time2" dataCellStyle="Normal"/>
-    <tableColumn id="23" name="Building Time32" dataCellStyle="Normal"/>
-    <tableColumn id="24" name="Resolution Time23" dataCellStyle="Normal"/>
-    <tableColumn id="25" name="Execution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="26" name="Building Time33" dataCellStyle="Normal"/>
-    <tableColumn id="27" name="Resolution Time24" dataCellStyle="Normal"/>
-    <tableColumn id="28" name="Execution Time25" dataCellStyle="Normal"/>
-    <tableColumn id="37" name="Variables3" dataCellStyle="Normal"/>
-    <tableColumn id="38" name="Constraints4" dataCellStyle="Normal"/>
-    <tableColumn id="39" name="Solutions5" dataCellStyle="Normal"/>
-    <tableColumn id="40" name="Nodes6" dataCellStyle="Normal"/>
-    <tableColumn id="41" name="Backtracks7" dataCellStyle="Normal"/>
-    <tableColumn id="42" name="Fails8" dataCellStyle="Normal"/>
-    <tableColumn id="43" name="Restarts9" dataCellStyle="Normal"/>
-    <tableColumn id="44" name="Building Time10" dataCellStyle="Normal"/>
-    <tableColumn id="45" name="Resolution Time11" dataCellStyle="Normal"/>
-    <tableColumn id="46" name="Execution Time12" dataCellStyle="Normal"/>
-    <tableColumn id="47" name="Building Time213" dataCellStyle="Normal"/>
-    <tableColumn id="48" name="Resolution Time314" dataCellStyle="Normal"/>
-    <tableColumn id="49" name="Execution Time415" dataCellStyle="Normal"/>
-    <tableColumn id="50" name="Building Time516" dataCellStyle="Normal"/>
-    <tableColumn id="51" name="Resolution Time617" dataCellStyle="Normal"/>
-    <tableColumn id="52" name="Execution Time718" dataCellStyle="Normal"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14378" displayName="Table14378" ref="A95:AI110" totalsRowShown="0" dataCellStyle="Normal">
-  <autoFilter ref="A95:AI110"/>
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
@@ -6001,10 +6041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6390,7 +6430,10 @@
         <f>HARMEAN('80 - Models'!L54:L56,'80 - Models'!O54:O56,'80 - Models'!R54:R56)</f>
         <v>8.4403439720453305E-2</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="7">
+        <f>HARMEAN('80 - Models'!L75:L77,'80 - Models'!O75:O77,'80 - Models'!R75:R77)</f>
+        <v>8.3752656488276206E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -6412,7 +6455,10 @@
         <f>HARMEAN('80 - Models'!L57:L59,'80 - Models'!O57:O59,'80 - Models'!R57:R59)</f>
         <v>0.12747786209302864</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7">
+        <f>HARMEAN('80 - Models'!L78:L80,'80 - Models'!O78:O80,'80 - Models'!R78:R80)</f>
+        <v>0.13285316265553723</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -6434,7 +6480,10 @@
         <f>HARMEAN('80 - Models'!L60:L62,'80 - Models'!O60:O62,'80 - Models'!R60:R62)</f>
         <v>0.16365266899139061</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7">
+        <f>HARMEAN('80 - Models'!L81:L83,'80 - Models'!O81:O83,'80 - Models'!R81:R83)</f>
+        <v>0.16262414002527026</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -6456,7 +6505,10 @@
         <f>HARMEAN('80 - Models'!L63:L65,'80 - Models'!O63:O65,'80 - Models'!R63:R65)</f>
         <v>0.20252825777913985</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7">
+        <f>HARMEAN('80 - Models'!L84:L86,'80 - Models'!O84:O86,'80 - Models'!R84:R86)</f>
+        <v>0.22716082133096244</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -6478,7 +6530,10 @@
         <f>HARMEAN('80 - Models'!L66:L68,'80 - Models'!O66:O68,'80 - Models'!R66:R68)</f>
         <v>0.23397925761994948</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <f>HARMEAN('80 - Models'!L87:L89,'80 - Models'!O87:O89,'80 - Models'!R87:R89)</f>
+        <v>0.24044982172616361</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -6520,7 +6575,10 @@
         <f>HARMEAN('80 - Models'!AB54:AB56,'80 - Models'!AE54:AE56,'80 - Models'!AH54:AH56)</f>
         <v>0.30892749190503238</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7">
+        <f>HARMEAN('80 - Models'!AB75:AB77,'80 - Models'!AE75:AE77,'80 - Models'!AH75:AH77)</f>
+        <v>0.36655533021610098</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -6542,7 +6600,10 @@
         <f>HARMEAN('80 - Models'!AB57:AB59,'80 - Models'!AE57:AE59,'80 - Models'!AH57:AH59)</f>
         <v>14.89973204291565</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="7">
+        <f>HARMEAN('80 - Models'!AB78:AB80,'80 - Models'!AE78:AE80,'80 - Models'!AH78:AH80)</f>
+        <v>15.063730824790003</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -6564,7 +6625,10 @@
         <f>HARMEAN('80 - Models'!AB60:AB62,'80 - Models'!AE60:AE62,'80 - Models'!AH60:AH62)</f>
         <v>14.235223571130939</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7">
+        <f>HARMEAN('80 - Models'!AB81:AB83,'80 - Models'!AE81:AE83,'80 - Models'!AH81:AH83)</f>
+        <v>14.441589155109996</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
@@ -6586,7 +6650,10 @@
         <f>HARMEAN('80 - Models'!AB63:AB65,'80 - Models'!AE63:AE65,'80 - Models'!AH63:AH65)</f>
         <v>9.8942436050518818</v>
       </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7">
+        <f>HARMEAN('80 - Models'!AB84:AB86,'80 - Models'!AE84:AE86,'80 - Models'!AH84:AH86)</f>
+        <v>9.6598031875659505</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -6608,16 +6675,151 @@
         <f>HARMEAN('80 - Models'!AB66:AB68,'80 - Models'!AE66:AE68,'80 - Models'!AH66:AH68)</f>
         <v>16.756228717733677</v>
       </c>
-      <c r="F34" s="7"/>
+      <c r="F34" s="7">
+        <f>HARMEAN('80 - Models'!AB87:AB89,'80 - Models'!AE87:AE89,'80 - Models'!AH87:AH89)</f>
+        <v>16.79035970925041</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -15621,10 +15823,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI110"/>
+  <dimension ref="A1:AI89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
-      <selection activeCell="V56" sqref="V56"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16278,7 +16480,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16">
         <v>2658</v>
@@ -16385,7 +16587,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17">
         <v>2616</v>
@@ -16492,7 +16694,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18">
         <v>3994</v>
@@ -16813,7 +17015,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21">
         <v>5414</v>
@@ -16920,7 +17122,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22">
         <v>5241</v>
@@ -17134,7 +17336,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24">
         <v>6561</v>
@@ -17241,7 +17443,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25">
         <v>6696</v>
@@ -17348,7 +17550,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26">
         <v>6475</v>
@@ -18048,7 +18250,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D37">
         <v>2658</v>
@@ -18155,7 +18357,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38">
         <v>2616</v>
@@ -18262,7 +18464,7 @@
         <v>3</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D39">
         <v>3994</v>
@@ -18583,7 +18785,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42">
         <v>5414</v>
@@ -18690,7 +18892,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D43">
         <v>5241</v>
@@ -18904,7 +19106,7 @@
         <v>5</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D45">
         <v>6561</v>
@@ -19011,7 +19213,7 @@
         <v>5</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D46">
         <v>6696</v>
@@ -19118,7 +19320,7 @@
         <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D47">
         <v>6475</v>
@@ -19818,7 +20020,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D58">
         <v>2658</v>
@@ -19925,7 +20127,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D59">
         <v>2616</v>
@@ -20032,7 +20234,7 @@
         <v>3</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D60">
         <v>3994</v>
@@ -20353,7 +20555,7 @@
         <v>4</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D63" s="2">
         <v>5414</v>
@@ -20460,7 +20662,7 @@
         <v>4</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D64">
         <v>5241</v>
@@ -20674,7 +20876,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D66">
         <v>6561</v>
@@ -20781,7 +20983,7 @@
         <v>5</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D67">
         <v>6696</v>
@@ -20888,7 +21090,7 @@
         <v>5</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D68">
         <v>6475</v>
@@ -21159,6 +21361,105 @@
       <c r="B75">
         <v>1</v>
       </c>
+      <c r="C75">
+        <v>19</v>
+      </c>
+      <c r="D75">
+        <v>1298</v>
+      </c>
+      <c r="E75">
+        <v>1420</v>
+      </c>
+      <c r="F75">
+        <v>10</v>
+      </c>
+      <c r="G75">
+        <v>37</v>
+      </c>
+      <c r="H75">
+        <v>24</v>
+      </c>
+      <c r="I75">
+        <v>5</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0.127</v>
+      </c>
+      <c r="L75">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="M75">
+        <v>0.12</v>
+      </c>
+      <c r="N75">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="O75">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="P75">
+        <v>0.127</v>
+      </c>
+      <c r="Q75">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="R75">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="S75">
+        <v>0.123</v>
+      </c>
+      <c r="T75">
+        <v>5258</v>
+      </c>
+      <c r="U75">
+        <v>5380</v>
+      </c>
+      <c r="V75">
+        <v>1000</v>
+      </c>
+      <c r="W75">
+        <v>33681</v>
+      </c>
+      <c r="X75">
+        <v>65329</v>
+      </c>
+      <c r="Y75">
+        <v>31674</v>
+      </c>
+      <c r="Z75">
+        <v>0</v>
+      </c>
+      <c r="AA75">
+        <v>0.188</v>
+      </c>
+      <c r="AB75">
+        <v>9.0540000000000003</v>
+      </c>
+      <c r="AC75">
+        <v>9.1189999999999998</v>
+      </c>
+      <c r="AD75">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="AE75">
+        <v>8.65</v>
+      </c>
+      <c r="AF75">
+        <v>8.6929999999999996</v>
+      </c>
+      <c r="AG75">
+        <v>0.127</v>
+      </c>
+      <c r="AH75">
+        <v>8.48</v>
+      </c>
+      <c r="AI75">
+        <v>8.5210000000000008</v>
+      </c>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A76">
@@ -21167,6 +21468,105 @@
       <c r="B76">
         <v>1</v>
       </c>
+      <c r="C76">
+        <v>24</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1401</v>
+      </c>
+      <c r="E76" s="2">
+        <v>1534</v>
+      </c>
+      <c r="F76" s="2">
+        <v>10</v>
+      </c>
+      <c r="G76" s="2">
+        <v>39</v>
+      </c>
+      <c r="H76" s="2">
+        <v>16</v>
+      </c>
+      <c r="I76" s="2">
+        <v>0</v>
+      </c>
+      <c r="J76" s="2">
+        <v>0</v>
+      </c>
+      <c r="K76" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="L76" s="2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="M76" s="2">
+        <v>0.127</v>
+      </c>
+      <c r="N76">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O76">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="P76">
+        <v>0.128</v>
+      </c>
+      <c r="Q76">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="R76">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="S76">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="T76">
+        <v>5361</v>
+      </c>
+      <c r="U76">
+        <v>5494</v>
+      </c>
+      <c r="V76">
+        <v>1000</v>
+      </c>
+      <c r="W76">
+        <v>18942</v>
+      </c>
+      <c r="X76">
+        <v>35842</v>
+      </c>
+      <c r="Y76">
+        <v>16927</v>
+      </c>
+      <c r="Z76">
+        <v>0</v>
+      </c>
+      <c r="AA76">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="AB76">
+        <v>5.7850000000000001</v>
+      </c>
+      <c r="AC76">
+        <v>5.8609999999999998</v>
+      </c>
+      <c r="AD76">
+        <v>0.126</v>
+      </c>
+      <c r="AE76">
+        <v>5.6920000000000002</v>
+      </c>
+      <c r="AF76">
+        <v>5.7329999999999997</v>
+      </c>
+      <c r="AG76">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AH76">
+        <v>5.3230000000000004</v>
+      </c>
+      <c r="AI76">
+        <v>5.367</v>
+      </c>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A77">
@@ -21175,6 +21575,105 @@
       <c r="B77">
         <v>1</v>
       </c>
+      <c r="C77">
+        <v>9</v>
+      </c>
+      <c r="D77">
+        <v>1324</v>
+      </c>
+      <c r="E77">
+        <v>1449</v>
+      </c>
+      <c r="F77">
+        <v>10</v>
+      </c>
+      <c r="G77">
+        <v>34</v>
+      </c>
+      <c r="H77">
+        <v>30</v>
+      </c>
+      <c r="I77">
+        <v>8</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="L77">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="M77">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="N77">
+        <v>0.13</v>
+      </c>
+      <c r="O77">
+        <v>7.8E-2</v>
+      </c>
+      <c r="P77">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="Q77">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="R77">
+        <v>7.8E-2</v>
+      </c>
+      <c r="S77">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="T77">
+        <v>1420</v>
+      </c>
+      <c r="U77">
+        <v>1545</v>
+      </c>
+      <c r="V77">
+        <v>34</v>
+      </c>
+      <c r="W77">
+        <v>108</v>
+      </c>
+      <c r="X77">
+        <v>149</v>
+      </c>
+      <c r="Y77">
+        <v>41</v>
+      </c>
+      <c r="Z77">
+        <v>0</v>
+      </c>
+      <c r="AA77">
+        <v>0.223</v>
+      </c>
+      <c r="AB77">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="AC77">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="AD77">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="AE77">
+        <v>0.111</v>
+      </c>
+      <c r="AF77">
+        <v>0.153</v>
+      </c>
+      <c r="AG77">
+        <v>0.129</v>
+      </c>
+      <c r="AH77">
+        <v>0.113</v>
+      </c>
+      <c r="AI77">
+        <v>0.156</v>
+      </c>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A78">
@@ -21183,7 +21682,105 @@
       <c r="B78">
         <v>2</v>
       </c>
-      <c r="C78" s="3"/>
+      <c r="C78" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78">
+        <v>2712</v>
+      </c>
+      <c r="E78">
+        <v>2986</v>
+      </c>
+      <c r="F78">
+        <v>10</v>
+      </c>
+      <c r="G78">
+        <v>65</v>
+      </c>
+      <c r="H78">
+        <v>39</v>
+      </c>
+      <c r="I78">
+        <v>12</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L78">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="M78">
+        <v>0.182</v>
+      </c>
+      <c r="N78">
+        <v>0.15</v>
+      </c>
+      <c r="O78">
+        <v>0.155</v>
+      </c>
+      <c r="P78">
+        <v>0.2</v>
+      </c>
+      <c r="Q78">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="R78">
+        <v>0.129</v>
+      </c>
+      <c r="S78">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="T78">
+        <v>6672</v>
+      </c>
+      <c r="U78">
+        <v>6946</v>
+      </c>
+      <c r="V78">
+        <v>1000</v>
+      </c>
+      <c r="W78">
+        <v>154743</v>
+      </c>
+      <c r="X78">
+        <v>307426</v>
+      </c>
+      <c r="Y78">
+        <v>152720</v>
+      </c>
+      <c r="Z78">
+        <v>0</v>
+      </c>
+      <c r="AA78">
+        <v>0.24</v>
+      </c>
+      <c r="AB78">
+        <v>48.652999999999999</v>
+      </c>
+      <c r="AC78">
+        <v>48.723999999999997</v>
+      </c>
+      <c r="AD78">
+        <v>0.18</v>
+      </c>
+      <c r="AE78">
+        <v>49.582000000000001</v>
+      </c>
+      <c r="AF78">
+        <v>49.631999999999998</v>
+      </c>
+      <c r="AG78">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="AH78">
+        <v>46.72</v>
+      </c>
+      <c r="AI78">
+        <v>46.764000000000003</v>
+      </c>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A79">
@@ -21192,13 +21789,105 @@
       <c r="B79">
         <v>2</v>
       </c>
-      <c r="C79" s="3"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="W79" s="2"/>
-      <c r="X79" s="2"/>
-      <c r="Y79" s="2"/>
+      <c r="C79" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79" s="2">
+        <v>2658</v>
+      </c>
+      <c r="E79" s="2">
+        <v>2921</v>
+      </c>
+      <c r="F79" s="2">
+        <v>10</v>
+      </c>
+      <c r="G79">
+        <v>61</v>
+      </c>
+      <c r="H79">
+        <v>17</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="L79">
+        <v>0.123</v>
+      </c>
+      <c r="M79">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="N79">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="O79">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="P79">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="Q79">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="R79">
+        <v>0.122</v>
+      </c>
+      <c r="S79">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="T79">
+        <v>6618</v>
+      </c>
+      <c r="U79">
+        <v>6881</v>
+      </c>
+      <c r="V79">
+        <v>1000</v>
+      </c>
+      <c r="W79" s="2">
+        <v>229831</v>
+      </c>
+      <c r="X79" s="2">
+        <v>457644</v>
+      </c>
+      <c r="Y79" s="2">
+        <v>227831</v>
+      </c>
+      <c r="Z79">
+        <v>0</v>
+      </c>
+      <c r="AA79">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="AB79">
+        <v>54.747</v>
+      </c>
+      <c r="AC79">
+        <v>54.819000000000003</v>
+      </c>
+      <c r="AD79">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AE79">
+        <v>54.491999999999997</v>
+      </c>
+      <c r="AF79">
+        <v>54.545000000000002</v>
+      </c>
+      <c r="AG79">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AH79">
+        <v>55.893000000000001</v>
+      </c>
+      <c r="AI79">
+        <v>55.938000000000002</v>
+      </c>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A80">
@@ -21207,7 +21896,105 @@
       <c r="B80">
         <v>2</v>
       </c>
-      <c r="C80" s="3"/>
+      <c r="C80" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80">
+        <v>2616</v>
+      </c>
+      <c r="E80">
+        <v>2878</v>
+      </c>
+      <c r="F80">
+        <v>10</v>
+      </c>
+      <c r="G80">
+        <v>45</v>
+      </c>
+      <c r="H80">
+        <v>15</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="L80">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="M80">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="N80">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="O80">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="P80">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="Q80">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="R80">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="S80">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="T80">
+        <v>6576</v>
+      </c>
+      <c r="U80">
+        <v>6838</v>
+      </c>
+      <c r="V80">
+        <v>1000</v>
+      </c>
+      <c r="W80">
+        <v>14081</v>
+      </c>
+      <c r="X80">
+        <v>26115</v>
+      </c>
+      <c r="Y80">
+        <v>12065</v>
+      </c>
+      <c r="Z80">
+        <v>0</v>
+      </c>
+      <c r="AA80">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AB80">
+        <v>6.8159999999999998</v>
+      </c>
+      <c r="AC80">
+        <v>6.859</v>
+      </c>
+      <c r="AD80">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="AE80">
+        <v>5.9829999999999997</v>
+      </c>
+      <c r="AF80">
+        <v>6.0279999999999996</v>
+      </c>
+      <c r="AG80">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="AH80">
+        <v>5.9889999999999999</v>
+      </c>
+      <c r="AI80">
+        <v>6.0359999999999996</v>
+      </c>
     </row>
     <row r="81" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A81">
@@ -21216,11 +22003,105 @@
       <c r="B81">
         <v>3</v>
       </c>
-      <c r="C81" s="3"/>
-      <c r="V81" s="2"/>
-      <c r="W81" s="2"/>
-      <c r="X81" s="2"/>
-      <c r="Y81" s="2"/>
+      <c r="C81" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D81">
+        <v>3994</v>
+      </c>
+      <c r="E81">
+        <v>4393</v>
+      </c>
+      <c r="F81">
+        <v>10</v>
+      </c>
+      <c r="G81">
+        <v>62</v>
+      </c>
+      <c r="H81">
+        <v>15</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="L81">
+        <v>0.157</v>
+      </c>
+      <c r="M81">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="N81">
+        <v>0.155</v>
+      </c>
+      <c r="O81">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="P81">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="Q81">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="R81">
+        <v>0.16</v>
+      </c>
+      <c r="S81">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="T81">
+        <v>7954</v>
+      </c>
+      <c r="U81">
+        <v>8353</v>
+      </c>
+      <c r="V81" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W81" s="2">
+        <v>28369</v>
+      </c>
+      <c r="X81" s="2">
+        <v>54658</v>
+      </c>
+      <c r="Y81" s="2">
+        <v>26336</v>
+      </c>
+      <c r="Z81">
+        <v>0</v>
+      </c>
+      <c r="AA81">
+        <v>0.219</v>
+      </c>
+      <c r="AB81">
+        <v>12.695</v>
+      </c>
+      <c r="AC81">
+        <v>12.77</v>
+      </c>
+      <c r="AD81">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AE81">
+        <v>11.866</v>
+      </c>
+      <c r="AF81">
+        <v>11.917</v>
+      </c>
+      <c r="AG81">
+        <v>0.157</v>
+      </c>
+      <c r="AH81">
+        <v>12.064</v>
+      </c>
+      <c r="AI81">
+        <v>12.115</v>
+      </c>
     </row>
     <row r="82" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A82">
@@ -21229,7 +22110,105 @@
       <c r="B82">
         <v>3</v>
       </c>
-      <c r="C82" s="3"/>
+      <c r="C82" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82">
+        <v>3886</v>
+      </c>
+      <c r="E82">
+        <v>4275</v>
+      </c>
+      <c r="F82">
+        <v>10</v>
+      </c>
+      <c r="G82">
+        <v>67</v>
+      </c>
+      <c r="H82">
+        <v>20</v>
+      </c>
+      <c r="I82">
+        <v>2</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0.155</v>
+      </c>
+      <c r="L82">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="M82">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="N82">
+        <v>0.153</v>
+      </c>
+      <c r="O82">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="P82">
+        <v>0.216</v>
+      </c>
+      <c r="Q82">
+        <v>0.153</v>
+      </c>
+      <c r="R82">
+        <v>0.159</v>
+      </c>
+      <c r="S82">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="T82">
+        <v>7846</v>
+      </c>
+      <c r="U82">
+        <v>8235</v>
+      </c>
+      <c r="V82">
+        <v>1000</v>
+      </c>
+      <c r="W82">
+        <v>23166</v>
+      </c>
+      <c r="X82">
+        <v>44246</v>
+      </c>
+      <c r="Y82">
+        <v>21128</v>
+      </c>
+      <c r="Z82">
+        <v>0</v>
+      </c>
+      <c r="AA82">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="AB82">
+        <v>10.513999999999999</v>
+      </c>
+      <c r="AC82">
+        <v>10.597</v>
+      </c>
+      <c r="AD82">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AE82">
+        <v>11.617000000000001</v>
+      </c>
+      <c r="AF82">
+        <v>11.688000000000001</v>
+      </c>
+      <c r="AG82">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AH82">
+        <v>10.31</v>
+      </c>
+      <c r="AI82">
+        <v>10.363</v>
+      </c>
     </row>
     <row r="83" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A83">
@@ -21238,7 +22217,105 @@
       <c r="B83">
         <v>3</v>
       </c>
-      <c r="C83" s="3"/>
+      <c r="C83" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83">
+        <v>3972</v>
+      </c>
+      <c r="E83">
+        <v>4371</v>
+      </c>
+      <c r="F83">
+        <v>10</v>
+      </c>
+      <c r="G83">
+        <v>45</v>
+      </c>
+      <c r="H83">
+        <v>15</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="L83">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="M83">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="N83">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="O83">
+        <v>0.185</v>
+      </c>
+      <c r="P83">
+        <v>0.245</v>
+      </c>
+      <c r="Q83">
+        <v>0.155</v>
+      </c>
+      <c r="R83">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="S83">
+        <v>0.215</v>
+      </c>
+      <c r="T83">
+        <v>7932</v>
+      </c>
+      <c r="U83">
+        <v>8331</v>
+      </c>
+      <c r="V83">
+        <v>1000</v>
+      </c>
+      <c r="W83">
+        <v>80859</v>
+      </c>
+      <c r="X83">
+        <v>159664</v>
+      </c>
+      <c r="Y83">
+        <v>78839</v>
+      </c>
+      <c r="Z83">
+        <v>0</v>
+      </c>
+      <c r="AA83">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AB83">
+        <v>29.734999999999999</v>
+      </c>
+      <c r="AC83">
+        <v>29.785</v>
+      </c>
+      <c r="AD83">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AE83">
+        <v>30.709</v>
+      </c>
+      <c r="AF83">
+        <v>30.76</v>
+      </c>
+      <c r="AG83">
+        <v>0.158</v>
+      </c>
+      <c r="AH83">
+        <v>30.41</v>
+      </c>
+      <c r="AI83">
+        <v>30.457999999999998</v>
+      </c>
     </row>
     <row r="84" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A84">
@@ -21247,13 +22324,105 @@
       <c r="B84">
         <v>4</v>
       </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="T84" s="2"/>
-      <c r="U84" s="2"/>
-      <c r="V84" s="2"/>
+      <c r="C84" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D84" s="2">
+        <v>5414</v>
+      </c>
+      <c r="E84" s="2">
+        <v>5955</v>
+      </c>
+      <c r="F84" s="2">
+        <v>10</v>
+      </c>
+      <c r="G84">
+        <v>61</v>
+      </c>
+      <c r="H84">
+        <v>15</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0.254</v>
+      </c>
+      <c r="L84">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="M84">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="N84">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="O84">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="P84">
+        <v>0.26</v>
+      </c>
+      <c r="Q84">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="R84">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="S84">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="T84" s="2">
+        <v>9374</v>
+      </c>
+      <c r="U84" s="2">
+        <v>9915</v>
+      </c>
+      <c r="V84" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W84">
+        <v>5715</v>
+      </c>
+      <c r="X84">
+        <v>9344</v>
+      </c>
+      <c r="Y84">
+        <v>3676</v>
+      </c>
+      <c r="Z84">
+        <v>0</v>
+      </c>
+      <c r="AA84">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="AB84">
+        <v>4.7670000000000003</v>
+      </c>
+      <c r="AC84">
+        <v>4.8540000000000001</v>
+      </c>
+      <c r="AD84">
+        <v>0.161</v>
+      </c>
+      <c r="AE84">
+        <v>4.41</v>
+      </c>
+      <c r="AF84">
+        <v>4.4710000000000001</v>
+      </c>
+      <c r="AG84">
+        <v>0.152</v>
+      </c>
+      <c r="AH84">
+        <v>4.5339999999999998</v>
+      </c>
+      <c r="AI84">
+        <v>4.59</v>
+      </c>
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A85">
@@ -21262,10 +22431,105 @@
       <c r="B85">
         <v>4</v>
       </c>
-      <c r="C85" s="3"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
+      <c r="C85" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85">
+        <v>5241</v>
+      </c>
+      <c r="E85">
+        <v>5768</v>
+      </c>
+      <c r="F85">
+        <v>10</v>
+      </c>
+      <c r="G85" s="2">
+        <v>82</v>
+      </c>
+      <c r="H85" s="2">
+        <v>17</v>
+      </c>
+      <c r="I85" s="2">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0.157</v>
+      </c>
+      <c r="L85">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="M85">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="N85">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="O85">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="P85">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="Q85">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="R85">
+        <v>0.189</v>
+      </c>
+      <c r="S85">
+        <v>0.248</v>
+      </c>
+      <c r="T85">
+        <v>9201</v>
+      </c>
+      <c r="U85">
+        <v>9728</v>
+      </c>
+      <c r="V85">
+        <v>1000</v>
+      </c>
+      <c r="W85">
+        <v>105867</v>
+      </c>
+      <c r="X85">
+        <v>209616</v>
+      </c>
+      <c r="Y85">
+        <v>103818</v>
+      </c>
+      <c r="Z85">
+        <v>0</v>
+      </c>
+      <c r="AA85">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="AB85">
+        <v>45.601999999999997</v>
+      </c>
+      <c r="AC85">
+        <v>45.689</v>
+      </c>
+      <c r="AD85">
+        <v>0.156</v>
+      </c>
+      <c r="AE85">
+        <v>44.393999999999998</v>
+      </c>
+      <c r="AF85">
+        <v>44.451000000000001</v>
+      </c>
+      <c r="AG85">
+        <v>0.155</v>
+      </c>
+      <c r="AH85">
+        <v>44.531999999999996</v>
+      </c>
+      <c r="AI85">
+        <v>44.588000000000001</v>
+      </c>
     </row>
     <row r="86" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A86">
@@ -21274,7 +22538,105 @@
       <c r="B86">
         <v>4</v>
       </c>
-      <c r="C86" s="3"/>
+      <c r="C86" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86">
+        <v>5291</v>
+      </c>
+      <c r="E86">
+        <v>5828</v>
+      </c>
+      <c r="F86">
+        <v>10</v>
+      </c>
+      <c r="G86">
+        <v>91</v>
+      </c>
+      <c r="H86">
+        <v>15</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="L86">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="M86">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="N86">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="O86">
+        <v>0.219</v>
+      </c>
+      <c r="P86">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="Q86">
+        <v>0.155</v>
+      </c>
+      <c r="R86">
+        <v>0.21</v>
+      </c>
+      <c r="S86">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="T86">
+        <v>9251</v>
+      </c>
+      <c r="U86">
+        <v>9788</v>
+      </c>
+      <c r="V86">
+        <v>1000</v>
+      </c>
+      <c r="W86">
+        <v>30823</v>
+      </c>
+      <c r="X86">
+        <v>59504</v>
+      </c>
+      <c r="Y86">
+        <v>28757</v>
+      </c>
+      <c r="Z86">
+        <v>0</v>
+      </c>
+      <c r="AA86">
+        <v>0.154</v>
+      </c>
+      <c r="AB86">
+        <v>14.582000000000001</v>
+      </c>
+      <c r="AC86">
+        <v>14.638</v>
+      </c>
+      <c r="AD86">
+        <v>0.156</v>
+      </c>
+      <c r="AE86">
+        <v>14.028</v>
+      </c>
+      <c r="AF86">
+        <v>14.082000000000001</v>
+      </c>
+      <c r="AG86">
+        <v>0.156</v>
+      </c>
+      <c r="AH86">
+        <v>14.742000000000001</v>
+      </c>
+      <c r="AI86">
+        <v>14.8</v>
+      </c>
     </row>
     <row r="87" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A87">
@@ -21283,7 +22645,105 @@
       <c r="B87">
         <v>5</v>
       </c>
-      <c r="C87" s="3"/>
+      <c r="C87" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D87">
+        <v>6561</v>
+      </c>
+      <c r="E87">
+        <v>7225</v>
+      </c>
+      <c r="F87">
+        <v>10</v>
+      </c>
+      <c r="G87">
+        <v>122</v>
+      </c>
+      <c r="H87">
+        <v>29</v>
+      </c>
+      <c r="I87">
+        <v>7</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0.17</v>
+      </c>
+      <c r="L87">
+        <v>0.24</v>
+      </c>
+      <c r="M87">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="N87">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="O87">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="P87">
+        <v>0.32</v>
+      </c>
+      <c r="Q87">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="R87">
+        <v>0.252</v>
+      </c>
+      <c r="S87">
+        <v>0.316</v>
+      </c>
+      <c r="T87" s="2">
+        <v>10521</v>
+      </c>
+      <c r="U87" s="2">
+        <v>11185</v>
+      </c>
+      <c r="V87" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W87">
+        <v>16150</v>
+      </c>
+      <c r="X87">
+        <v>30116</v>
+      </c>
+      <c r="Y87">
+        <v>14066</v>
+      </c>
+      <c r="Z87">
+        <v>0</v>
+      </c>
+      <c r="AA87">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AB87">
+        <v>10.587999999999999</v>
+      </c>
+      <c r="AC87">
+        <v>10.648999999999999</v>
+      </c>
+      <c r="AD87">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AE87">
+        <v>11.691000000000001</v>
+      </c>
+      <c r="AF87">
+        <v>11.755000000000001</v>
+      </c>
+      <c r="AG87">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="AH87">
+        <v>11.372999999999999</v>
+      </c>
+      <c r="AI87">
+        <v>11.430999999999999</v>
+      </c>
     </row>
     <row r="88" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A88">
@@ -21292,10 +22752,105 @@
       <c r="B88">
         <v>5</v>
       </c>
-      <c r="C88" s="3"/>
-      <c r="T88" s="2"/>
-      <c r="U88" s="2"/>
-      <c r="V88" s="2"/>
+      <c r="C88" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D88">
+        <v>6696</v>
+      </c>
+      <c r="E88">
+        <v>7372</v>
+      </c>
+      <c r="F88">
+        <v>10</v>
+      </c>
+      <c r="G88">
+        <v>110</v>
+      </c>
+      <c r="H88">
+        <v>15</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="L88">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="M88">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="N88">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="O88">
+        <v>0.218</v>
+      </c>
+      <c r="P88">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="Q88">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="R88">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="S88">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="T88" s="2">
+        <v>10656</v>
+      </c>
+      <c r="U88" s="2">
+        <v>11332</v>
+      </c>
+      <c r="V88" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W88">
+        <v>43420</v>
+      </c>
+      <c r="X88">
+        <v>84661</v>
+      </c>
+      <c r="Y88">
+        <v>41334</v>
+      </c>
+      <c r="Z88">
+        <v>0</v>
+      </c>
+      <c r="AA88" s="2">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="AB88" s="2">
+        <v>21.933</v>
+      </c>
+      <c r="AC88" s="2">
+        <v>22.01</v>
+      </c>
+      <c r="AD88">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="AE88">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="AF88">
+        <v>23.045999999999999</v>
+      </c>
+      <c r="AG88">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="AH88">
+        <v>23.678000000000001</v>
+      </c>
+      <c r="AI88">
+        <v>23.742000000000001</v>
+      </c>
     </row>
     <row r="89" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A89">
@@ -21304,352 +22859,108 @@
       <c r="B89">
         <v>5</v>
       </c>
-      <c r="C89" s="3"/>
-      <c r="T89" s="2"/>
-      <c r="U89" s="2"/>
-      <c r="V89" s="2"/>
-      <c r="AA89" s="2"/>
-      <c r="AB89" s="2"/>
-      <c r="AC89" s="2"/>
-    </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
-      <c r="K94" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L94" s="8"/>
-      <c r="M94" s="8"/>
-      <c r="N94" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="O94" s="8"/>
-      <c r="P94" s="8"/>
-      <c r="Q94" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R94" s="8"/>
-      <c r="S94" s="8"/>
-      <c r="T94" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="U94" s="8"/>
-      <c r="V94" s="8"/>
-      <c r="W94" s="8"/>
-      <c r="X94" s="8"/>
-      <c r="Y94" s="8"/>
-      <c r="Z94" s="8"/>
-      <c r="AA94" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB94" s="8"/>
-      <c r="AC94" s="8"/>
-      <c r="AD94" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE94" s="8"/>
-      <c r="AF94" s="8"/>
-      <c r="AG94" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH94" s="8"/>
-      <c r="AI94" s="8"/>
-    </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>0</v>
-      </c>
-      <c r="B95" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" t="s">
-        <v>3</v>
-      </c>
-      <c r="D95" t="s">
-        <v>27</v>
-      </c>
-      <c r="E95" t="s">
-        <v>28</v>
-      </c>
-      <c r="F95" t="s">
-        <v>29</v>
-      </c>
-      <c r="G95" t="s">
-        <v>30</v>
-      </c>
-      <c r="H95" t="s">
-        <v>36</v>
-      </c>
-      <c r="I95" t="s">
-        <v>31</v>
-      </c>
-      <c r="J95" t="s">
-        <v>32</v>
-      </c>
-      <c r="K95" t="s">
-        <v>17</v>
-      </c>
-      <c r="L95" t="s">
+      <c r="C89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D89">
+        <v>6475</v>
+      </c>
+      <c r="E89">
+        <v>7136</v>
+      </c>
+      <c r="F89">
+        <v>10</v>
+      </c>
+      <c r="G89">
+        <v>80</v>
+      </c>
+      <c r="H89">
         <v>18</v>
       </c>
-      <c r="M95" t="s">
-        <v>19</v>
-      </c>
-      <c r="N95" t="s">
-        <v>20</v>
-      </c>
-      <c r="O95" t="s">
-        <v>21</v>
-      </c>
-      <c r="P95" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>23</v>
-      </c>
-      <c r="R95" t="s">
-        <v>24</v>
-      </c>
-      <c r="S95" t="s">
-        <v>25</v>
-      </c>
-      <c r="T95" t="s">
-        <v>37</v>
-      </c>
-      <c r="U95" t="s">
-        <v>38</v>
-      </c>
-      <c r="V95" t="s">
-        <v>39</v>
-      </c>
-      <c r="W95" t="s">
-        <v>40</v>
-      </c>
-      <c r="X95" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y95" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z95" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA95" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB95" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC95" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD95" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE95" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF95" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG95" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH95" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI95" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <v>0</v>
-      </c>
-      <c r="B96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <v>1</v>
-      </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A98">
+      <c r="I89">
         <v>2</v>
       </c>
-      <c r="B98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <v>10</v>
-      </c>
-      <c r="B99">
-        <v>2</v>
-      </c>
-      <c r="C99" s="3"/>
-      <c r="T99" s="2"/>
-      <c r="U99" s="2"/>
-      <c r="V99" s="2"/>
-    </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>11</v>
-      </c>
-      <c r="B100">
-        <v>2</v>
-      </c>
-      <c r="C100" s="3"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="W100" s="2"/>
-      <c r="X100" s="2"/>
-      <c r="Y100" s="2"/>
-    </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>12</v>
-      </c>
-      <c r="B101">
-        <v>2</v>
-      </c>
-      <c r="C101" s="3"/>
-      <c r="T101" s="2"/>
-      <c r="U101" s="2"/>
-      <c r="V101" s="2"/>
-    </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <v>20</v>
-      </c>
-      <c r="B102">
-        <v>3</v>
-      </c>
-      <c r="C102" s="3"/>
-      <c r="V102" s="2"/>
-      <c r="W102" s="2"/>
-      <c r="X102" s="2"/>
-      <c r="Y102" s="2"/>
-    </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <v>21</v>
-      </c>
-      <c r="B103">
-        <v>3</v>
-      </c>
-      <c r="C103" s="3"/>
-    </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A104">
-        <v>22</v>
-      </c>
-      <c r="B104">
-        <v>3</v>
-      </c>
-      <c r="C104" s="3"/>
-    </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A105">
-        <v>30</v>
-      </c>
-      <c r="B105">
-        <v>4</v>
-      </c>
-      <c r="C105" s="3"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-      <c r="T105" s="2"/>
-      <c r="U105" s="2"/>
-      <c r="V105" s="2"/>
-    </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A106">
-        <v>31</v>
-      </c>
-      <c r="B106">
-        <v>4</v>
-      </c>
-      <c r="C106" s="3"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-    </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A107">
-        <v>32</v>
-      </c>
-      <c r="B107">
-        <v>4</v>
-      </c>
-      <c r="C107" s="3"/>
-    </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <v>40</v>
-      </c>
-      <c r="B108">
-        <v>5</v>
-      </c>
-      <c r="C108" s="3"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
-    </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A109">
-        <v>41</v>
-      </c>
-      <c r="B109">
-        <v>5</v>
-      </c>
-      <c r="C109" s="3"/>
-      <c r="T109" s="2"/>
-      <c r="U109" s="2"/>
-      <c r="V109" s="2"/>
-      <c r="AA109" s="2"/>
-      <c r="AB109" s="2"/>
-      <c r="AC109" s="2"/>
-    </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <v>42</v>
-      </c>
-      <c r="B110">
-        <v>5</v>
-      </c>
-      <c r="C110" s="3"/>
-      <c r="T110" s="2"/>
-      <c r="U110" s="2"/>
-      <c r="V110" s="2"/>
-      <c r="AA110" s="2"/>
-      <c r="AB110" s="2"/>
-      <c r="AC110" s="2"/>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="L89">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="M89">
+        <v>0.3</v>
+      </c>
+      <c r="N89">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="O89">
+        <v>0.254</v>
+      </c>
+      <c r="P89">
+        <v>0.313</v>
+      </c>
+      <c r="Q89">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="R89">
+        <v>0.22</v>
+      </c>
+      <c r="S89">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="T89" s="2">
+        <v>10435</v>
+      </c>
+      <c r="U89" s="2">
+        <v>11096</v>
+      </c>
+      <c r="V89" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W89">
+        <v>38334</v>
+      </c>
+      <c r="X89">
+        <v>74561</v>
+      </c>
+      <c r="Y89">
+        <v>36291</v>
+      </c>
+      <c r="Z89">
+        <v>0</v>
+      </c>
+      <c r="AA89" s="2">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="AB89" s="2">
+        <v>21.204000000000001</v>
+      </c>
+      <c r="AC89" s="2">
+        <v>21.280999999999999</v>
+      </c>
+      <c r="AD89">
+        <v>0.161</v>
+      </c>
+      <c r="AE89">
+        <v>21.405999999999999</v>
+      </c>
+      <c r="AF89">
+        <v>21.463000000000001</v>
+      </c>
+      <c r="AG89">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="AH89">
+        <v>23.306999999999999</v>
+      </c>
+      <c r="AI89">
+        <v>23.373999999999999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="32">
     <mergeCell ref="AD10:AF10"/>
     <mergeCell ref="AG10:AI10"/>
     <mergeCell ref="D31:J31"/>
@@ -21682,22 +22993,13 @@
     <mergeCell ref="Q52:S52"/>
     <mergeCell ref="T52:Z52"/>
     <mergeCell ref="AA52:AC52"/>
-    <mergeCell ref="AD94:AF94"/>
-    <mergeCell ref="AG94:AI94"/>
-    <mergeCell ref="D94:J94"/>
-    <mergeCell ref="K94:M94"/>
-    <mergeCell ref="N94:P94"/>
-    <mergeCell ref="Q94:S94"/>
-    <mergeCell ref="T94:Z94"/>
-    <mergeCell ref="AA94:AC94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating tests summary for Heuristic 1 + 160.
</commit_message>
<xml_diff>
--- a/docs/testsFSG/tests-summary.xlsx
+++ b/docs/testsFSG/tests-summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8232" windowHeight="4296" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8232" windowHeight="4296" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Constraints" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="97">
   <si>
     <t>Run</t>
   </si>
@@ -3269,6 +3269,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.19992273496842214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21353666647650751</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28366371982754124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48866628896033271</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9812948177069396</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3800,6 +3815,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.2052998606581884</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.994521587515987</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.332615378285439</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.132571282451323</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.695150497408196</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8060,7 +8090,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="2" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -8120,7 +8150,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="1" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -8164,7 +8194,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="0" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -8252,7 +8282,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="5" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -8296,7 +8326,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="4" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -8340,7 +8370,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="3" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -8428,7 +8458,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="8" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -8472,7 +8502,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="7" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -8516,7 +8546,7 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Run" dataCellStyle="Normal"/>
     <tableColumn id="2" name="#Models" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Selected models" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Selected models" dataDxfId="6" dataCellStyle="Normal"/>
     <tableColumn id="31" name="Variables2" dataCellStyle="Normal"/>
     <tableColumn id="30" name="Constraints3" dataCellStyle="Normal"/>
     <tableColumn id="35" name="Solutions4" dataCellStyle="Normal"/>
@@ -8968,7 +8998,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9078,6 +9108,22 @@
       <c r="H3">
         <v>4</v>
       </c>
+      <c r="I3">
+        <f>HARMEAN('Summary - Models'!C5,'Summary - Models'!C23)</f>
+        <v>0.11813897880583678</v>
+      </c>
+      <c r="J3">
+        <f>HARMEAN('Summary - Models'!D5,'Summary - Models'!D23)</f>
+        <v>9.7958669093294704E-2</v>
+      </c>
+      <c r="K3">
+        <f>HARMEAN('Summary - Models'!E5,'Summary - Models'!E23)</f>
+        <v>8.2001009294525404E-2</v>
+      </c>
+      <c r="L3">
+        <f>HARMEAN('Summary - Models'!F5,'Summary - Models'!F23)</f>
+        <v>7.8983911371815957E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
@@ -9558,8 +9604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="D28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10307,7 +10353,10 @@
         <f>HARMEAN('160 - Models'!L12:L14,'160 - Models'!O12:O14,'160 - Models'!R12:R14)</f>
         <v>0.19992273496842214</v>
       </c>
-      <c r="D42" s="7"/>
+      <c r="D42" s="7">
+        <f>HARMEAN('160 - Models'!L12:L14,'160 - Models'!O12:O14,'160 - Models'!R12:R14)</f>
+        <v>0.19992273496842214</v>
+      </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
     </row>
@@ -10323,7 +10372,10 @@
         <f>HARMEAN('160 - Models'!L15:L17,'160 - Models'!O15:O17,'160 - Models'!R15:R17)</f>
         <v>0.48255409989671955</v>
       </c>
-      <c r="D43" s="7"/>
+      <c r="D43" s="7">
+        <f>HARMEAN('160 - Models'!L36:L38,'160 - Models'!O36:O38,'160 - Models'!R36:R38)</f>
+        <v>0.21353666647650751</v>
+      </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
     </row>
@@ -10339,7 +10391,10 @@
         <f>HARMEAN('160 - Models'!L18:L20,'160 - Models'!O18:O20,'160 - Models'!R18:R20)</f>
         <v>0.9326603567024776</v>
       </c>
-      <c r="D44" s="7"/>
+      <c r="D44" s="7">
+        <f>HARMEAN('160 - Models'!L39:L41,'160 - Models'!O39:O41,'160 - Models'!R39:R41)</f>
+        <v>0.28366371982754124</v>
+      </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
     </row>
@@ -10355,7 +10410,10 @@
         <f>HARMEAN('160 - Models'!L21:L23,'160 - Models'!O21:O23,'160 - Models'!R21:R23)</f>
         <v>1.32805075686389</v>
       </c>
-      <c r="D45" s="7"/>
+      <c r="D45" s="7">
+        <f>HARMEAN('160 - Models'!L42:L44,'160 - Models'!R42:R44,'160 - Models'!O42:O44)</f>
+        <v>0.48866628896033271</v>
+      </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
     </row>
@@ -10371,7 +10429,10 @@
         <f>HARMEAN('160 - Models'!L24:L26,'160 - Models'!O24:O26,'160 - Models'!R24:R26)</f>
         <v>1.5081057095703692</v>
       </c>
-      <c r="D46" s="7"/>
+      <c r="D46" s="7">
+        <f>HARMEAN('160 - Models'!O45:O47,'160 - Models'!R45:R47,'160 - Models'!U45:U47)</f>
+        <v>0.9812948177069396</v>
+      </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
     </row>
@@ -10423,7 +10484,10 @@
         <f>HARMEAN('160 - Models'!AB12:AB14,'160 - Models'!AE12:AE14,'160 - Models'!AH12:AH14)</f>
         <v>7.6469880237127192</v>
       </c>
-      <c r="D51" s="7"/>
+      <c r="D51" s="7">
+        <f>HARMEAN('160 - Models'!AB33:AB35,'160 - Models'!AE33:AE35,'160 - Models'!AH33:AH35)</f>
+        <v>5.2052998606581884</v>
+      </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
     </row>
@@ -10439,7 +10503,10 @@
         <f>HARMEAN('160 - Models'!AB15:AB17,'160 - Models'!AE15:AE17,'160 - Models'!AH15:AH17)</f>
         <v>33.63532095104884</v>
       </c>
-      <c r="D52" s="7"/>
+      <c r="D52" s="7">
+        <f>HARMEAN('160 - Models'!AB36:AB38,'160 - Models'!AE36:AE38,'160 - Models'!AH36:AH38)</f>
+        <v>11.994521587515987</v>
+      </c>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
     </row>
@@ -10455,7 +10522,10 @@
         <f>HARMEAN('160 - Models'!AB18:AB20,'160 - Models'!AE18:AE20,'160 - Models'!AH18:AH20)</f>
         <v>30.083124143729631</v>
       </c>
-      <c r="D53" s="7"/>
+      <c r="D53" s="7">
+        <f>HARMEAN('160 - Models'!AB39:AB41,'160 - Models'!AE39:AE41,'160 - Models'!AH39:AH41)</f>
+        <v>17.332615378285439</v>
+      </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
     </row>
@@ -10471,7 +10541,10 @@
         <f>HARMEAN('160 - Models'!AB21:AB23,'160 - Models'!AE21:AE23,'160 - Models'!AH21:AH23)</f>
         <v>31.976986274077074</v>
       </c>
-      <c r="D54" s="7"/>
+      <c r="D54" s="7">
+        <f>HARMEAN('160 - Models'!AB42:AB44,'160 - Models'!AE42:AE44,'160 - Models'!AH42:AH44)</f>
+        <v>25.132571282451323</v>
+      </c>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
     </row>
@@ -10487,7 +10560,10 @@
         <f>HARMEAN('160 - Models'!AB24:AB26,'160 - Models'!AE24:AE26,'160 - Models'!AH24:AH26)</f>
         <v>131.20788481112584</v>
       </c>
-      <c r="D55" s="7"/>
+      <c r="D55" s="7">
+        <f>HARMEAN('160 - Models'!AB45:AB47,'160 - Models'!AE45:AE47,'160 - Models'!AH45:AH47)</f>
+        <v>17.695150497408196</v>
+      </c>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
     </row>
@@ -26690,8 +26766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI89"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28679,146 +28755,1610 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>19</v>
+      </c>
+      <c r="D33">
+        <v>2733</v>
+      </c>
+      <c r="E33">
+        <v>2998</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="G33">
+        <v>40</v>
+      </c>
+      <c r="H33">
+        <v>16</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0.15</v>
+      </c>
+      <c r="L33">
+        <v>0.153</v>
+      </c>
+      <c r="M33">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="N33">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="O33">
+        <v>0.129</v>
+      </c>
+      <c r="P33">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="Q33">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="R33">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="S33">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="T33">
+        <v>6693</v>
+      </c>
+      <c r="U33">
+        <v>6958</v>
+      </c>
+      <c r="V33">
+        <v>1000</v>
+      </c>
+      <c r="W33">
+        <v>121609</v>
+      </c>
+      <c r="X33">
+        <v>241145</v>
+      </c>
+      <c r="Y33">
+        <v>119577</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>0.156</v>
+      </c>
+      <c r="AB33">
+        <v>52.21</v>
+      </c>
+      <c r="AC33">
+        <v>52.26</v>
+      </c>
+      <c r="AD33">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="AE33">
+        <v>60.807000000000002</v>
+      </c>
+      <c r="AF33">
+        <v>60.854999999999997</v>
+      </c>
+      <c r="AG33">
+        <v>0.2</v>
+      </c>
+      <c r="AH33">
+        <v>69.863</v>
+      </c>
+      <c r="AI33">
+        <v>69.935000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>24</v>
+      </c>
+      <c r="D34">
+        <v>2748</v>
+      </c>
+      <c r="E34">
+        <v>3015</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34">
+        <v>65</v>
+      </c>
+      <c r="H34">
+        <v>17</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="L34">
+        <v>0.123</v>
+      </c>
+      <c r="M34">
+        <v>0.17</v>
+      </c>
+      <c r="N34">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="O34">
+        <v>0.12</v>
+      </c>
+      <c r="P34">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="Q34">
+        <v>0.15</v>
+      </c>
+      <c r="R34">
+        <v>0.127</v>
+      </c>
+      <c r="S34">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="T34" s="2">
+        <v>6708</v>
+      </c>
+      <c r="U34" s="2">
+        <v>6975</v>
+      </c>
+      <c r="V34" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W34">
+        <v>4448</v>
+      </c>
+      <c r="X34">
+        <v>6812</v>
+      </c>
+      <c r="Y34">
+        <v>2412</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>0.157</v>
+      </c>
+      <c r="AB34">
+        <v>2.5920000000000001</v>
+      </c>
+      <c r="AC34">
+        <v>2.6419999999999999</v>
+      </c>
+      <c r="AD34">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="AE34">
+        <v>2.5419999999999998</v>
+      </c>
+      <c r="AF34">
+        <v>2.5870000000000002</v>
+      </c>
+      <c r="AG34">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="AH34">
+        <v>2.5830000000000002</v>
+      </c>
+      <c r="AI34">
+        <v>2.629</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>2737</v>
+      </c>
+      <c r="E35">
+        <v>3002</v>
+      </c>
+      <c r="F35">
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <v>57</v>
+      </c>
+      <c r="H35">
+        <v>17</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="L35">
+        <v>0.122</v>
+      </c>
+      <c r="M35">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="N35">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="O35">
+        <v>0.124</v>
+      </c>
+      <c r="P35">
+        <v>0.17</v>
+      </c>
+      <c r="Q35">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="R35">
+        <v>0.121</v>
+      </c>
+      <c r="S35">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="T35">
+        <v>6697</v>
+      </c>
+      <c r="U35">
+        <v>6962</v>
+      </c>
+      <c r="V35">
+        <v>1000</v>
+      </c>
+      <c r="W35">
+        <v>11803</v>
+      </c>
+      <c r="X35">
+        <v>21544</v>
+      </c>
+      <c r="Y35">
+        <v>9778</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="AB35">
+        <v>5.9459999999999997</v>
+      </c>
+      <c r="AC35">
+        <v>6.032</v>
+      </c>
+      <c r="AD35">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AE35">
+        <v>5.8410000000000002</v>
+      </c>
+      <c r="AF35">
+        <v>5.8890000000000002</v>
+      </c>
+      <c r="AG35">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="AH35">
+        <v>5.7679999999999998</v>
+      </c>
+      <c r="AI35">
+        <v>5.8140000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36">
+        <v>5437</v>
+      </c>
+      <c r="E36">
+        <v>5982</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="G36">
+        <v>88</v>
+      </c>
+      <c r="H36">
+        <v>17</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="L36">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="M36">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="N36">
+        <v>0.158</v>
+      </c>
+      <c r="O36">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="P36">
+        <v>0.253</v>
+      </c>
+      <c r="Q36">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="R36">
+        <v>0.192</v>
+      </c>
+      <c r="S36">
+        <v>0.248</v>
+      </c>
+      <c r="T36">
+        <v>9397</v>
+      </c>
+      <c r="U36">
+        <v>9942</v>
+      </c>
+      <c r="V36">
+        <v>1000</v>
+      </c>
+      <c r="W36">
+        <v>8107</v>
+      </c>
+      <c r="X36">
+        <v>14088</v>
+      </c>
+      <c r="Y36">
+        <v>6050</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <v>0.309</v>
+      </c>
+      <c r="AB36">
+        <v>7.266</v>
+      </c>
+      <c r="AC36">
+        <v>7.3780000000000001</v>
+      </c>
+      <c r="AD36">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="AE36">
+        <v>6.65</v>
+      </c>
+      <c r="AF36">
+        <v>6.7210000000000001</v>
+      </c>
+      <c r="AG36">
+        <v>0.224</v>
+      </c>
+      <c r="AH36">
+        <v>6.9880000000000004</v>
+      </c>
+      <c r="AI36">
+        <v>7.069</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>11</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>5283</v>
+      </c>
+      <c r="E37">
+        <v>5818</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37">
+        <v>86</v>
+      </c>
+      <c r="H37">
+        <v>17</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="L37">
+        <v>0.249</v>
+      </c>
+      <c r="M37">
+        <v>0.308</v>
+      </c>
+      <c r="N37">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="O37">
+        <v>0.215</v>
+      </c>
+      <c r="P37">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="Q37">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="R37">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="S37">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="T37" s="2">
+        <v>9243</v>
+      </c>
+      <c r="U37" s="2">
+        <v>9778</v>
+      </c>
+      <c r="V37" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W37">
+        <v>44566</v>
+      </c>
+      <c r="X37">
+        <v>86966</v>
+      </c>
+      <c r="Y37">
+        <v>42487</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AB37">
+        <v>19.457000000000001</v>
+      </c>
+      <c r="AC37">
+        <v>19.568999999999999</v>
+      </c>
+      <c r="AD37">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="AE37">
+        <v>17.951000000000001</v>
+      </c>
+      <c r="AF37">
+        <v>18.012</v>
+      </c>
+      <c r="AG37">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="AH37">
+        <v>18.03</v>
+      </c>
+      <c r="AI37">
+        <v>18.09</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>12</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>5414</v>
+      </c>
+      <c r="E38">
+        <v>5955</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <v>101</v>
+      </c>
+      <c r="H38">
+        <v>17</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="L38">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="M38">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="N38">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="O38">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="P38">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="Q38">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="R38">
+        <v>0.224</v>
+      </c>
+      <c r="S38">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="T38">
+        <v>9374</v>
+      </c>
+      <c r="U38">
+        <v>9915</v>
+      </c>
+      <c r="V38">
+        <v>1000</v>
+      </c>
+      <c r="W38">
+        <v>41543</v>
+      </c>
+      <c r="X38">
+        <v>80930</v>
+      </c>
+      <c r="Y38">
+        <v>39472</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <v>0.312</v>
+      </c>
+      <c r="AB38">
+        <v>19.940999999999999</v>
+      </c>
+      <c r="AC38">
+        <v>20.047000000000001</v>
+      </c>
+      <c r="AD38">
+        <v>0.16</v>
+      </c>
+      <c r="AE38">
+        <v>18.983000000000001</v>
+      </c>
+      <c r="AF38">
+        <v>19.041</v>
+      </c>
+      <c r="AG38">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="AH38">
+        <v>18.571999999999999</v>
+      </c>
+      <c r="AI38">
+        <v>18.631</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C39" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39">
+        <v>8113</v>
+      </c>
+      <c r="E39">
+        <v>8934</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>95</v>
+      </c>
+      <c r="H39">
+        <v>15</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0.185</v>
+      </c>
+      <c r="L39">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="M39">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="N39">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="O39">
+        <v>0.313</v>
+      </c>
+      <c r="P39">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="Q39">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="R39">
+        <v>0.248</v>
+      </c>
+      <c r="S39">
+        <v>0.312</v>
+      </c>
+      <c r="T39">
+        <v>12073</v>
+      </c>
+      <c r="U39">
+        <v>12894</v>
+      </c>
+      <c r="V39">
+        <v>1000</v>
+      </c>
+      <c r="W39">
+        <v>98055</v>
+      </c>
+      <c r="X39">
+        <v>193979</v>
+      </c>
+      <c r="Y39">
+        <v>95998</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
+      <c r="AA39">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="AB39">
+        <v>49.79</v>
+      </c>
+      <c r="AC39">
+        <v>49.866999999999997</v>
+      </c>
+      <c r="AD39">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="AE39">
+        <v>51.338000000000001</v>
+      </c>
+      <c r="AF39">
+        <v>51.412999999999997</v>
+      </c>
+      <c r="AG39">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="AH39">
+        <v>50.268999999999998</v>
+      </c>
+      <c r="AI39">
+        <v>50.348999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>21</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>8122</v>
+      </c>
+      <c r="E40">
+        <v>8941</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>109</v>
+      </c>
+      <c r="H40">
+        <v>15</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0.18</v>
+      </c>
+      <c r="L40">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="M40">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="N40">
+        <v>0.214</v>
+      </c>
+      <c r="O40">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="P40">
+        <v>0.4</v>
+      </c>
+      <c r="Q40">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="R40">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="S40">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="T40">
+        <v>12082</v>
+      </c>
+      <c r="U40">
+        <v>12901</v>
+      </c>
+      <c r="V40">
+        <v>1000</v>
+      </c>
+      <c r="W40">
+        <v>17747</v>
+      </c>
+      <c r="X40">
+        <v>33317</v>
+      </c>
+      <c r="Y40">
+        <v>15664</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
+      <c r="AA40">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="AB40">
+        <v>16.295999999999999</v>
+      </c>
+      <c r="AC40">
+        <v>16.364999999999998</v>
+      </c>
+      <c r="AD40">
+        <v>0.185</v>
+      </c>
+      <c r="AE40">
+        <v>15.064</v>
+      </c>
+      <c r="AF40">
+        <v>15.134</v>
+      </c>
+      <c r="AG40">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="AH40">
+        <v>17.177</v>
+      </c>
+      <c r="AI40">
+        <v>17.241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>22</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>7872</v>
+      </c>
+      <c r="E41">
+        <v>8669</v>
+      </c>
+      <c r="F41">
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>96</v>
+      </c>
+      <c r="H41">
+        <v>23</v>
+      </c>
+      <c r="I41">
+        <v>4</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="L41">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M41">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="N41">
+        <v>0.193</v>
+      </c>
+      <c r="O41">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="P41">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="Q41">
+        <v>0.222</v>
+      </c>
+      <c r="R41">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="S41">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="T41">
+        <v>11832</v>
+      </c>
+      <c r="U41">
+        <v>12629</v>
+      </c>
+      <c r="V41">
+        <v>1000</v>
+      </c>
+      <c r="W41">
+        <v>8860</v>
+      </c>
+      <c r="X41">
+        <v>15588</v>
+      </c>
+      <c r="Y41">
+        <v>6800</v>
+      </c>
+      <c r="Z41">
+        <v>0</v>
+      </c>
+      <c r="AA41">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="AB41">
+        <v>10.86</v>
+      </c>
+      <c r="AC41">
+        <v>10.981999999999999</v>
+      </c>
+      <c r="AD41">
+        <v>0.247</v>
+      </c>
+      <c r="AE41">
+        <v>11.305999999999999</v>
+      </c>
+      <c r="AF41">
+        <v>11.401999999999999</v>
+      </c>
+      <c r="AG41">
+        <v>0.252</v>
+      </c>
+      <c r="AH41">
+        <v>10.718</v>
+      </c>
+      <c r="AI41">
+        <v>10.808999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>30</v>
       </c>
       <c r="B42">
         <v>4</v>
       </c>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>10758</v>
+      </c>
+      <c r="E42">
+        <v>11850</v>
+      </c>
+      <c r="F42">
+        <v>10</v>
+      </c>
+      <c r="G42">
+        <v>150</v>
+      </c>
+      <c r="H42">
+        <v>21</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="L42">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="M42">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="N42">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="O42">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="P42">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="Q42">
+        <v>0.315</v>
+      </c>
+      <c r="R42">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="S42">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="T42">
+        <v>14718</v>
+      </c>
+      <c r="U42">
+        <v>15810</v>
+      </c>
+      <c r="V42">
+        <v>1000</v>
+      </c>
+      <c r="W42">
+        <v>122867</v>
+      </c>
+      <c r="X42">
+        <v>243489</v>
+      </c>
+      <c r="Y42">
+        <v>120752</v>
+      </c>
+      <c r="Z42">
+        <v>0</v>
+      </c>
+      <c r="AA42">
+        <v>0.376</v>
+      </c>
+      <c r="AB42">
+        <v>108.59099999999999</v>
+      </c>
+      <c r="AC42">
+        <v>108.74299999999999</v>
+      </c>
+      <c r="AD42">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="AE42">
+        <v>83.774000000000001</v>
+      </c>
+      <c r="AF42">
+        <v>83.87</v>
+      </c>
+      <c r="AG42">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="AH42">
+        <v>100.738</v>
+      </c>
+      <c r="AI42">
+        <v>100.836</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>31</v>
       </c>
       <c r="B43">
         <v>4</v>
       </c>
-      <c r="C43" s="3"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43">
+        <v>10727</v>
+      </c>
+      <c r="E43">
+        <v>11820</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+      <c r="G43">
+        <v>116</v>
+      </c>
+      <c r="H43">
+        <v>17</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="L43">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="M43">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="N43">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="O43">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="P43">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="Q43">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="R43">
+        <v>0.438</v>
+      </c>
+      <c r="S43">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="T43">
+        <v>14687</v>
+      </c>
+      <c r="U43">
+        <v>15780</v>
+      </c>
+      <c r="V43">
+        <v>1000</v>
+      </c>
+      <c r="W43">
+        <v>6848</v>
+      </c>
+      <c r="X43">
+        <v>11516</v>
+      </c>
+      <c r="Y43">
+        <v>4762</v>
+      </c>
+      <c r="Z43">
+        <v>0</v>
+      </c>
+      <c r="AA43">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="AB43">
+        <v>13.981</v>
+      </c>
+      <c r="AC43">
+        <v>14.105</v>
+      </c>
+      <c r="AD43">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="AE43">
+        <v>12.379</v>
+      </c>
+      <c r="AF43">
+        <v>12.569000000000001</v>
+      </c>
+      <c r="AG43">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="AH43">
+        <v>10.513999999999999</v>
+      </c>
+      <c r="AI43">
+        <v>10.632999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>32</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44">
+        <v>10656</v>
+      </c>
+      <c r="E44">
+        <v>11734</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+      <c r="G44">
+        <v>99</v>
+      </c>
+      <c r="H44">
+        <v>28</v>
+      </c>
+      <c r="I44">
+        <v>8</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="L44">
+        <v>0.437</v>
+      </c>
+      <c r="M44">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="N44">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="O44">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="P44">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="Q44">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="R44">
+        <v>0.45</v>
+      </c>
+      <c r="S44">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="T44">
+        <v>14616</v>
+      </c>
+      <c r="U44">
+        <v>15694</v>
+      </c>
+      <c r="V44">
+        <v>1000</v>
+      </c>
+      <c r="W44">
+        <v>32702</v>
+      </c>
+      <c r="X44">
+        <v>63270</v>
+      </c>
+      <c r="Y44">
+        <v>30642</v>
+      </c>
+      <c r="Z44">
+        <v>0</v>
+      </c>
+      <c r="AA44">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="AB44">
+        <v>33.536999999999999</v>
+      </c>
+      <c r="AC44">
+        <v>33.658000000000001</v>
+      </c>
+      <c r="AD44">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="AE44">
+        <v>34.786000000000001</v>
+      </c>
+      <c r="AF44">
+        <v>34.878999999999998</v>
+      </c>
+      <c r="AG44">
+        <v>0.221</v>
+      </c>
+      <c r="AH44">
+        <v>47.518000000000001</v>
+      </c>
+      <c r="AI44">
+        <v>47.604999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>40</v>
       </c>
       <c r="B45">
         <v>5</v>
       </c>
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45">
+        <v>13237</v>
+      </c>
+      <c r="E45">
+        <v>14585</v>
+      </c>
+      <c r="F45">
+        <v>10</v>
+      </c>
+      <c r="G45">
+        <v>177</v>
+      </c>
+      <c r="H45">
+        <v>23</v>
+      </c>
+      <c r="I45">
+        <v>4</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="L45">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="M45">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="N45">
+        <v>0.318</v>
+      </c>
+      <c r="O45">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="P45">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="Q45">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="R45">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="S45">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="T45">
+        <v>17197</v>
+      </c>
+      <c r="U45">
+        <v>18545</v>
+      </c>
+      <c r="V45">
+        <v>1000</v>
+      </c>
+      <c r="W45">
+        <v>6257</v>
+      </c>
+      <c r="X45">
+        <v>10217</v>
+      </c>
+      <c r="Y45">
+        <v>4116</v>
+      </c>
+      <c r="Z45">
+        <v>0</v>
+      </c>
+      <c r="AA45">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="AB45">
+        <v>13.382</v>
+      </c>
+      <c r="AC45">
+        <v>13.5</v>
+      </c>
+      <c r="AD45">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="AE45">
+        <v>10.835000000000001</v>
+      </c>
+      <c r="AF45">
+        <v>10.929</v>
+      </c>
+      <c r="AG45">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="AH45">
+        <v>12.493</v>
+      </c>
+      <c r="AI45">
+        <v>12.612</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>41</v>
       </c>
       <c r="B46">
         <v>5</v>
       </c>
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46">
+        <v>13444</v>
+      </c>
+      <c r="E46">
+        <v>14812</v>
+      </c>
+      <c r="F46">
+        <v>10</v>
+      </c>
+      <c r="G46">
+        <v>66</v>
+      </c>
+      <c r="H46">
+        <v>16</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="L46">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="M46">
+        <v>0.76</v>
+      </c>
+      <c r="N46">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="O46">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="P46">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="Q46">
+        <v>0.33</v>
+      </c>
+      <c r="R46">
+        <v>0.63</v>
+      </c>
+      <c r="S46">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="T46">
+        <v>17404</v>
+      </c>
+      <c r="U46">
+        <v>18772</v>
+      </c>
+      <c r="V46">
+        <v>1000</v>
+      </c>
+      <c r="W46">
+        <v>8328</v>
+      </c>
+      <c r="X46">
+        <v>14566</v>
+      </c>
+      <c r="Y46">
+        <v>6287</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
+      <c r="AA46">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="AB46">
+        <v>13.738</v>
+      </c>
+      <c r="AC46">
+        <v>13.888</v>
+      </c>
+      <c r="AD46">
+        <v>0.32</v>
+      </c>
+      <c r="AE46">
+        <v>14.705</v>
+      </c>
+      <c r="AF46">
+        <v>14.831</v>
+      </c>
+      <c r="AG46">
+        <v>0.311</v>
+      </c>
+      <c r="AH46">
+        <v>13.565</v>
+      </c>
+      <c r="AI46">
+        <v>13.701000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>42</v>
       </c>
       <c r="B47">
         <v>5</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
+      <c r="C47" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D47">
+        <v>13328</v>
+      </c>
+      <c r="E47">
+        <v>14685</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47">
+        <v>83</v>
+      </c>
+      <c r="H47">
+        <v>17</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="L47">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="M47">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="N47">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="O47">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="P47">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="Q47">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="R47">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="S47">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="T47" s="2">
+        <v>17288</v>
+      </c>
+      <c r="U47" s="2">
+        <v>18645</v>
+      </c>
+      <c r="V47" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W47">
+        <v>60053</v>
+      </c>
+      <c r="X47">
+        <v>117991</v>
+      </c>
+      <c r="Y47">
+        <v>58001</v>
+      </c>
+      <c r="Z47">
+        <v>0</v>
+      </c>
+      <c r="AA47">
+        <v>0.35</v>
+      </c>
+      <c r="AB47">
+        <v>68.697000000000003</v>
+      </c>
+      <c r="AC47">
+        <v>68.852000000000004</v>
+      </c>
+      <c r="AD47">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="AE47">
+        <v>51.957999999999998</v>
+      </c>
+      <c r="AF47">
+        <v>52.067</v>
+      </c>
+      <c r="AG47">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="AH47">
+        <v>75.578000000000003</v>
+      </c>
+      <c r="AI47">
+        <v>75.721999999999994</v>
+      </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
@@ -28992,6 +30532,9 @@
       <c r="B54">
         <v>1</v>
       </c>
+      <c r="C54">
+        <v>19</v>
+      </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -29000,6 +30543,9 @@
       <c r="B55">
         <v>1</v>
       </c>
+      <c r="C55">
+        <v>24</v>
+      </c>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -29008,6 +30554,9 @@
       <c r="B56">
         <v>1</v>
       </c>
+      <c r="C56">
+        <v>9</v>
+      </c>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -29016,7 +30565,9 @@
       <c r="B57">
         <v>2</v>
       </c>
-      <c r="C57" s="3"/>
+      <c r="C57" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -29025,7 +30576,9 @@
       <c r="B58">
         <v>2</v>
       </c>
-      <c r="C58" s="3"/>
+      <c r="C58" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="W58" s="2"/>
       <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
@@ -29037,7 +30590,9 @@
       <c r="B59">
         <v>2</v>
       </c>
-      <c r="C59" s="3"/>
+      <c r="C59" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A60">
@@ -29046,7 +30601,9 @@
       <c r="B60">
         <v>3</v>
       </c>
-      <c r="C60" s="3"/>
+      <c r="C60" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -29061,7 +30618,9 @@
       <c r="B61">
         <v>3</v>
       </c>
-      <c r="C61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -29075,7 +30634,9 @@
       <c r="B62">
         <v>3</v>
       </c>
-      <c r="C62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A63">
@@ -29084,7 +30645,9 @@
       <c r="B63">
         <v>4</v>
       </c>
-      <c r="C63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -29099,7 +30662,9 @@
       <c r="B64">
         <v>4</v>
       </c>
-      <c r="C64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -29111,7 +30676,9 @@
       <c r="B65">
         <v>4</v>
       </c>
-      <c r="C65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A66">
@@ -29120,7 +30687,9 @@
       <c r="B66">
         <v>5</v>
       </c>
-      <c r="C66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A67">
@@ -29129,7 +30698,9 @@
       <c r="B67">
         <v>5</v>
       </c>
-      <c r="C67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="T67" s="2"/>
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
@@ -29143,7 +30714,9 @@
       <c r="B68">
         <v>5</v>
       </c>
-      <c r="C68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="T68" s="2"/>
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
@@ -29323,6 +30896,9 @@
       <c r="B75">
         <v>1</v>
       </c>
+      <c r="C75">
+        <v>19</v>
+      </c>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A76">
@@ -29330,6 +30906,9 @@
       </c>
       <c r="B76">
         <v>1</v>
+      </c>
+      <c r="C76">
+        <v>24</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -29349,6 +30928,9 @@
       <c r="B77">
         <v>1</v>
       </c>
+      <c r="C77">
+        <v>9</v>
+      </c>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A78">
@@ -29357,7 +30939,9 @@
       <c r="B78">
         <v>2</v>
       </c>
-      <c r="C78" s="3"/>
+      <c r="C78" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A79">
@@ -29366,7 +30950,9 @@
       <c r="B79">
         <v>2</v>
       </c>
-      <c r="C79" s="3"/>
+      <c r="C79" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -29381,7 +30967,9 @@
       <c r="B80">
         <v>2</v>
       </c>
-      <c r="C80" s="3"/>
+      <c r="C80" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81">
@@ -29390,7 +30978,9 @@
       <c r="B81">
         <v>3</v>
       </c>
-      <c r="C81" s="3"/>
+      <c r="C81" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="V81" s="2"/>
       <c r="W81" s="2"/>
       <c r="X81" s="2"/>
@@ -29403,7 +30993,9 @@
       <c r="B82">
         <v>3</v>
       </c>
-      <c r="C82" s="3"/>
+      <c r="C82" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83">
@@ -29412,7 +31004,9 @@
       <c r="B83">
         <v>3</v>
       </c>
-      <c r="C83" s="3"/>
+      <c r="C83" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="84" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A84">
@@ -29421,7 +31015,9 @@
       <c r="B84">
         <v>4</v>
       </c>
-      <c r="C84" s="3"/>
+      <c r="C84" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
@@ -29436,7 +31032,9 @@
       <c r="B85">
         <v>4</v>
       </c>
-      <c r="C85" s="3"/>
+      <c r="C85" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -29448,7 +31046,9 @@
       <c r="B86">
         <v>4</v>
       </c>
-      <c r="C86" s="3"/>
+      <c r="C86" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87">
@@ -29457,7 +31057,9 @@
       <c r="B87">
         <v>5</v>
       </c>
-      <c r="C87" s="3"/>
+      <c r="C87" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="T87" s="2"/>
       <c r="U87" s="2"/>
       <c r="V87" s="2"/>
@@ -29469,7 +31071,9 @@
       <c r="B88">
         <v>5</v>
       </c>
-      <c r="C88" s="3"/>
+      <c r="C88" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="T88" s="2"/>
       <c r="U88" s="2"/>
       <c r="V88" s="2"/>
@@ -29484,7 +31088,9 @@
       <c r="B89">
         <v>5</v>
       </c>
-      <c r="C89" s="3"/>
+      <c r="C89" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="T89" s="2"/>
       <c r="U89" s="2"/>
       <c r="V89" s="2"/>

</xml_diff>

<commit_message>
Updating tests summary for Heuristic 3 + 160.
</commit_message>
<xml_diff>
--- a/docs/testsFSG/tests-summary.xlsx
+++ b/docs/testsFSG/tests-summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8232" windowHeight="4296" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8232" windowHeight="4296" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Constraints" sheetId="6" r:id="rId1"/>
@@ -1169,7 +1169,7 @@
                   <c:v>0.10156336722046637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12786435704368879</c:v>
+                  <c:v>0.15115110713730162</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.15417903466059946</c:v>
@@ -1178,16 +1178,16 @@
                   <c:v>0.16262414002527026</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.22716082133096244</c:v>
+                  <c:v>0.22327018007930705</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.24044982172616361</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.31945853588623524</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.57024115125874641</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1405,6 +1405,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>1000 Solutions</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1554,7 +1579,7 @@
                 <c:pt idx="6">
                   <c:v>25.18549233492114</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>42.83365578908839</c:v>
                 </c:pt>
               </c:numCache>
@@ -1675,7 +1700,7 @@
                 <c:pt idx="6">
                   <c:v>12.865052853918522</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>8.5724833041754245</c:v>
                 </c:pt>
               </c:numCache>
@@ -1796,7 +1821,7 @@
                 <c:pt idx="6">
                   <c:v>15.758058682833097</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>16.756228717733677</c:v>
                 </c:pt>
               </c:numCache>
@@ -1915,9 +1940,9 @@
                   <c:v>14.441589155109996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.6598031875659505</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
+                  <c:v>14.251047098065008</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16.79035970925041</c:v>
                 </c:pt>
               </c:numCache>
@@ -4948,6 +4973,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.23774923623549168</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21951056668767799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31945853588623524</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42407293399927654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57024115125874641</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5509,6 +5549,21 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.019550040108641</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.16004739392222</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.210225981036634</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.534879232324485</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.685382650143971</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11747,8 +11802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="E18" workbookViewId="0">
-      <selection activeCell="I23" activeCellId="1" sqref="F23:F40 I23:L40"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11950,7 +12005,7 @@
       </c>
       <c r="L5" s="7">
         <f>HARMEAN('Summary - Models'!F7,'Summary - Models'!F24,'Summary - Models'!F42)</f>
-        <v>0.12786435704368879</v>
+        <v>0.15115110713730162</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -12067,7 +12122,7 @@
       </c>
       <c r="L8" s="14">
         <f>HARMEAN('Summary - Models'!F26,'Summary - Models'!F43)</f>
-        <v>0.22716082133096244</v>
+        <v>0.22327018007930705</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -12145,7 +12200,7 @@
       </c>
       <c r="L10" s="7">
         <f>'Summary - Models'!F44</f>
-        <v>0</v>
+        <v>0.31945853588623524</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -12211,7 +12266,7 @@
       </c>
       <c r="L12" s="7">
         <f>'Summary - Models'!F46</f>
-        <v>0</v>
+        <v>0.57024115125874641</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -12689,7 +12744,7 @@
       </c>
       <c r="L30" s="14">
         <f>HARMEAN('Summary - Models'!F35,'Summary - Models'!F52)</f>
-        <v>9.6598031875659505</v>
+        <v>14.251047098065008</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -12702,19 +12757,19 @@
       <c r="H31">
         <v>20</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="7">
         <f>'Summary - Models'!C36</f>
         <v>42.83365578908839</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="7">
         <f>'Summary - Models'!D36</f>
         <v>8.5724833041754245</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="7">
         <f>'Summary - Models'!E36</f>
         <v>16.756228717733677</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="7">
         <f>'Summary - Models'!F36</f>
         <v>16.79035970925041</v>
       </c>
@@ -12861,8 +12916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView topLeftCell="D37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13618,7 +13673,10 @@
         <f>HARMEAN('160 - Models'!L54:L56,'160 - Models'!O54:O56,'160 - Models'!R54:R56)</f>
         <v>0.16627748000652248</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="7">
+        <f>HARMEAN('160 - Models'!L75:L77,'160 - Models'!O75:O77,'160 - Models'!R75:R77)</f>
+        <v>0.23774923623549168</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
@@ -13640,7 +13698,10 @@
         <f>HARMEAN('160 - Models'!L57:L59,'160 - Models'!O57:O59,'160 - Models'!R57:R59)</f>
         <v>0.26165791948762801</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="7">
+        <f>HARMEAN('160 - Models'!L78:L80,'160 - Models'!O78:O80,'160 - Models'!R78:R80)</f>
+        <v>0.21951056668767799</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
@@ -13662,7 +13723,10 @@
         <f>HARMEAN('160 - Models'!L60:L62,'160 - Models'!O60:O62,'160 - Models'!R60:R62)</f>
         <v>0.28407873426735769</v>
       </c>
-      <c r="F44" s="7"/>
+      <c r="F44" s="7">
+        <f>HARMEAN('160 - Models'!L81:L83,'160 - Models'!O81:O83,'160 - Models'!R81:R83)</f>
+        <v>0.31945853588623524</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -13684,7 +13748,10 @@
         <f>HARMEAN('160 - Models'!L63:L65,'160 - Models'!O63:O65,'160 - Models'!R63:R65)</f>
         <v>0.33768944938022039</v>
       </c>
-      <c r="F45" s="7"/>
+      <c r="F45" s="7">
+        <f>HARMEAN('160 - Models'!L84:L86,'160 - Models'!O84:O86,'160 - Models'!R84:R86)</f>
+        <v>0.42407293399927654</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -13706,7 +13773,10 @@
         <f>HARMEAN('160 - Models'!L66:L68,'160 - Models'!O66:O68,'160 - Models'!R66:R68)</f>
         <v>0.3939455246647362</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="7">
+        <f>HARMEAN('160 - Models'!L87:L89,'160 - Models'!O87:O89,'160 - Models'!R87:R89)</f>
+        <v>0.57024115125874641</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -13764,7 +13834,10 @@
         <f>HARMEAN('160 - Models'!AB54:AB56,'160 - Models'!AE54:AE56,'160 - Models'!AH54:AH56)</f>
         <v>25.732582179426373</v>
       </c>
-      <c r="F51" s="7"/>
+      <c r="F51" s="7">
+        <f>HARMEAN('160 - Models'!AB75:AB77,'160 - Models'!AE75:AE77,'160 - Models'!AH75:AH77)</f>
+        <v>32.019550040108641</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
@@ -13786,7 +13859,10 @@
         <f>HARMEAN('160 - Models'!AB57:AB59,'160 - Models'!AE57:AE59,'160 - Models'!AH57:AH59)</f>
         <v>38.684241711696046</v>
       </c>
-      <c r="F52" s="7"/>
+      <c r="F52" s="7">
+        <f>HARMEAN('160 - Models'!AB78:AB80,'160 - Models'!AE78:AE80,'160 - Models'!AH78:AH80)</f>
+        <v>27.16004739392222</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
@@ -13808,7 +13884,10 @@
         <f>HARMEAN('160 - Models'!AB60:AB62,'160 - Models'!AE60:AE62,'160 - Models'!AH60:AH62)</f>
         <v>15.573600803808091</v>
       </c>
-      <c r="F53" s="7"/>
+      <c r="F53" s="7">
+        <f>HARMEAN('160 - Models'!AB81:AB83,'160 - Models'!AE81:AE83,'160 - Models'!AH81:AH83)</f>
+        <v>14.210225981036634</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
@@ -13830,7 +13909,10 @@
         <f>HARMEAN('160 - Models'!AB63:AB65,'160 - Models'!AE63:AE65,'160 - Models'!AH63:AH65)</f>
         <v>95.117950666124415</v>
       </c>
-      <c r="F54" s="7"/>
+      <c r="F54" s="7">
+        <f>HARMEAN('160 - Models'!AB84:AB86,'160 - Models'!AE84:AE86,'160 - Models'!AH84:AH86)</f>
+        <v>87.534879232324485</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -13852,7 +13934,10 @@
         <f>HARMEAN('160 - Models'!AB66:AB68,'160 - Models'!AE66:AE68,'160 - Models'!AH66:AH68)</f>
         <v>28.374654062644559</v>
       </c>
-      <c r="F55" s="7"/>
+      <c r="F55" s="7">
+        <f>HARMEAN('160 - Models'!AB87:AB89,'160 - Models'!AE87:AE89,'160 - Models'!AH87:AH89)</f>
+        <v>27.685382650143971</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30053,8 +30138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P49" workbookViewId="0">
-      <selection activeCell="AH69" sqref="AH69"/>
+    <sheetView tabSelected="1" topLeftCell="P79" workbookViewId="0">
+      <selection activeCell="AI90" sqref="AI90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35592,6 +35677,102 @@
       <c r="C75">
         <v>19</v>
       </c>
+      <c r="D75">
+        <v>2733</v>
+      </c>
+      <c r="E75">
+        <v>2998</v>
+      </c>
+      <c r="F75">
+        <v>10</v>
+      </c>
+      <c r="G75">
+        <v>48</v>
+      </c>
+      <c r="H75">
+        <v>15</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="L75">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M75">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="N75">
+        <v>0.23</v>
+      </c>
+      <c r="O75">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="P75">
+        <v>0.318</v>
+      </c>
+      <c r="Q75">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="R75">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="S75">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="T75">
+        <v>6693</v>
+      </c>
+      <c r="U75">
+        <v>6958</v>
+      </c>
+      <c r="V75">
+        <v>1000</v>
+      </c>
+      <c r="W75">
+        <v>45370</v>
+      </c>
+      <c r="X75">
+        <v>88688</v>
+      </c>
+      <c r="Y75">
+        <v>43351</v>
+      </c>
+      <c r="Z75">
+        <v>0</v>
+      </c>
+      <c r="AA75">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="AB75">
+        <v>34.372999999999998</v>
+      </c>
+      <c r="AC75">
+        <v>34.529000000000003</v>
+      </c>
+      <c r="AD75">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="AE75">
+        <v>29.844000000000001</v>
+      </c>
+      <c r="AF75">
+        <v>29.920999999999999</v>
+      </c>
+      <c r="AG75">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="AH75">
+        <v>30.536999999999999</v>
+      </c>
+      <c r="AI75">
+        <v>30.620999999999999</v>
+      </c>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A76">
@@ -35603,16 +35784,102 @@
       <c r="C76">
         <v>24</v>
       </c>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
+      <c r="D76" s="2">
+        <v>2748</v>
+      </c>
+      <c r="E76" s="2">
+        <v>3015</v>
+      </c>
+      <c r="F76" s="2">
+        <v>10</v>
+      </c>
+      <c r="G76" s="2">
+        <v>64</v>
+      </c>
+      <c r="H76" s="2">
+        <v>22</v>
+      </c>
+      <c r="I76" s="2">
+        <v>4</v>
+      </c>
+      <c r="J76" s="2">
+        <v>0</v>
+      </c>
+      <c r="K76" s="2">
+        <v>0.246</v>
+      </c>
+      <c r="L76" s="2">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="M76" s="2">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="N76">
+        <v>0.24</v>
+      </c>
+      <c r="O76">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="P76">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="Q76">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="R76">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="S76">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="T76">
+        <v>6708</v>
+      </c>
+      <c r="U76">
+        <v>6975</v>
+      </c>
+      <c r="V76">
+        <v>1000</v>
+      </c>
+      <c r="W76">
+        <v>32553</v>
+      </c>
+      <c r="X76">
+        <v>63025</v>
+      </c>
+      <c r="Y76">
+        <v>30519</v>
+      </c>
+      <c r="Z76">
+        <v>0</v>
+      </c>
+      <c r="AA76">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="AB76">
+        <v>24.923999999999999</v>
+      </c>
+      <c r="AC76">
+        <v>25.103000000000002</v>
+      </c>
+      <c r="AD76">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="AE76">
+        <v>25.863</v>
+      </c>
+      <c r="AF76">
+        <v>25.972000000000001</v>
+      </c>
+      <c r="AG76">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="AH76">
+        <v>22.983000000000001</v>
+      </c>
+      <c r="AI76">
+        <v>23.081</v>
+      </c>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A77">
@@ -35624,6 +35891,102 @@
       <c r="C77">
         <v>9</v>
       </c>
+      <c r="D77">
+        <v>2737</v>
+      </c>
+      <c r="E77">
+        <v>3002</v>
+      </c>
+      <c r="F77">
+        <v>10</v>
+      </c>
+      <c r="G77">
+        <v>48</v>
+      </c>
+      <c r="H77">
+        <v>15</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0.22</v>
+      </c>
+      <c r="L77">
+        <v>0.223</v>
+      </c>
+      <c r="M77">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="N77">
+        <v>0.432</v>
+      </c>
+      <c r="O77">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P77">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="Q77">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="R77">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="S77">
+        <v>0.2</v>
+      </c>
+      <c r="T77">
+        <v>6697</v>
+      </c>
+      <c r="U77">
+        <v>6962</v>
+      </c>
+      <c r="V77">
+        <v>1000</v>
+      </c>
+      <c r="W77">
+        <v>145425</v>
+      </c>
+      <c r="X77">
+        <v>288791</v>
+      </c>
+      <c r="Y77">
+        <v>143402</v>
+      </c>
+      <c r="Z77">
+        <v>0</v>
+      </c>
+      <c r="AA77">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AB77">
+        <v>44.908999999999999</v>
+      </c>
+      <c r="AC77">
+        <v>44.954000000000001</v>
+      </c>
+      <c r="AD77">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="AE77">
+        <v>48.473999999999997</v>
+      </c>
+      <c r="AF77">
+        <v>48.52</v>
+      </c>
+      <c r="AG77">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AH77">
+        <v>48.694000000000003</v>
+      </c>
+      <c r="AI77">
+        <v>48.741999999999997</v>
+      </c>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A78">
@@ -35635,6 +35998,102 @@
       <c r="C78" s="3" t="s">
         <v>77</v>
       </c>
+      <c r="D78">
+        <v>5437</v>
+      </c>
+      <c r="E78">
+        <v>5982</v>
+      </c>
+      <c r="F78">
+        <v>10</v>
+      </c>
+      <c r="G78">
+        <v>93</v>
+      </c>
+      <c r="H78">
+        <v>16</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="L78">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="M78">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="N78">
+        <v>0.16</v>
+      </c>
+      <c r="O78">
+        <v>0.22</v>
+      </c>
+      <c r="P78">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="Q78">
+        <v>0.16</v>
+      </c>
+      <c r="R78">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="S78">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="T78">
+        <v>9397</v>
+      </c>
+      <c r="U78">
+        <v>9942</v>
+      </c>
+      <c r="V78">
+        <v>1000</v>
+      </c>
+      <c r="W78">
+        <v>104034</v>
+      </c>
+      <c r="X78">
+        <v>205931</v>
+      </c>
+      <c r="Y78">
+        <v>101974</v>
+      </c>
+      <c r="Z78">
+        <v>0</v>
+      </c>
+      <c r="AA78">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="AB78">
+        <v>41.918999999999997</v>
+      </c>
+      <c r="AC78">
+        <v>42.015000000000001</v>
+      </c>
+      <c r="AD78">
+        <v>0.154</v>
+      </c>
+      <c r="AE78">
+        <v>42.179000000000002</v>
+      </c>
+      <c r="AF78">
+        <v>42.234000000000002</v>
+      </c>
+      <c r="AG78">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="AH78">
+        <v>50.225999999999999</v>
+      </c>
+      <c r="AI78">
+        <v>50.286000000000001</v>
+      </c>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A79">
@@ -35646,12 +36105,102 @@
       <c r="C79" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="W79" s="2"/>
-      <c r="X79" s="2"/>
-      <c r="Y79" s="2"/>
+      <c r="D79" s="2">
+        <v>5283</v>
+      </c>
+      <c r="E79" s="2">
+        <v>5818</v>
+      </c>
+      <c r="F79" s="2">
+        <v>10</v>
+      </c>
+      <c r="G79">
+        <v>103</v>
+      </c>
+      <c r="H79">
+        <v>20</v>
+      </c>
+      <c r="I79">
+        <v>4</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0.216</v>
+      </c>
+      <c r="L79">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="M79">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="N79">
+        <v>0.157</v>
+      </c>
+      <c r="O79">
+        <v>0.2</v>
+      </c>
+      <c r="P79">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="Q79">
+        <v>0.155</v>
+      </c>
+      <c r="R79">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="S79">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="T79">
+        <v>9243</v>
+      </c>
+      <c r="U79">
+        <v>9778</v>
+      </c>
+      <c r="V79">
+        <v>1000</v>
+      </c>
+      <c r="W79" s="2">
+        <v>219311</v>
+      </c>
+      <c r="X79" s="2">
+        <v>436474</v>
+      </c>
+      <c r="Y79" s="2">
+        <v>217248</v>
+      </c>
+      <c r="Z79">
+        <v>0</v>
+      </c>
+      <c r="AA79">
+        <v>0.249</v>
+      </c>
+      <c r="AB79">
+        <v>83.888999999999996</v>
+      </c>
+      <c r="AC79">
+        <v>83.977000000000004</v>
+      </c>
+      <c r="AD79">
+        <v>0.151</v>
+      </c>
+      <c r="AE79">
+        <v>77.947999999999993</v>
+      </c>
+      <c r="AF79">
+        <v>78.001999999999995</v>
+      </c>
+      <c r="AG79">
+        <v>0.151</v>
+      </c>
+      <c r="AH79">
+        <v>80.748000000000005</v>
+      </c>
+      <c r="AI79">
+        <v>80.802000000000007</v>
+      </c>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A80">
@@ -35663,8 +36212,104 @@
       <c r="C80" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>5414</v>
+      </c>
+      <c r="E80">
+        <v>5955</v>
+      </c>
+      <c r="F80">
+        <v>10</v>
+      </c>
+      <c r="G80">
+        <v>72</v>
+      </c>
+      <c r="H80">
+        <v>18</v>
+      </c>
+      <c r="I80">
+        <v>2</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0.155</v>
+      </c>
+      <c r="L80">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="M80">
+        <v>0.251</v>
+      </c>
+      <c r="N80">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="O80">
+        <v>0.192</v>
+      </c>
+      <c r="P80">
+        <v>0.247</v>
+      </c>
+      <c r="Q80">
+        <v>0.154</v>
+      </c>
+      <c r="R80">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="S80">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="T80">
+        <v>9374</v>
+      </c>
+      <c r="U80">
+        <v>9915</v>
+      </c>
+      <c r="V80">
+        <v>1000</v>
+      </c>
+      <c r="W80">
+        <v>28510</v>
+      </c>
+      <c r="X80">
+        <v>54918</v>
+      </c>
+      <c r="Y80">
+        <v>26465</v>
+      </c>
+      <c r="Z80">
+        <v>0</v>
+      </c>
+      <c r="AA80">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AB80">
+        <v>14.013</v>
+      </c>
+      <c r="AC80">
+        <v>14.08</v>
+      </c>
+      <c r="AD80">
+        <v>0.15</v>
+      </c>
+      <c r="AE80">
+        <v>13.196999999999999</v>
+      </c>
+      <c r="AF80">
+        <v>13.25</v>
+      </c>
+      <c r="AG80">
+        <v>0.158</v>
+      </c>
+      <c r="AH80">
+        <v>12.558999999999999</v>
+      </c>
+      <c r="AI80">
+        <v>12.614000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>20</v>
       </c>
@@ -35674,12 +36319,104 @@
       <c r="C81" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="V81" s="2"/>
-      <c r="W81" s="2"/>
-      <c r="X81" s="2"/>
-      <c r="Y81" s="2"/>
-    </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>8113</v>
+      </c>
+      <c r="E81">
+        <v>8934</v>
+      </c>
+      <c r="F81">
+        <v>10</v>
+      </c>
+      <c r="G81">
+        <v>98</v>
+      </c>
+      <c r="H81">
+        <v>17</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0.185</v>
+      </c>
+      <c r="L81">
+        <v>0.376</v>
+      </c>
+      <c r="M81">
+        <v>0.443</v>
+      </c>
+      <c r="N81">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="O81">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="P81">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="Q81">
+        <v>0.192</v>
+      </c>
+      <c r="R81">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="S81">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="T81">
+        <v>12073</v>
+      </c>
+      <c r="U81">
+        <v>12894</v>
+      </c>
+      <c r="V81" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W81" s="2">
+        <v>12468</v>
+      </c>
+      <c r="X81" s="2">
+        <v>22783</v>
+      </c>
+      <c r="Y81" s="2">
+        <v>10395</v>
+      </c>
+      <c r="Z81">
+        <v>0</v>
+      </c>
+      <c r="AA81">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="AB81">
+        <v>9.1280000000000001</v>
+      </c>
+      <c r="AC81">
+        <v>9.2059999999999995</v>
+      </c>
+      <c r="AD81">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="AE81">
+        <v>9.6280000000000001</v>
+      </c>
+      <c r="AF81">
+        <v>9.6910000000000007</v>
+      </c>
+      <c r="AG81">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AH81">
+        <v>9.0190000000000001</v>
+      </c>
+      <c r="AI81">
+        <v>9.08</v>
+      </c>
+    </row>
+    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>21</v>
       </c>
@@ -35689,8 +36426,104 @@
       <c r="C82" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>8122</v>
+      </c>
+      <c r="E82">
+        <v>8941</v>
+      </c>
+      <c r="F82">
+        <v>10</v>
+      </c>
+      <c r="G82">
+        <v>96</v>
+      </c>
+      <c r="H82">
+        <v>28</v>
+      </c>
+      <c r="I82">
+        <v>7</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="L82">
+        <v>0.317</v>
+      </c>
+      <c r="M82">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="N82">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="O82">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="P82">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="Q82">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="R82">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="S82">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="T82">
+        <v>12082</v>
+      </c>
+      <c r="U82">
+        <v>12901</v>
+      </c>
+      <c r="V82">
+        <v>1000</v>
+      </c>
+      <c r="W82">
+        <v>136912</v>
+      </c>
+      <c r="X82">
+        <v>271688</v>
+      </c>
+      <c r="Y82">
+        <v>134854</v>
+      </c>
+      <c r="Z82">
+        <v>0</v>
+      </c>
+      <c r="AA82">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="AB82">
+        <v>67.608000000000004</v>
+      </c>
+      <c r="AC82">
+        <v>67.698999999999998</v>
+      </c>
+      <c r="AD82">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AE82">
+        <v>71.647000000000006</v>
+      </c>
+      <c r="AF82">
+        <v>71.709000000000003</v>
+      </c>
+      <c r="AG82">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="AH82">
+        <v>73.241</v>
+      </c>
+      <c r="AI82">
+        <v>73.311999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>22</v>
       </c>
@@ -35700,8 +36533,104 @@
       <c r="C83" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>7872</v>
+      </c>
+      <c r="E83">
+        <v>8669</v>
+      </c>
+      <c r="F83">
+        <v>10</v>
+      </c>
+      <c r="G83">
+        <v>93</v>
+      </c>
+      <c r="H83">
+        <v>15</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0.17</v>
+      </c>
+      <c r="L83">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="M83">
+        <v>0.35</v>
+      </c>
+      <c r="N83">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="O83">
+        <v>0.3</v>
+      </c>
+      <c r="P83">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="Q83">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="R83">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="S83">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="T83">
+        <v>11832</v>
+      </c>
+      <c r="U83">
+        <v>12629</v>
+      </c>
+      <c r="V83">
+        <v>1000</v>
+      </c>
+      <c r="W83">
+        <v>17229</v>
+      </c>
+      <c r="X83">
+        <v>32321</v>
+      </c>
+      <c r="Y83">
+        <v>15168</v>
+      </c>
+      <c r="Z83">
+        <v>0</v>
+      </c>
+      <c r="AA83">
+        <v>0.183</v>
+      </c>
+      <c r="AB83">
+        <v>11.141999999999999</v>
+      </c>
+      <c r="AC83">
+        <v>11.208</v>
+      </c>
+      <c r="AD83">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="AE83">
+        <v>11.353999999999999</v>
+      </c>
+      <c r="AF83">
+        <v>11.419</v>
+      </c>
+      <c r="AG83">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="AH83">
+        <v>11.257999999999999</v>
+      </c>
+      <c r="AI83">
+        <v>11.32</v>
+      </c>
+    </row>
+    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>30</v>
       </c>
@@ -35711,14 +36640,104 @@
       <c r="C84" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="T84" s="2"/>
-      <c r="U84" s="2"/>
-      <c r="V84" s="2"/>
-    </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D84" s="2">
+        <v>10758</v>
+      </c>
+      <c r="E84" s="2">
+        <v>11850</v>
+      </c>
+      <c r="F84" s="2">
+        <v>10</v>
+      </c>
+      <c r="G84">
+        <v>148</v>
+      </c>
+      <c r="H84">
+        <v>17</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="L84">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="M84">
+        <v>0.52</v>
+      </c>
+      <c r="N84">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="O84">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="P84">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="Q84">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="R84">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="S84">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="T84" s="2">
+        <v>14718</v>
+      </c>
+      <c r="U84" s="2">
+        <v>15810</v>
+      </c>
+      <c r="V84" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W84">
+        <v>381758</v>
+      </c>
+      <c r="X84">
+        <v>761502</v>
+      </c>
+      <c r="Y84">
+        <v>379758</v>
+      </c>
+      <c r="Z84">
+        <v>0</v>
+      </c>
+      <c r="AA84">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="AB84">
+        <v>224.4</v>
+      </c>
+      <c r="AC84">
+        <v>224.489</v>
+      </c>
+      <c r="AD84">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="AE84">
+        <v>250.154</v>
+      </c>
+      <c r="AF84">
+        <v>250.244</v>
+      </c>
+      <c r="AG84">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="AH84">
+        <v>215.17</v>
+      </c>
+      <c r="AI84">
+        <v>215.262</v>
+      </c>
+    </row>
+    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>31</v>
       </c>
@@ -35728,11 +36747,104 @@
       <c r="C85" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-    </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>10727</v>
+      </c>
+      <c r="E85">
+        <v>11820</v>
+      </c>
+      <c r="F85">
+        <v>10</v>
+      </c>
+      <c r="G85" s="2">
+        <v>92</v>
+      </c>
+      <c r="H85" s="2">
+        <v>16</v>
+      </c>
+      <c r="I85" s="2">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="L85">
+        <v>0.435</v>
+      </c>
+      <c r="M85">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="N85">
+        <v>0.192</v>
+      </c>
+      <c r="O85">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="P85">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="Q85">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="R85">
+        <v>0.4</v>
+      </c>
+      <c r="S85">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="T85">
+        <v>14687</v>
+      </c>
+      <c r="U85">
+        <v>15780</v>
+      </c>
+      <c r="V85">
+        <v>1000</v>
+      </c>
+      <c r="W85">
+        <v>140911</v>
+      </c>
+      <c r="X85">
+        <v>279688</v>
+      </c>
+      <c r="Y85">
+        <v>138853</v>
+      </c>
+      <c r="Z85">
+        <v>0</v>
+      </c>
+      <c r="AA85">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="AB85">
+        <v>82.102999999999994</v>
+      </c>
+      <c r="AC85">
+        <v>82.234999999999999</v>
+      </c>
+      <c r="AD85">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="AE85">
+        <v>84.32</v>
+      </c>
+      <c r="AF85">
+        <v>84.406000000000006</v>
+      </c>
+      <c r="AG85">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="AH85">
+        <v>105.449</v>
+      </c>
+      <c r="AI85">
+        <v>105.556</v>
+      </c>
+    </row>
+    <row r="86" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>32</v>
       </c>
@@ -35742,8 +36854,104 @@
       <c r="C86" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>10656</v>
+      </c>
+      <c r="E86">
+        <v>11734</v>
+      </c>
+      <c r="F86">
+        <v>10</v>
+      </c>
+      <c r="G86">
+        <v>84</v>
+      </c>
+      <c r="H86">
+        <v>16</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0.2</v>
+      </c>
+      <c r="L86">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="M86">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="N86">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="O86">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="P86">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="Q86">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="R86">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="S86">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="T86">
+        <v>14616</v>
+      </c>
+      <c r="U86">
+        <v>15694</v>
+      </c>
+      <c r="V86">
+        <v>1000</v>
+      </c>
+      <c r="W86">
+        <v>86514</v>
+      </c>
+      <c r="X86">
+        <v>170908</v>
+      </c>
+      <c r="Y86">
+        <v>84462</v>
+      </c>
+      <c r="Z86">
+        <v>0</v>
+      </c>
+      <c r="AA86">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="AB86">
+        <v>52.631999999999998</v>
+      </c>
+      <c r="AC86">
+        <v>52.710999999999999</v>
+      </c>
+      <c r="AD86">
+        <v>0.215</v>
+      </c>
+      <c r="AE86">
+        <v>51.997</v>
+      </c>
+      <c r="AF86">
+        <v>52.098999999999997</v>
+      </c>
+      <c r="AG86">
+        <v>0.2</v>
+      </c>
+      <c r="AH86">
+        <v>55.677999999999997</v>
+      </c>
+      <c r="AI86">
+        <v>55.767000000000003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>40</v>
       </c>
@@ -35753,11 +36961,104 @@
       <c r="C87" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T87" s="2"/>
-      <c r="U87" s="2"/>
-      <c r="V87" s="2"/>
-    </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>13237</v>
+      </c>
+      <c r="E87">
+        <v>14585</v>
+      </c>
+      <c r="F87">
+        <v>10</v>
+      </c>
+      <c r="G87">
+        <v>161</v>
+      </c>
+      <c r="H87">
+        <v>20</v>
+      </c>
+      <c r="I87">
+        <v>3</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0.216</v>
+      </c>
+      <c r="L87">
+        <v>0.62</v>
+      </c>
+      <c r="M87">
+        <v>0.71</v>
+      </c>
+      <c r="N87">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="O87">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="P87">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="Q87">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="R87">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="S87">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="T87" s="2">
+        <v>17197</v>
+      </c>
+      <c r="U87" s="2">
+        <v>18545</v>
+      </c>
+      <c r="V87" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W87">
+        <v>15776</v>
+      </c>
+      <c r="X87">
+        <v>29277</v>
+      </c>
+      <c r="Y87">
+        <v>13643</v>
+      </c>
+      <c r="Z87">
+        <v>0</v>
+      </c>
+      <c r="AA87">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="AB87">
+        <v>20.248999999999999</v>
+      </c>
+      <c r="AC87">
+        <v>20.373000000000001</v>
+      </c>
+      <c r="AD87">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="AE87">
+        <v>15.726000000000001</v>
+      </c>
+      <c r="AF87">
+        <v>15.813000000000001</v>
+      </c>
+      <c r="AG87">
+        <v>0.215</v>
+      </c>
+      <c r="AH87">
+        <v>15.691000000000001</v>
+      </c>
+      <c r="AI87">
+        <v>15.776999999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>41</v>
       </c>
@@ -35767,14 +37068,104 @@
       <c r="C88" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="T88" s="2"/>
-      <c r="U88" s="2"/>
-      <c r="V88" s="2"/>
-      <c r="AA88" s="2"/>
-      <c r="AB88" s="2"/>
-      <c r="AC88" s="2"/>
-    </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>13444</v>
+      </c>
+      <c r="E88">
+        <v>14812</v>
+      </c>
+      <c r="F88">
+        <v>10</v>
+      </c>
+      <c r="G88">
+        <v>61</v>
+      </c>
+      <c r="H88">
+        <v>16</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="L88">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="M88">
+        <v>0.61</v>
+      </c>
+      <c r="N88">
+        <v>0.223</v>
+      </c>
+      <c r="O88">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="P88">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="Q88">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="R88">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="S88">
+        <v>0.622</v>
+      </c>
+      <c r="T88" s="2">
+        <v>17404</v>
+      </c>
+      <c r="U88" s="2">
+        <v>18772</v>
+      </c>
+      <c r="V88" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W88">
+        <v>191613</v>
+      </c>
+      <c r="X88">
+        <v>381146</v>
+      </c>
+      <c r="Y88">
+        <v>189578</v>
+      </c>
+      <c r="Z88">
+        <v>0</v>
+      </c>
+      <c r="AA88" s="2">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="AB88" s="2">
+        <v>116.07599999999999</v>
+      </c>
+      <c r="AC88" s="2">
+        <v>116.17400000000001</v>
+      </c>
+      <c r="AD88">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="AE88">
+        <v>119.691</v>
+      </c>
+      <c r="AF88">
+        <v>119.791</v>
+      </c>
+      <c r="AG88">
+        <v>0.37</v>
+      </c>
+      <c r="AH88">
+        <v>157.28</v>
+      </c>
+      <c r="AI88">
+        <v>157.41999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>42</v>
       </c>
@@ -35784,12 +37175,102 @@
       <c r="C89" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="T89" s="2"/>
-      <c r="U89" s="2"/>
-      <c r="V89" s="2"/>
-      <c r="AA89" s="2"/>
-      <c r="AB89" s="2"/>
-      <c r="AC89" s="2"/>
+      <c r="D89">
+        <v>13328</v>
+      </c>
+      <c r="E89">
+        <v>14685</v>
+      </c>
+      <c r="F89">
+        <v>10</v>
+      </c>
+      <c r="G89">
+        <v>88</v>
+      </c>
+      <c r="H89">
+        <v>18</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0.215</v>
+      </c>
+      <c r="L89">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="M89">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="N89">
+        <v>0.214</v>
+      </c>
+      <c r="O89">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="P89">
+        <v>0.625</v>
+      </c>
+      <c r="Q89">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="R89">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="S89">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="T89" s="2">
+        <v>17288</v>
+      </c>
+      <c r="U89" s="2">
+        <v>18645</v>
+      </c>
+      <c r="V89" s="2">
+        <v>1000</v>
+      </c>
+      <c r="W89">
+        <v>27434</v>
+      </c>
+      <c r="X89">
+        <v>52738</v>
+      </c>
+      <c r="Y89">
+        <v>25374</v>
+      </c>
+      <c r="Z89">
+        <v>0</v>
+      </c>
+      <c r="AA89" s="2">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="AB89" s="2">
+        <v>24.077999999999999</v>
+      </c>
+      <c r="AC89" s="2">
+        <v>24.25</v>
+      </c>
+      <c r="AD89">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="AE89">
+        <v>23.879000000000001</v>
+      </c>
+      <c r="AF89">
+        <v>23.988</v>
+      </c>
+      <c r="AG89">
+        <v>0.215</v>
+      </c>
+      <c r="AH89">
+        <v>24.015999999999998</v>
+      </c>
+      <c r="AI89">
+        <v>24.105</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="32">

</xml_diff>